<commit_message>
Add further history of private law cards
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VL Geschichte des Privaten Rechts (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VL Geschichte des Privaten Rechts (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
   <si>
     <t>Question</t>
   </si>
@@ -19,118 +19,772 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Herrscht heute formelles oder materielles Eintrittsrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Formelles&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erbe erbt aus &lt;strong&gt;eigenem Recht&lt;/strong&gt;, &lt;strong&gt;nicht &lt;/strong&gt;aus Recht des &lt;strong&gt;Gradnächsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;d.h. bei &lt;strong&gt;Erbunfähigkeit &lt;/strong&gt;des &lt;strong&gt;Gradnächsten &lt;/strong&gt;erben dessen &lt;strong&gt;Nachkommen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wovon hängt die Handlungsfähigkeit heutzutage ab?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Alter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;geistige &lt;/strong&gt;und &lt;strong&gt;seelische Verfassung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Unterschiede gibt es zwischen „Rechtsfähigkeit“ und „Handlungsfähigkeit“?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Rechtsfähigkeit&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Menschen verfügen über &lt;strong&gt;angeborene &lt;/strong&gt;und &lt;strong&gt;erworbene Rechten &lt;/strong&gt;und &lt;strong&gt;Pflichte&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Handlungsfähigkeit&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Fähigkeit &lt;/strong&gt;eines Menschen, durch &lt;strong&gt;eigenes Handeln Rechte &lt;/strong&gt;und &lt;strong&gt;Pflichten &lt;/strong&gt;zu &lt;strong&gt;begründen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Wird &lt;em&gt;nicht mit Geburt&lt;/em&gt; erworben&lt;/li&gt;&lt;li&gt;Sondern von &lt;strong&gt;&lt;em&gt;Rechtsordnung &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;verliehen&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;an Personen&lt;/strong&gt; die in der &lt;strong&gt;Lage sind &lt;/strong&gt;Ihre &lt;strong&gt;Angelegenheiten selbst &lt;/strong&gt;zu &lt;strong&gt;regeln&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Besteht&lt;strong&gt; &lt;/strong&gt;aus &lt;strong&gt;Geschäftsfähigkeit &lt;/strong&gt;und &lt;strong&gt;Deliktsfähigkeit &lt;/strong&gt;(siehe eigene Frage)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche wesentlichen Unterschiede zwischen „Ehegesetz 1938“ und „ABGB“, vor allem&lt;/p&gt;&lt;p&gt;welchen Grundsatz gibt es heute noch?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Konfessionelle &lt;strong&gt;Dreiteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sonderregelungen &lt;/strong&gt;für &lt;strong&gt;Katholiken: Keine Scheidung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Grundsatz EheG 1938 &amp;amp; Heutiges Recht: &lt;em&gt;obligatorische Zivilehe&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus welchem Wirtschaftsystem kommt die Unterscheidung zwischen mittelbaren und unmittelbaren Geweren im Liegenschaftsrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Wirtschaftlicher &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Feudalismus&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;mittelalterliche Grundherrschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;leihender &lt;strong&gt;Bauer&lt;/strong&gt;: &lt;strong&gt;unmittelbare &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grundherr&lt;/strong&gt;: &lt;strong&gt;mittelbare &lt;/strong&gt;Gewere &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer konnte sich im ABGB 1811 nicht scheiden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Katholiken &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehe &lt;strong&gt;nur durch Tod &lt;/strong&gt;gelöst&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die leibliche Haftung (anders als die persönliche)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Schuldner haftet mit &lt;strong&gt;Körper&lt;/strong&gt; oder &lt;strong&gt;Freiheit&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind &lt;strong&gt;leibliche Haftung&lt;/strong&gt;, &lt;strong&gt;Sachhaftung&lt;/strong&gt;, &lt;strong&gt;Vermögenshaftung&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;leibliche Haftung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;G&lt;/strong&gt; kann S &lt;strong&gt;töten&lt;/strong&gt;, &lt;strong&gt;verstümmeln&lt;/strong&gt;, &lt;strong&gt;verknechten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;am &lt;strong&gt;Vermögen schadlos &lt;/strong&gt;halten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gewaltunterworfene &lt;/strong&gt;als &lt;strong&gt;Geiseln &lt;/strong&gt;nehmen bis Bezahlung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Sachhaftung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;G&lt;/strong&gt; hatte &lt;strong&gt;Sachherrschaft&lt;/strong&gt;, bei &lt;strong&gt;Nichtbezahlung Eigentum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Später &lt;strong&gt;nur &lt;/strong&gt;noch &lt;strong&gt;Verwertungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Vermögenshaftung (persönliche Haftung)&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aus &lt;strong&gt;leiblicher Haftung&lt;/strong&gt; wurde &lt;strong&gt;Schuldknechtschaft&lt;/strong&gt;, dann &lt;strong&gt;Schuldhaft &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;G&lt;/strong&gt; konnte aber dann &lt;strong&gt;keinen&lt;/strong&gt; &lt;strong&gt;Nutzen&lt;/strong&gt; &lt;strong&gt;aus S&lt;/strong&gt; ziehen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;war also &lt;strong&gt;nur&lt;/strong&gt; ein &lt;strong&gt;Druckmittel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher: &lt;em&gt;Vermögenshaftung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zugriff &lt;/strong&gt;auf das &lt;strong&gt;Vermögen&lt;/strong&gt; &lt;strong&gt;des S&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man die unbeschränkte Haftung eines Erben?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Vermögenshaftung &lt;/strong&gt;bzw &lt;strong&gt;persönliche &lt;/strong&gt;Haftung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Seit&lt;/strong&gt; &lt;strong&gt;wann &lt;/strong&gt;kennen wir das Prinzip, wonach Erben unbeschränkt haften können? Durch&lt;/p&gt;&lt;p&gt;welchen &lt;strong&gt;Einfluss&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Seit der &lt;strong&gt;Neuzeit &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;durch den &lt;strong&gt;Einfluss&lt;/strong&gt; der &lt;strong&gt;Rezeption&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herauslösen &lt;/strong&gt;des &lt;strong&gt;Schuldrechts aus&lt;/strong&gt; dem &lt;strong&gt;Strafrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Es gab in Einzelfällen die Veranlassung, dass Erben Schulden zu begleichen hatten – Warum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bei &lt;strong&gt;Vertragsschulden&lt;/strong&gt;, wenn &lt;strong&gt;Geschäftspartner &lt;/strong&gt;des Erblassers &lt;strong&gt;bereits&lt;/strong&gt; &lt;strong&gt;geleistet&lt;/strong&gt; hat&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist der Legatar ein Erbe? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nein - &lt;strong&gt;Vermächtnis&lt;/strong&gt;/&lt;strong&gt;Legat &lt;/strong&gt;hat &lt;strong&gt;keine Erbeinsetzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wie röm. &lt;strong&gt;Damnationslegat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur &lt;strong&gt;schuldrechtlicher Anspruch &lt;/strong&gt;ggü. dem &lt;strong&gt;Erben &lt;/strong&gt;auf &lt;strong&gt;Herausgabe &lt;/strong&gt;der vermachten Sachen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktionierten Testament und Testierfreiheit in der Neuzeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Testierfreiheit &lt;/strong&gt;mit &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Altersgrenze &lt;/strong&gt;(F &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;18&lt;/span&gt;, M &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;20&lt;/span&gt;)&lt;/li&gt;&lt;li&gt;Arten&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;: &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Testament&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Kodizill &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Erbvertrag &lt;/strong&gt;bekannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;subsidiär gesetzl. &lt;/strong&gt;Erbfolge.&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Pflichtteilsrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Möglichkeit der &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Enterbung&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbfolgeakte außergerichtlich &lt;/strong&gt;(Eröffnung des Testaments, Antreten der Erbschaft, Ergreifung des Nachlassbesitzes)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Anerbenrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;bäuerliche&lt;/em&gt; &lt;em&gt;Erbfolge &lt;/em&gt;- besonderes Erbrecht an &lt;strong&gt;landwirtschaftl&lt;/strong&gt;. &lt;strong&gt;Höfen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unteilbar &lt;/strong&gt;- nur&lt;strong&gt; einer von mehreren Erben&lt;/strong&gt; bekam den &lt;strong&gt;ganzen Hof&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;um &lt;strong&gt;Wirtschaftlichkeit &lt;/strong&gt;des Betriebs zu &lt;strong&gt;garantieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Auch im &lt;em&gt;ABGB 1811&lt;/em&gt; noch als &lt;em&gt;gesetzl&lt;/em&gt;. &lt;em&gt;Erbrecht &lt;/em&gt;enthalten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;konnte &lt;/strong&gt;aber per &lt;strong&gt;letztwilliger&lt;/strong&gt; &lt;strong&gt;Verfügung ausgeschlossen &lt;/strong&gt;werden&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die fränkische Affatomie und langobardische Thinx?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Affatomie&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur möglich wenn &lt;strong&gt;keine leibl. Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;König &lt;/strong&gt;musste Affatomie &lt;strong&gt;zustimmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;erbloses Gut normalerweise &lt;/strong&gt;an &lt;strong&gt;König&lt;/strong&gt; &lt;strong&gt;fiel&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Thinx&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verschaffte&lt;/strong&gt; &lt;strong&gt;Begünstigtem &lt;/strong&gt;die &lt;strong&gt;Rechtsstellung&lt;/strong&gt; eines &lt;strong&gt;Sohnes &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;quasi &lt;em&gt;Adoption&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erbe &lt;/strong&gt;damit &lt;strong&gt;ohne Blutsverwandtschaft &lt;/strong&gt;möglich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Teilung nach Köpfen und die Teilung nach Stämmen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;nach &lt;em&gt;Köpfen&lt;/em&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;alle&lt;/strong&gt; zur Erbschaft berufenen &lt;strong&gt;teilen Nachlass gleichmäßig &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;nach &lt;em&gt;Stämmen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;basierend auf &lt;strong&gt;Repräsentationsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;der jeweils &lt;strong&gt;Gradnächste &lt;/strong&gt;erbt&lt;/li&gt;&lt;li&gt;Also: &lt;strong&gt;Sohn &lt;/strong&gt;des &lt;strong&gt;Erblassers&lt;/strong&gt; schließt &lt;strong&gt;Enkel aus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie entwickelte sich das Erbrecht der &lt;strong&gt;un&lt;/strong&gt;ehelichen Kinder?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleiche Rechte&lt;/strong&gt;, wenn in Hausverband aufgenommen&lt;/li&gt;&lt;li&gt;Später &lt;strong&gt;christlichem Einfluss:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein Erbrechts&lt;/strong&gt; ggü. &lt;strong&gt;Vater&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehebruchskinder&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein &lt;/strong&gt;Erbrecht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;natürliche &lt;/strong&gt;Kinder (&lt;strong&gt;kein Ehehindernis &lt;/strong&gt;bei Eltern):&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbrecht &lt;strong&gt;gegen Mutter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Josephinisches Gesetzbuch&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Angleichung &lt;/strong&gt;an Rechtsstellung der &lt;strong&gt;ehelichen&lt;/strong&gt; &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;außer Ehebruchskinder&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zunächst &lt;strong&gt;keine Ansprüche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ab&lt;strong&gt; TN 1918&lt;/strong&gt;: Erbrecht &lt;strong&gt;nur gegen Mutter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Erbrechtsänderungsgesetz 1989&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;völlige Gleichstellung&lt;/strong&gt; mit ehelichen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wurden eheliche den unehelichen Kindern gleichgestellt?&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Wie lange&lt;/strong&gt; hielt das an? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Josephinische Ehegesetzgebung 1786&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ausnahme: &lt;strong&gt;Ehebruchskinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Endete &lt;/strong&gt;mit &lt;strong&gt;Leopold II 1791 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Leopold musste viele der als radikal geltenden Reformen Joseph II zurücknehmen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Erbquote des überlebenden Ehegatten in der gesetzl. Erbfolge heute?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Quote &lt;strong&gt;abhängig&lt;/strong&gt; von &lt;strong&gt;restlicher&lt;/strong&gt; &lt;strong&gt;Verwandtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ggü. lebender&lt;strong&gt; 1. Parentel&lt;/strong&gt;: &lt;strong&gt;1/3&lt;/strong&gt; Ehegatte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ggü. lebender &lt;strong&gt;2. Parentel&lt;/strong&gt;: &lt;strong&gt;2/3&lt;/strong&gt; Ehegatee&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Unabhängig von Erbrecht: &lt;strong&gt;gesetzl Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;alle zum &lt;strong&gt;Haushalt &lt;/strong&gt;gehörenden &lt;strong&gt;beweglichen Sachen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anspruch &lt;/strong&gt;auf &lt;strong&gt;verbleib &lt;/strong&gt;in der &lt;strong&gt;ehelichen Wohnung&lt;/strong&gt; gegen Erben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Besteht im Mittelalter ein Ehegattenerbrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;im &lt;strong&gt;heimischen Gewohnheitsrecht&lt;/strong&gt; &lt;strong&gt;kein Erbrecht&lt;/strong&gt; der Ehegatten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eheschließung &lt;/strong&gt;begründet &lt;strong&gt;keine Verwandtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fallrecht &lt;/strong&gt;stand einem &lt;strong&gt;Ehegattenrecht entgegen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Auch kein Drang: &lt;strong&gt;Ehegüterrecht &lt;/strong&gt;ermöglichte für &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert der Erbschaftserwerb heute?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;gerichtliches Nachlassverfahren (&lt;strong&gt;Verlassenschaftsabhandlung&lt;/strong&gt;) legt Nachlass fest &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Todesfallaufnahme&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dann &lt;strong&gt;Erbserklärung &lt;/strong&gt;des berufenen Erben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der sein Recht beweisen muss - &lt;strong&gt;Erbrechtsausweis&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ist alles vorhanden, folgt die &lt;em&gt;gerichtliche Besitzeinweisung &lt;/em&gt;(&lt;strong&gt;Einantwortung&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bis dahin&lt;/strong&gt; &lt;strong&gt;ruht &lt;/strong&gt;der Nachlass&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der ausgewiesene &lt;strong&gt;Erbe kann &lt;/strong&gt;diesen aber schon &lt;strong&gt;verwalten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das beneficium inventarii?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Beschränkte Erbenhaftung&lt;/strong&gt; - haftet &lt;strong&gt;nur mit &lt;/strong&gt;dem &lt;strong&gt;Nachlass&lt;/strong&gt;, nicht persönlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Was &lt;/strong&gt;und &lt;strong&gt;wann&lt;/strong&gt; waren die drei Phasen der Rezeption?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Frührezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;12.&lt;/strong&gt; und &lt;strong&gt;13&lt;/strong&gt;. JH &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Hauptrezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;15 &lt;/strong&gt;bis &lt;strong&gt;17&lt;/strong&gt;. JH &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Nachrezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;18&lt;/strong&gt; JH&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;in &lt;/strong&gt;Ö vor allem &lt;strong&gt;erbrechtliche &lt;/strong&gt;Bestimmungen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Parentelenordnung im MA?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ursprünglich&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;engerer &lt;/strong&gt;Erbenkreis: &lt;strong&gt;Hausgemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;weiterer&lt;/strong&gt; Erbenkreis: &lt;strong&gt;Blutsverwandte &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Parentelenordnung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anerkennung &lt;/strong&gt;des &lt;strong&gt;Repräsentationsrecht &lt;/strong&gt;für &lt;strong&gt;Kinder &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;dehnte engeren&lt;/strong&gt; Erbenkreis &lt;strong&gt;aus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;führte zu &lt;strong&gt;Parentelenordnung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;jüngere Generation ist älterer erbrechtlich vorangestellt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;strong&gt;Das Gut rinnt wie das Blut&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Erbgut und Kaufgut?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbgut&lt;/em&gt;: hat man &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;selbst vererbt &lt;/strong&gt;bekommen, wird &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;familiär weitergegeben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Kaufgut&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;selbst erwirtschaftetes &lt;/strong&gt;Vermögen zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;freien&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verfügung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Spezialsukzession?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der &lt;strong&gt;Nachlass &lt;/strong&gt;zerfällt in &lt;strong&gt;verschiedene Vermögensmassen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gehen in &lt;strong&gt;spezifischer Erbfolge &lt;/strong&gt;auf die &lt;strong&gt;Erben &lt;/strong&gt;über&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abweichung &lt;/strong&gt;von der &lt;strong&gt;gesetzlichen Erbfolge&lt;/strong&gt; ist &lt;strong&gt;möglich &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren Näherrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;dingliche Erwerbsrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Bei &lt;strong&gt;Eigentumswechsel &lt;/strong&gt;kann ein &lt;strong&gt;näher Berechtigter &lt;/strong&gt;(z.B.: Sippengenosse)&lt;strong&gt; &lt;/strong&gt;als der neue Eigentümer &lt;strong&gt;innerhalb &lt;/strong&gt;einer gewissen &lt;strong&gt;Frist&lt;/strong&gt; das &lt;strong&gt;Gut &lt;/strong&gt;an &lt;strong&gt;sich nehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schützt &lt;strong&gt;Sippeneigentum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abschwächung &lt;/strong&gt;zu &lt;strong&gt;Vorkaufs&lt;/strong&gt;- und &lt;strong&gt;Einstandsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Besserberechtigte musste &lt;strong&gt;Kaufpreis &lt;/strong&gt;und &lt;strong&gt;Kosten erstatten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur &lt;strong&gt;vertraglich begründete &lt;/strong&gt;Näherrechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren Leiherechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bodenleihe &lt;/strong&gt;verschaffte &lt;strong&gt;gegen&lt;/strong&gt; &lt;strong&gt;Entgelt Nutzungsrechte &lt;/strong&gt;an fremden Boden&lt;/li&gt;&lt;li&gt;Unterscheidung:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;freihe &lt;/em&gt;Leihe: &lt;strong&gt;Leistung&lt;/strong&gt; &lt;strong&gt;aus &lt;/strong&gt;dem &lt;strong&gt;Leihgut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;unfreie &lt;/em&gt;Leihe: &lt;strong&gt;persönliche &lt;/strong&gt;und &lt;strong&gt;wirtschaftliche Leistung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Arten (nach &lt;strong&gt;Personengruppen&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;bäuerliche&lt;/em&gt; Leihe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;städtische &lt;/em&gt;Leihe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ritterliche &lt;/em&gt;Leihe&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Ewigsatzung, was die Totsatzung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Ewigsatzung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Früchte &lt;/strong&gt;werden &lt;strong&gt;nicht&lt;/strong&gt; auf die &lt;strong&gt;Schuld angerechnet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pfand &lt;strong&gt;löst &lt;/strong&gt;sich &lt;strong&gt;NICHT selbst&lt;/strong&gt; auf.&lt;/li&gt;&lt;li&gt;&lt;em&gt;Totsatzung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Früchte &lt;/strong&gt;wurden auf die &lt;strong&gt;Schuld angerechnet &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pfand löst &lt;/strong&gt;sich somit nach gewisser Zeit &lt;strong&gt;selbst auf&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Fahrnispfandrecht? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Faustpfand &lt;/strong&gt;-&amp;gt; Übertragung &lt;strong&gt;leibliche Gewere &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;wurde &lt;strong&gt;Eigentümer&lt;/strong&gt;, wenn &lt;strong&gt;nicht in Frist eingelöst&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;13 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;konnte auf &lt;strong&gt;gesamtes Vermögen &lt;/strong&gt;zugreifen, wenn Pfand &lt;strong&gt;unterging &lt;/strong&gt;oder an &lt;strong&gt;Wert verlor &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Einführung des &lt;strong&gt;Verkaufspfandes&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Entwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;konnte durch &lt;strong&gt;Willensübereinstimmung &lt;/strong&gt;entstehen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;rechtlich schwach &lt;/strong&gt;(&lt;strong&gt;keine Verfolgungsklage &lt;/strong&gt;des Gläubigers &lt;strong&gt;ggü Dritten&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;18 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rückkehr zum &lt;strong&gt;Faustpfand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Faustpfand&lt;/strong&gt; und &lt;strong&gt;Hypothek&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Hypothek?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Pfandrecht &lt;/strong&gt;der &lt;strong&gt;jüngeren Satzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;besitzloses &lt;/strong&gt;Pfand im Liegenschaftsrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;in der &lt;strong&gt;Rezeption &lt;/strong&gt;(&lt;strong&gt;Neuzeit&lt;/strong&gt;) entwickelt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;hat &lt;strong&gt;Hypothek &lt;/strong&gt;(&lt;em&gt;beschränkt dingliches Recht&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;Nichtbegleichung &lt;/strong&gt;der Schuld kann er es &lt;strong&gt;geltend machen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Begründet durch&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;formfreien Vertrag &lt;/strong&gt;(&lt;strong&gt;Vertrags&lt;/strong&gt;pfandrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kraft &lt;strong&gt;Gesetz &lt;/strong&gt;(&lt;strong&gt;gesetzliches &lt;/strong&gt;Pfandrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;richterliche &lt;/strong&gt;Verfügung (&lt;strong&gt;Pfändungs&lt;/strong&gt;pfandrecht)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Dienstbarkeiten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Übernommen aus &lt;strong&gt;RR&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Grunddienstbarkeiten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;beschränkt dingliche Rechte &lt;/strong&gt;an &lt;strong&gt;Grundstücken&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eigentümer&lt;/strong&gt; muss &lt;strong&gt;Ausübung &lt;/strong&gt;des Rechts &lt;strong&gt;dulden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ins &lt;strong&gt;ABGB 1811&lt;/strong&gt; übernommen&lt;/li&gt;&lt;li&gt;&lt;em&gt;persönliche&lt;/em&gt; &lt;em&gt;Dienstbarkeiten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grunddienstbarkeiten &lt;/strong&gt;die einer &lt;strong&gt;bestimmten Person &lt;/strong&gt;zugeordnet werden -&amp;gt; &lt;em&gt;Leibzucht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;durch&lt;strong&gt; Rezeption&lt;/strong&gt;: &lt;strong&gt;Personalservituten &lt;/strong&gt;(&lt;em&gt;ususfructus, usus, habitatio&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind beschränkt dingliche Rechte?&lt;/p&gt;&lt;p&gt;Nennen sie ein Beispiel&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Belastungen &lt;/strong&gt;des Eigentums &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beschränkt&lt;/strong&gt; die Rechte des &lt;strong&gt;Eigentümers&lt;/strong&gt;, &lt;/li&gt;&lt;li class="ql-indent-1"&gt;gibt &lt;strong&gt;Teilberechtigungen&lt;/strong&gt; an den &lt;strong&gt;Berechtigten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Arten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pfand&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dienstbarkeiten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reallasten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Aufbau des ABGB?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Institutionensystem &lt;/em&gt;(auch &lt;strong&gt;gaianisches &lt;/strong&gt;System)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zweiteilung in &lt;strong&gt;Personen&lt;/strong&gt;- und &lt;strong&gt;Vermögensrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Pandektensystem&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aufteilung in &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Allgemeinen &lt;/strong&gt;Teil&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schuld&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sachen&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Familien&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erb&lt;/strong&gt;recht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Landtafeln?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Seit 13/14 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Form / Teil des &lt;strong&gt;Grundbuchs&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;für &lt;strong&gt;Adelige&lt;/strong&gt; &lt;strong&gt;Liegenschaften &lt;/strong&gt;- &lt;em&gt;Eintragungspflicht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;dingliche Rechte &lt;/strong&gt;gelten nur mit &lt;strong&gt;Eintragung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Typenzwang?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sachenrecht definiert &lt;/strong&gt;alle möglichen &lt;strong&gt;dingliche Berechtigungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es können &lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;weiteren &lt;/strong&gt;"&lt;strong&gt;erfunden&lt;/strong&gt;" werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;= &lt;em&gt;numerus clausus&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Stellung unehelicher Kinder im älteren Recht?&lt;/p&gt;&lt;p&gt;Wann änderte sich dies?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleichstellung &lt;/strong&gt;mit &lt;strong&gt;ehelichen&lt;/strong&gt;, wenn in &lt;strong&gt;Hausverband aufgenommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;sonst &lt;/strong&gt;Zugehörigkeit zu &lt;strong&gt;Muttersippe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schlechterstellung &lt;/strong&gt;ab &lt;strong&gt;christlicher &lt;/strong&gt;Zeit&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Stellung Joseph II zu unehelichen Kindern&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundsätzliche Gleichstellung &lt;/strong&gt;eheliche und uneheliche&lt;/li&gt;&lt;li&gt;Ausnahme: &lt;strong&gt;Ehebruchskinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Stellung der ehelichen und unehelichen Kinder im MA und im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Eheliche &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eheliche Kinder unter &lt;strong&gt;Munt &lt;/strong&gt;des Vaters&lt;/li&gt;&lt;li class="ql-indent-2"&gt;u.a. &lt;strong&gt;Verwaltung &lt;/strong&gt;von &lt;strong&gt;Vermögen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste &lt;/strong&gt;Form der &lt;strong&gt;Unterhaltspflicht&lt;/strong&gt;: &lt;strong&gt;Zweckbindung &lt;/strong&gt;es &lt;strong&gt;Kindesvermögens&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aussteuer &lt;/strong&gt;(Ausstattung) bei Ausscheiden des Kindes &lt;strong&gt;aus Muntgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Uneheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gleichberechtigt &lt;/strong&gt;wenn in Hausverband &lt;strong&gt;aufgenommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Christlicher &lt;/strong&gt;Einfluss:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Verlust Erbrecht &lt;/strong&gt;gegen Vater&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Ausschluss &lt;/strong&gt;aus &lt;strong&gt;Berufen &lt;/strong&gt;und &lt;strong&gt;Zünften&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;keine kirchlichen &lt;/strong&gt;Ämter&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Eheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unterhalt &lt;/strong&gt;Vater, &lt;strong&gt;Pflege &lt;/strong&gt;Mutter&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater &lt;strong&gt;gesetzlicher Vertreter&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater &lt;strong&gt;verwaltet Kindesvermögen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kind erhält &lt;strong&gt;Familien&lt;/strong&gt;+ &lt;strong&gt;Standesrecht &lt;/strong&gt;des &lt;strong&gt;Vaters&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Uneheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bis 1. TN &lt;strong&gt;kein Verwandtschaftsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dann gegenüber Mutter &lt;/strong&gt;gleiche Rechte &lt;strong&gt;wie eheliche&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater: &lt;strong&gt;Unterhaltsanspruch&lt;/strong&gt;, &lt;strong&gt;Besuchsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ehe- und Familienmodell ABGB 1811 und welches war davor?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;patriarchales &lt;/strong&gt;Familienmodell - "&lt;strong&gt;Überlegenheit &lt;/strong&gt;des &lt;strong&gt;Mannes&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;davor&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vernunftrechtliche &lt;/strong&gt;Familie: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ansätze partnerschaftlichen &lt;/strong&gt;Modells&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Recht auf &lt;strong&gt;Persönlichkeitsentfaltung Frau &lt;/strong&gt;+ &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Selbstbestimmungsrecht der Frau bei Ehe - früher und heute?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Frau unter &lt;strong&gt;Muntgewalt &lt;/strong&gt;- wenig Selbstbestimmung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Mittelalter&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Besserstellung &lt;/strong&gt;der Frau durch &lt;strong&gt;christlichen &lt;/strong&gt;Einfluss&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehemann vertrat &lt;/strong&gt;Frau vor &lt;strong&gt;Gericht &lt;/strong&gt;und bei &lt;strong&gt;Rechtsgeschäften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Frau &lt;/strong&gt;konnte &lt;strong&gt;alltägliche Rechtsgeschäfte &lt;/strong&gt;&lt;em&gt;für Mann &lt;/em&gt;durchführen&lt;/li&gt;&lt;li&gt;Aufkommen &lt;strong&gt;gegenseitiger Treuepflicht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeit&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leitungsfunktion &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;ausgebaut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verpflichtung &lt;/strong&gt;der &lt;strong&gt;Sicherung &lt;/strong&gt;des &lt;strong&gt;Unterhalts &lt;/strong&gt;der Frau&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Treue- und Beistandspflicht usus (aber nicht rechtlich verankert)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Naturrechtliche Lehre&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Katalog&lt;strong&gt; gegenseitige Rechte &lt;/strong&gt;und &lt;strong&gt;Pflichten &lt;/strong&gt;der Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Seit &lt;em&gt;Familienrechtsreform 1975&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;eheliche &lt;strong&gt;Gleichberechtigung &lt;/strong&gt;von Mann und Frau&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Seit wann gibt es in Österreich die Zivilehe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Seit den &lt;strong&gt;Maigesetzen 1868&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Notzivilehe &lt;/strong&gt;-&amp;gt; ohne kanonische Vorschriften&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Seit &lt;em&gt;1945&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;obligatorische&lt;/em&gt; Zivilehe&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Eliminierung &lt;/strong&gt;der &lt;strong&gt;nationalsozialistischen &lt;/strong&gt;Bestimmungen des &lt;strong&gt;dt. Ehegestez 1938&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Übernahme &lt;/strong&gt;ins &lt;strong&gt;ABGB&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eheschließung bis ABGB 1811&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Mittelalter: &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mehrere&lt;/strong&gt; &lt;strong&gt;Formen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Kirche &lt;/em&gt;hatte &lt;em&gt;Ehehoheit &lt;/em&gt;&lt;/li&gt;&lt;li&gt;Siehe Frage "&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Welche Arten der Ehe gab es im Mittelalter?"&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kompetenzkonflikt &lt;/strong&gt;Kirche vs Staat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Staatliches &lt;/strong&gt;Eherecht &lt;strong&gt;als&lt;/strong&gt; &lt;strong&gt;zweites&lt;/strong&gt;, ebenso &lt;strong&gt;gültiges&lt;/strong&gt;, Eherecht &lt;strong&gt;neben Kirchlichem&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;18 JH (vernunftrechtlische Naturrecht) &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehe dient &lt;/strong&gt;dem&lt;strong&gt; Staats&lt;/strong&gt;interesse&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;polizeistaatliches Ehemodell&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Joseph II 1783&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trennung Ehesakrament&lt;/strong&gt; &lt;strong&gt;Ehevertrag&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;nicht obligatorische &lt;/strong&gt;Zivilehe&lt;/li&gt;&lt;li&gt;Siehe Karte&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;dreigeteilt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Siehe Karte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hat es eine Zeit gegeben, in der das kanonische Recht auch für Katholiken-Ehen gegolten hat?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zwischen Konkordat 1855 und Maigesetze 1868&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die weitere Entwicklung des Eherechts nach ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Konkordat 1855&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit Kirche &lt;/strong&gt;unterstellt&lt;/li&gt;&lt;li&gt;&lt;em&gt;Maigesetze 1868 &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Notzivilehe &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wiederherstellung &lt;/strong&gt;Eherecht &lt;strong&gt;ABGB &lt;/strong&gt;1811&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit &lt;/strong&gt;wieder &lt;strong&gt;staatlich &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Festsetzung &lt;strong&gt;Monogamie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;keine &lt;/strong&gt;Möglichkeit der &lt;strong&gt;Scheidung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dispensehe 1919 &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Frage dazu&lt;/li&gt;&lt;li&gt;&lt;em&gt;Konkordat 1934&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eherecht&lt;/strong&gt; für &lt;strong&gt;Katholiken&lt;/strong&gt; wieder an &lt;strong&gt;Kirche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dt. Ehegesetz 1938&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;einheitliches Eherecht &lt;/strong&gt;im ganzen Reich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;siehe Frage dazu&lt;/li&gt;&lt;li&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übernommen aus &lt;strong&gt;Ehegesetz 1938 &lt;/strong&gt;"&lt;strong&gt;entnazifizert&lt;/strong&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Obligatorische Zivilehe &lt;/strong&gt;für alle Konfessionen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eherecht ABGB 1811 - Unterschied zu heute&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ABGB &lt;/em&gt;hatte (anders als heute) &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dreifach gegliedertes &lt;/strong&gt;Eherecht: Katholiken, Protestanten, Juden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehehindernis&lt;/strong&gt;: Wiederverheiratung nicht möglich, solange &lt;strong&gt;katholischer&lt;/strong&gt; &lt;strong&gt;Ehepartner noch lebt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Keine &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Zivilehe&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Güterstand im Älteren Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Vermögenstrennung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;hat Recht auf &lt;strong&gt;Verwaltung &lt;/strong&gt;+ &lt;strong&gt;Nutzung &lt;/strong&gt;von &lt;strong&gt;Frauenvermögen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Leibgedinge&lt;/em&gt;: &lt;strong&gt;unentgeltliches Nutzungsrecht &lt;/strong&gt;auf Lebenszeit an einem Objekt des Ehepartners.&lt;/li&gt;&lt;li&gt;&lt;em&gt;Heiratsgabensystem&lt;/em&gt;: &lt;strong&gt;Heimsteuer &lt;/strong&gt;+ &lt;strong&gt;Widerlage&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Heiratsgabensystem im Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;= Zur &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Heimsteuer&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Heiratsgabe der &lt;strong&gt;Frau &lt;/strong&gt;- Zuschuss zu finanziellen Lasten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gegengewicht &lt;/strong&gt;zu &lt;strong&gt;Mann &lt;/strong&gt;als einzige &lt;strong&gt;Einnahmequelle&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Widerlage &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;fällig bei (&lt;strong&gt;Vor&lt;/strong&gt;)&lt;strong&gt;Tod&lt;/strong&gt; des &lt;strong&gt;Mannes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;wenn Heimsteuer &lt;/strong&gt;geleistet wurde&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Im &lt;strong&gt;Todesfalle &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;-&amp;gt; beides zusammen zur &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Güterstand im Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;beschränkte Gütergemeinschaft &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur für &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;bestimmte&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Objekte&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(z.B.: &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Liegenschaften&lt;/span&gt;)&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;Gesamthand&lt;/strong&gt;" -&amp;gt; Rechtsgeschäfte erfordern Zu&lt;strong&gt;stimmung beider&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Errungenschaftsgemeinschaften&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;der &lt;strong&gt;beschränkten &lt;/strong&gt;Gütergemeinschaft&lt;/li&gt;&lt;li&gt;Auch &lt;strong&gt;zukünftiges Vermögen &lt;/strong&gt;miteinbezogen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Fahrnisgemeinschaft&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Errungenschaften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eingebrachte&lt;/strong&gt; und &lt;strong&gt;unentgeltlich erworbene &lt;/strong&gt;&lt;em&gt;Fahrnis&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Rentleinsheirat&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;allgemeine &lt;/strong&gt;&lt;strong&gt;Gütergemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;eingebrachtes&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erworbenes&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Vermögen beider&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die große Familienrechtsreform?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1970er&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Verwirklichung des &lt;strong&gt;Gleichberechtigungsgrundsatzes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;elterliche Gleichberechtigung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;verstärkter&lt;strong&gt; Schutz&lt;/strong&gt; der &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anerkennung&lt;/strong&gt; der &lt;strong&gt;Privatautonomie &lt;/strong&gt;im &lt;strong&gt;familiären &lt;/strong&gt;Bereich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Polizeistaatliche Familienmodell?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Christliche &lt;strong&gt;Familie &lt;/strong&gt;hatte &lt;strong&gt;im MA &lt;/strong&gt;im &lt;strong&gt;Obrigkeitsstaat &lt;/strong&gt;eine &lt;strong&gt;staatsdienende&lt;/strong&gt; Bedeutung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wurde durch &lt;strong&gt;aristotelische Hauslehre &lt;/strong&gt;erklärt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hausherr&lt;/strong&gt; sorgt für &lt;em&gt;obrigkeitstreues Verhalten &lt;/em&gt;der &lt;strong&gt;Hausgenossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Staat überwacht &lt;/strong&gt;die Pflichterfüllung des &lt;strong&gt;Hausherrn&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Familie &lt;/strong&gt;war also &lt;strong&gt;Element &lt;/strong&gt;des &lt;strong&gt;Polizeistaats&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Beziehung der Ehegatten untereinander im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;als "&lt;strong&gt;Haupt&lt;/strong&gt;" der Familie&lt;/li&gt;&lt;li class="ql-indent-1"&gt;hat &lt;strong&gt;Unterhaltspflicht &lt;/strong&gt;und &lt;strong&gt;Leitungsrecht&lt;/strong&gt; &lt;strong&gt;gegenüber Frau&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ansicht der "traditionelle Rollenverteilung"&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Aristotelische Hauslehre?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Haus &lt;/strong&gt;(Familie) ist &lt;strong&gt;Teil &lt;/strong&gt;einer &lt;strong&gt;übergeordneten Gemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestimmt den &lt;em&gt;Sozialstatus &lt;/em&gt;der Menschen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater vertritt &lt;/strong&gt;Familie nach außen &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater &lt;/strong&gt;hat &lt;strong&gt;Gewalt &lt;/strong&gt;über &lt;strong&gt;Hausgemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Majorenitäts-Jahresbestimmung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Volljährigkeit &lt;/strong&gt;in allen &lt;strong&gt;dt. Erbkönigreichen&lt;/strong&gt; und &lt;strong&gt;Ländern &lt;/strong&gt;auf &lt;strong&gt;24 Jahre&lt;/strong&gt; festgesetzt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Fähigkeiten kommen abgeschichteten Söhnen zu?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vermögensrechtlich Selbständig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Familiengründung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;etc&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet Abschichtung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Erreichen der &lt;strong&gt;Mündigkeit &lt;/strong&gt;von &lt;strong&gt;Haussöhnen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Nach &lt;strong&gt;Ausscheiden &lt;/strong&gt;aus dem &lt;strong&gt;väterlichen Haushalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Teilbereiche der Handlungsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Deliktsfähigkeit&lt;/em&gt;: Fähigkeit, sich durch &lt;strong&gt;rechtswidriges Verhalten&lt;/strong&gt; zu &lt;strong&gt;verpflichten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Geschäftsfähigkeit&lt;/em&gt;: Fähigkeit sich durch &lt;strong&gt;Rechtsgeschäfte&lt;/strong&gt; zu &lt;strong&gt;verpflichten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die allgemeine (unbeschränkte) Rechtsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Recht der&lt;/strong&gt; &lt;strong&gt;Persönlichkeit&lt;/strong&gt; im &lt;em&gt;Naturrecht&lt;/em&gt; und &lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Siehe auch Frage "Statuslehre"&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Statuslehre?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;röm Recht übernommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;libertatis&lt;/strong&gt;: &lt;em&gt;Freie&lt;/em&gt; vs &lt;em&gt;Sklaven&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;civitatis&lt;/strong&gt;: &lt;em&gt;Bürger &lt;/em&gt;vs &lt;em&gt;Fremde&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;familiae&lt;/strong&gt;: &lt;em&gt;Zugehörigkeit &lt;/em&gt;zu &lt;em&gt;Familie&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Entwicklung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Codex &lt;strong&gt;Theresianus &lt;/strong&gt;folgte &lt;strong&gt;Statuslehre&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ablösung &lt;/strong&gt;durch &lt;strong&gt;naturrechtliche &lt;/strong&gt;Vorstellungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Recht der Persönlichkeit&lt;/em&gt; (angeborenes Recht, &lt;strong&gt;frei zu handeln &lt;/strong&gt;und seine &lt;strong&gt;Würde &lt;/strong&gt;zu &lt;strong&gt;behaupten&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;= Allgemeine (unbeschränkte) Rechtsfähigkeit&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Übernahme&lt;/strong&gt; ins &lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Abhängigkeit der Bauern?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geteilt in &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;freie &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unfreie &lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Leibeigenschaft &lt;/strong&gt;in&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; Ö &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;nicht institutionalisiert&lt;/strong&gt;, &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;aber &lt;/span&gt;diverse &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Einschränkungen &lt;/strong&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Abhängigkeiten&lt;/span&gt; der &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unfreien &lt;/em&gt;&lt;em&gt;Bauern&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Sachenrechtlich &lt;/em&gt;(&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Abgaben &lt;/strong&gt;für Grund und Boden)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Politisch &lt;/em&gt;(&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundherr &lt;/span&gt;hatte &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichts&lt;/strong&gt;- und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Verwaltungsaufgaben&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Persönlich &lt;/em&gt;(&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Heiratsbewilligung&lt;/strong&gt;, befohlene &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Tätigkeit&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wohnsitzentscheidungen&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ab &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;16. JH&lt;/em&gt; (&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Bauernkriege&lt;/strong&gt;) -&amp;gt; Trend zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufhebung &lt;/strong&gt;der &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;persönlichen Abhängigkeit&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erst &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;18/19 JH beseitigt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Aufgaben hatte das Ehegüterrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Versorgung &lt;/strong&gt;des &lt;strong&gt;überlebenden &lt;/strong&gt;Ehegatten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufteilung &lt;/strong&gt;der &lt;strong&gt;finanziellen &lt;/strong&gt;Lasten (Finanzieller &lt;strong&gt;Beitrag der&lt;/strong&gt; &lt;strong&gt;Frau &lt;/strong&gt;wurde gefordert) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist mit Geschlechtervormundschaft gemeint?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Frau &lt;/strong&gt;ist &lt;strong&gt;immer unter &lt;/strong&gt;der &lt;strong&gt;Muntgewalt&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Väterliche Munt &lt;/em&gt;bis zur Verheiratung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dann &lt;em&gt;eheherrliche Munt&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Bei Ableben des Vaters vor Hochzeit:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;verwandsschaftliche Munt &lt;/em&gt;(Bruder oder anderer männl. Verwandter)&lt;/li&gt;&lt;li&gt;als Witwe entweder Munt der Verwandschaft oder des toten Ehemanns&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Salvatorische Klausel?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nach der Salvatorischen Klausel sollte das &lt;strong&gt;ius commune &lt;/strong&gt;nur &lt;strong&gt;subsidiär &lt;/strong&gt;gelten&lt;/p&gt;&lt;ul&gt;&lt;li&gt; &lt;strong&gt;Geltungsnachweises &lt;/strong&gt;für das &lt;strong&gt;Gewohnheitsrecht &lt;/strong&gt;war jedoch &lt;strong&gt;schwierig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher &lt;strong&gt;Trendumkehr&lt;/strong&gt;: Gegner musste &lt;em&gt;Beweis der Nichtrezeption&lt;/em&gt; erbringen, um das &lt;strong&gt;Gewohnheitsrecht durchzusetzen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Aussteuer?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mitgift&lt;/strong&gt; der &lt;strong&gt;Familie&lt;/strong&gt; der &lt;strong&gt;Frau&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;auch &lt;strong&gt;Heimsteuer&lt;/strong&gt; genannt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Güterstand in der Neuzeit/Rezeption?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundsätzlich &lt;/strong&gt;MA Prinzip der &lt;strong&gt;Gütertrennung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aber &lt;strong&gt;Vielzahl vertraglicher Gütergemeinschaftstypen &lt;/strong&gt;kamen auf&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann brauchte man das Erbenlob außer beim Veräußern?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bei &lt;strong&gt;Verpfändung &lt;/strong&gt;(nach &lt;strong&gt;älteren &lt;/strong&gt;Satzung) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wodurch wurde die väterliche Munt eingeschränkt/kontrolliert?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zugriff&lt;/strong&gt; aufs &lt;strong&gt;Kindesvermögen &lt;/strong&gt;rechtl. &lt;strong&gt;eingeschränkt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;"Kindesgut ist eisern Gut"&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur &lt;strong&gt;verwalten&lt;/strong&gt; und &lt;strong&gt;nutzen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Substanz &lt;/strong&gt;durfte &lt;strong&gt;nicht angegriffen &lt;/strong&gt;werden&lt;/li&gt;&lt;li&gt;&lt;em&gt;Erbenlaub/Erbenlob&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbgut &lt;/strong&gt;und &lt;strong&gt;Liegenschaften&lt;/strong&gt; nur mit &lt;strong&gt;Zustimmung &lt;/strong&gt;der Kinder &lt;strong&gt;veräußert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Grund für Religionsspezifische Regeln im Eherecht im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Staat&lt;/strong&gt; hatte &lt;strong&gt;Interesse &lt;/strong&gt;daran &lt;strong&gt;Ehe gesetzlich &lt;/strong&gt;zu &lt;strong&gt;regeln &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Formell&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Inhaltlich &lt;/strong&gt;aber &lt;strong&gt;Regeln&lt;/strong&gt; &lt;strong&gt;der Konfessionen &lt;/strong&gt;übernommen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Materiell&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verhindert&lt;/strong&gt;, dass &lt;strong&gt;Gläubige &lt;/strong&gt;durch staatl. &lt;strong&gt;Eherecht gezwungen&lt;/strong&gt; sind &lt;strong&gt;gegen Regeln &lt;/strong&gt;ihrer &lt;strong&gt;Konfession&lt;/strong&gt; zu &lt;strong&gt;verstoßen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer ist normalerweise Erbe im MA?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gut an &lt;strong&gt;Sippe gebunden &lt;/strong&gt;- &lt;strong&gt;Gesamthand&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Anwachsung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;später im MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Parentelerbfolge&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Das Gut rinnt wie das Blut&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Deszendenten &lt;/strong&gt;vor &lt;strong&gt;Aszendeten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frauen subsidiär&lt;/strong&gt; -&amp;gt; nur wenn keine männlichen Erben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Welche Liegenschaftsgewere werden unterschieden? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Liegenschaftsrecht&lt;/strong&gt;: auch &lt;strong&gt;Gewere &lt;/strong&gt;zuerkannt, &lt;strong&gt;wer &lt;/strong&gt;bloß &lt;strong&gt;mittelbare&lt;/strong&gt; &lt;strong&gt;Nutzung &lt;/strong&gt;aus der Sache &lt;strong&gt;zog&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unterscheidung "&lt;strong&gt;Nutzen&lt;/strong&gt;" und "&lt;strong&gt;Brauchen&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Arten d. Gewere:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Unmittelbare &lt;/strong&gt;Gewere &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;leiheberechtigter Bauer&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bearbeitete&lt;/strong&gt; Liegenschaft und &lt;strong&gt;zog Nutzen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mittelbare &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;Grundherr&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zog Nutzen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Eigengewere &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Umfassendes &lt;em&gt;Herrschaftsrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beschränktes &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;einzelne dingliche &lt;/em&gt;Nutzungsrechte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: &lt;strong&gt;&lt;em&gt;Leibzucht&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;oder &lt;strong&gt;Vormundschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Leibliche &lt;/strong&gt;Gewere &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;unmittelbarer &lt;/em&gt;Besitz bei &lt;em&gt;Innehabung&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ideelle &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;besitzlose &lt;/em&gt;Gewere im Liegenschaftsrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Begründungsakt &lt;/strong&gt;musste &lt;strong&gt;offenkundig &lt;/strong&gt;sein, wie z.B.:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Tod&lt;/strong&gt; des &lt;strong&gt;Erblassers&lt;/strong&gt; (&lt;strong&gt;auch wenn &lt;/strong&gt;jemand &lt;strong&gt;anderer &lt;/strong&gt;sich der &lt;strong&gt;Sache&lt;/strong&gt; &lt;strong&gt;bemächtigt&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gerichtliches Urteil &lt;/strong&gt;zu &lt;strong&gt;Übertragung&lt;/strong&gt;/&lt;strong&gt;Auflassung &lt;/strong&gt;des Grundstücks &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sonderformen&lt;/strong&gt; der &lt;strong&gt;Idellen&lt;/strong&gt; Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ruhende &lt;/strong&gt;Gewere (für &lt;strong&gt;Pfandschuldner&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;anwartschaftliche&lt;/strong&gt; Gewere (z.B.: &lt;strong&gt;Schenkung &lt;/strong&gt;auf den &lt;strong&gt;Todesfall&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Liegenschaftsgewere?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Fahrnisgewere &lt;/strong&gt;nur auf Fälle &lt;strong&gt;unmittelbarer Sachherrschaft &lt;/strong&gt;beschränkt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Liegenschaftsgewere &lt;/strong&gt;auch für &lt;strong&gt;mittelbare &lt;/strong&gt;Nutzung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sachherrschaft über Liegenschaften eine von zwei Formen: Nutzen oder Brauchen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind Fahrnisgewere?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gewere an &lt;strong&gt;beweglicher Sache &lt;/strong&gt;(Fahrnis) untrennbar &lt;strong&gt;an&lt;/strong&gt; &lt;strong&gt;körperliche Innehabung gebunden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erworben &lt;/strong&gt;durch &lt;strong&gt;Ergreifen &lt;/strong&gt;oder &lt;strong&gt;Übergabe von Hand zu Hand&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geht mit &lt;strong&gt;Verlust &lt;/strong&gt;der &lt;strong&gt;körperlichen Herrschaft verloren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Recht der &lt;strong&gt;Fahrnisverfolgung im älteren Recht&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Strenge &lt;strong&gt;Unterscheidung &lt;/strong&gt;zwischen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;freiwilliger&lt;/strong&gt; &lt;strong&gt;Besitzaufgabe&lt;/strong&gt; (&lt;em&gt;Hand wahre Hand&lt;/em&gt;) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;und &lt;strong&gt;unfreiwilligem Besitzverlust &lt;/strong&gt;(&lt;em&gt;Anefangsklage, Dritthandverfahren&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet „Hand wahre Hand“?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;War die Sache bereits in die &lt;strong&gt;Hand eines Dritten gelangt&lt;/strong&gt;, so galt das mittelalterliche &lt;strong&gt;Rechtssprichwort &lt;/strong&gt;„&lt;em&gt;Wo du deinen Glauben gelassen hast, dort sollst du ihn auch suchen&lt;/em&gt;“ oder „&lt;em&gt;Hand wahre Hand&lt;/em&gt;“. &lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;Eigentümer einer beweglichen &lt;/strong&gt;Sache, der diese einem &lt;strong&gt;anderen anvertraut &lt;/strong&gt;hat, kann diese &lt;strong&gt;nur von diesem&lt;/strong&gt;, nicht von einem Dritten &lt;strong&gt;herausverlangen&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;basierend auf &lt;strong&gt;Publizitätsgedanken &lt;/strong&gt;des &lt;strong&gt;Fahrnisrecht&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;der &lt;strong&gt;Dritte kennt&lt;/strong&gt; den &lt;strong&gt;Besitz &lt;/strong&gt;(&lt;em&gt;leibliche Gewere&lt;/em&gt;) des Entlehners,&lt;strong&gt; aber nicht den Rechtsmangel&lt;/strong&gt; des Vertrauensmannes&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Heute: &lt;strong&gt;gutgläubiger Erwerb vom Nichtberechtigten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Dritthandverfahren?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Teil der &lt;strong&gt;Anefangklage &lt;/strong&gt;(mittelalterlicher &lt;strong&gt;Rechtsbehelf &lt;/strong&gt;gegen eine &lt;strong&gt;abhandengekommene Sache &lt;/strong&gt;war)&lt;/li&gt;&lt;li&gt;Für die &lt;strong&gt;Klageerhebung &lt;/strong&gt;war das &lt;strong&gt;außergerichtliche Anfassen &lt;/strong&gt;der beweglichen Sache (&lt;strong&gt;Fahrnis&lt;/strong&gt;) zwingend &lt;strong&gt;erforderlich &lt;/strong&gt;(diese Handlung bezeichnete genau die Sache, die abhandengekommen war)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dadurch wurde &lt;strong&gt;klar&lt;/strong&gt;, dass die &lt;strong&gt;Sache dem Kläger abhandengekommen &lt;/strong&gt;ist.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;aktuelle Besitzer &lt;/strong&gt;musste zur &lt;strong&gt;Exkulpation &lt;/strong&gt;einen &lt;strong&gt;Dritten &lt;/strong&gt;bzw einen &lt;strong&gt;Vormann &lt;/strong&gt;öffentlich &lt;strong&gt;benennen&lt;/strong&gt;,&lt;/li&gt;&lt;li class="ql-indent-2"&gt;von dem sich seine &lt;strong&gt;rechtmäßige&lt;/strong&gt; &lt;strong&gt;Gewere ableitet&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Konnte &lt;/strong&gt;er das &lt;strong&gt;nicht&lt;/strong&gt;, war er als &lt;strong&gt;Dieb &lt;/strong&gt;überführt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Deshalb &lt;/strong&gt;heißt das Verfahren auch &lt;strong&gt;Dritthandverfahren&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Bedeutung von Munt im Älteren Recht? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Munt = &lt;strong&gt;väterliche Gewalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Personen unter Munt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;beschränkt Geschäftsfähig&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nicht verpflichtungsfähig&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zustimmung &lt;/strong&gt;des &lt;strong&gt;Muntwalts &lt;/strong&gt;erforderlich (&lt;em&gt;Gewere zur rechten Vormundschaft&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mündel konnte &lt;strong&gt;Rechtsgeschäfte &lt;/strong&gt;nach &lt;strong&gt;Erreichen&lt;/strong&gt; der &lt;strong&gt;Mündigkeit widerrufen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schutz &lt;/strong&gt;vor Leichtsinn/&lt;strong&gt;Vermögensverschleuderung&lt;/strong&gt; durch &lt;strong&gt;Muntwalt &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Muntgewalt?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gewalt des Hausvaters&lt;/strong&gt; über &lt;strong&gt;alle im Haus lebenden Personen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;gegliedert in &lt;strong&gt;Herrschafts&lt;/strong&gt;- und &lt;strong&gt;Schutzverhältnis&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dritten &lt;/strong&gt;gegenüber übernahm der Munt(walt) eine &lt;strong&gt;Schutzfunktion&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;im &lt;strong&gt;Innenverhältnis &lt;/strong&gt;stand der &lt;strong&gt;Herrschaftsaspekt &lt;/strong&gt;im Vordergrund. &lt;/li&gt;&lt;li&gt;Die Muntgewalt zerfiel ferner in die &lt;strong&gt;väterliche&lt;/strong&gt;, &lt;strong&gt;eheliche &lt;/strong&gt;und &lt;strong&gt;gesinderechtliche und/oder vormundschaftsrechtliche Munt&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind ältere und jüngere Satzung? (Altes/Neues Pfandrecht)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Es geht um &lt;strong&gt;Pfandrecht&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ältere Satzung:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Ursprünglich&lt;/em&gt;&lt;/strong&gt;: &lt;strong&gt;Sicherheitsübereignung&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;G&lt;/strong&gt; erhielt &lt;strong&gt;Eigentum &lt;/strong&gt;durch Kauf von S&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;S &lt;/strong&gt;hatte &lt;strong&gt;Wiederkaufsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Später&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;S&lt;/strong&gt; hatte &lt;strong&gt;ruhende Eigengewere&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;G&lt;/strong&gt; hatte &lt;strong&gt;leibliche Gewere&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;-&amp;gt; Besitzpfand&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Entweder &lt;strong&gt;Ewigsatzung &lt;/strong&gt;oder &lt;strong&gt;Totsatzung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Benötigte &lt;em&gt;Erbenlaub!&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reine Sachhaftung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Jüngere Satzung:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Situation &lt;/strong&gt;von &lt;strong&gt;S und G&lt;/strong&gt; im Vergleich zur älteren Satzung &lt;strong&gt;umgedreht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;S&lt;/strong&gt; behält &lt;strong&gt;leibliche &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;G&lt;/strong&gt; erhält &lt;strong&gt;anwartschaftliche &lt;/strong&gt;Gewere &lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Besitzloses Pfand&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mehrfachverpfändung &lt;/strong&gt;möglich &lt;/li&gt;&lt;li class="ql-indent-1"&gt;in &lt;strong&gt;älterer Satzung&lt;/strong&gt; &lt;strong&gt;nicht&lt;/strong&gt;, weil ja an Gläubiger übereignet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Primär Sachhaftung&lt;/strong&gt;, &lt;strong&gt;subsidiär Vermögenshaftung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Güterstand ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Gütertrennung&lt;/strong&gt; in der &lt;strong&gt;Ehe &lt;/strong&gt;-&amp;gt; jeder hatte sein &lt;strong&gt;eigenes Vermögen&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aber: &lt;strong&gt;Zweifelsregelungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sogn. "&lt;strong&gt;verschämte&lt;/strong&gt; &lt;strong&gt;Gütergemeinschaft&lt;/strong&gt;" bzw "&lt;strong&gt;vermutete Verwaltungsgemeinschaft&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Im&lt;/strong&gt; &lt;strong&gt;Zweifel &lt;/strong&gt;wird vermutet:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dass &lt;strong&gt;Erwerb vom&lt;/strong&gt; &lt;strong&gt;Mann &lt;/strong&gt;stammt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dass Frau &lt;strong&gt;bis auf&lt;/strong&gt; &lt;strong&gt;Widerruf &lt;/strong&gt;die &lt;strong&gt;Verwaltung &lt;/strong&gt;des &lt;strong&gt;Vermögens &lt;/strong&gt;dem &lt;strong&gt;Mann&lt;/strong&gt; anvertraut hat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mann haftet &lt;/strong&gt;als Verwalter des Frauenvermögens für &lt;strong&gt;Stammgut &lt;/strong&gt;und &lt;strong&gt;Kapital&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Reallasten, Rentenkauf?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reallast: dinglich wirkende Belastung&lt;/strong&gt; eines &lt;strong&gt;Grundstücks&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;für &lt;strong&gt;bestimmte&lt;/strong&gt;, idR &lt;strong&gt;wiederkehrende&lt;/strong&gt; &lt;strong&gt;Leistungen &lt;/strong&gt;des &lt;strong&gt;Eigentümers&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;Leistungsverpflichtete &lt;/strong&gt;wird also über das &lt;strong&gt;Eigentum &lt;/strong&gt;am Grundstück &lt;strong&gt;bestimmt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wesentlich&lt;strong&gt;: sachliche Haftung&lt;/strong&gt; -&amp;gt; &lt;strong&gt;verdinglichte&lt;/strong&gt; &lt;strong&gt;Leistungspflicht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Haftung &lt;/strong&gt;auch &lt;strong&gt;persönlich &lt;/strong&gt;für fällig gewordenen &lt;strong&gt;Leistungen!&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Arten:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dienstleistungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgabe von &lt;strong&gt;Produkten&lt;/strong&gt; des &lt;strong&gt;Grundstücks&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geldrenten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Einschränkung&lt;/strong&gt;: &lt;strong&gt;Leistung &lt;/strong&gt;und &lt;strong&gt;wirtschaftliche Beschaffenheit &lt;/strong&gt;des &lt;strong&gt;GS &lt;/strong&gt;müssen &lt;strong&gt;zusammenhängen&lt;/strong&gt; (&lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;willkürlichen &lt;/strong&gt;Verpflichtungen)&lt;/li&gt;&lt;li&gt;In Ö: keine geschlossene gesetzliche Regelung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Älteres Recht: &lt;/em&gt;Viele&lt;/strong&gt; Arten der Reallasten&lt;/p&gt;&lt;p&gt;&lt;strong&gt;→ &lt;em&gt;Obrigkeitliche&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;Reallasten:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;in Form von &lt;strong&gt;Grundzins&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;basierte auf &lt;strong&gt;wirtschaftlichem &lt;/strong&gt;und &lt;strong&gt;herrschaftlichem&lt;/strong&gt; &lt;strong&gt;Abhängigkeitsverhältnis&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;→ &lt;em&gt;privatrechtliche &lt;/em&gt;&lt;/strong&gt;Reallasten:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;seit &lt;strong&gt;hohem MA&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;kein Abhängigkeitsverhältnis&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ältere &lt;/strong&gt;Reallast: &lt;strong&gt;wiederkehrende Abgaben&lt;/strong&gt; des &lt;strong&gt;Gewere&lt;/strong&gt;inhabers an &lt;strong&gt;Träger &lt;/strong&gt;geistlicher und weltlicher &lt;strong&gt;Hoheitsgewalt &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Neuere &lt;/strong&gt;Reallast:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;entsprach &lt;strong&gt;Kredit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;begründet durch &lt;strong&gt;dingliche Einigung&lt;/strong&gt; der Vertragspartner vor &lt;strong&gt;Gericht &lt;/strong&gt;+ &lt;strong&gt;Eintragung &lt;/strong&gt;in &lt;strong&gt;öffentliche Bücher&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rentenkäufer &lt;/strong&gt;bekommt &lt;strong&gt;Grundrente &lt;/strong&gt;aus &lt;strong&gt;Teil &lt;/strong&gt;des &lt;strong&gt;Ertragswertes&lt;/strong&gt; der Liegenschaft&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eigentümer (&lt;strong&gt;Reallastverpflichteter&lt;/strong&gt;) leistet &lt;strong&gt;Natural&lt;/strong&gt;-, &lt;strong&gt;Dienst&lt;/strong&gt;- oder &lt;strong&gt;Geldleistungen&lt;/strong&gt; an &lt;strong&gt;Rentenkäufer&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bei &lt;strong&gt;Nichterbringung&lt;/strong&gt;: &lt;strong&gt;Haftung &lt;/strong&gt;mit &lt;strong&gt;Grundstück&lt;/strong&gt;, aber &lt;strong&gt;nicht persönlich&lt;/strong&gt; oder mit übrigem &lt;strong&gt;Vermögen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;reine&lt;/strong&gt; &lt;strong&gt;Sachhaftung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Befriedigung &lt;/strong&gt;aus dem belasteten Grundstück&lt;/li&gt;&lt;li class="ql-indent-1"&gt;im &lt;strong&gt;Hochmittelalter&lt;/strong&gt;: &lt;strong&gt;eigenständige &lt;/strong&gt;Verpfändung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ausgehendes &lt;/strong&gt;Mittelalter: &lt;strong&gt;gerichtliche &lt;/strong&gt;Verpfändung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das (&lt;em&gt;neuzeitliche&lt;/em&gt;) Parentelensystem?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Parentelen&lt;/strong&gt;: sind &lt;strong&gt;Verwandte&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;nähere &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verwandte &lt;/span&gt;des &lt;strong&gt;Erblassers &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;schließen &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;weitere aus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;neuzeitliches &lt;/strong&gt;System geht auf Kaiser &lt;strong&gt;Joseph II&lt;/strong&gt; zurück&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Parentelensystem &lt;/strong&gt;ist Teil der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;gesetzlichen &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbfolge&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;also &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;subsidiär&lt;/strong&gt;, &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;wenn &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;keine letztwillige &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verfügung&lt;/span&gt;!&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;neben Parentelensystem, &lt;/strong&gt;ab &lt;em&gt;ABGB 1811&lt;/em&gt;: &lt;strong&gt;Ehegatte &lt;/strong&gt;steht &lt;strong&gt;&lt;em&gt;gesetzliches &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Vorausvermächtnis &lt;/em&gt;zu (&lt;strong&gt;bewegliche Sachen &lt;/strong&gt;aus Haushalt, heute auch: Verbleib in &lt;strong&gt;ehelicher Wohnung&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;System Kaiser &lt;strong&gt;Josephs&lt;/strong&gt;: &lt;strong&gt;6 Parentelen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ABGB 1811&lt;/strong&gt;: Grenze bei &lt;strong&gt;4. Parentele&lt;/strong&gt;, d.h. in der &lt;strong&gt;vierten &lt;/strong&gt;Linie &lt;strong&gt;kein Repräsentationsrecht &lt;/strong&gt;der &lt;strong&gt;Nachkommen &lt;/strong&gt;mehr&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Parentelen:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1&lt;/strong&gt;. Parentele: &lt;strong&gt;Deszendenten &lt;/strong&gt;(Kinder) des Erblassers&lt;/li&gt;&lt;li&gt;&lt;strong&gt;2&lt;/strong&gt;. Parentele: &lt;strong&gt;Eltern &lt;/strong&gt;+ &lt;strong&gt;Nachkommen &lt;/strong&gt;(&lt;em&gt;Geschwister&lt;/em&gt;, &lt;em&gt;Nichten,&lt;/em&gt; &lt;em&gt;Neffen&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;3&lt;/strong&gt;. Parentele: &lt;strong&gt;Großeltern &lt;/strong&gt;+ &lt;strong&gt;Nachkommen&lt;/strong&gt; (&lt;em&gt;Tante&lt;/em&gt;, &lt;em&gt;Onkel&lt;/em&gt;, &lt;em&gt;Cousins&lt;/em&gt;, &lt;em&gt;Cousinen&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;4&lt;/strong&gt;. Parentele: nur &lt;strong&gt;Urgroßeltern &lt;/strong&gt;(keine Nachkommen!)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war Erbenlaub/Erbenlob?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zustimmung &lt;/strong&gt;des nächsten &lt;strong&gt;Erben &lt;/strong&gt;zu &lt;strong&gt;Rechtsgeschäften über Erbgut&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Bezeichnung&lt;/em&gt;:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wartrecht &lt;/strong&gt;für im Hausverband Lebende&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beispruchsrecht &lt;/strong&gt;für entfernte Sippengenossen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Wenn &lt;strong&gt;&lt;em&gt;Erbenlob fehlt&lt;/em&gt;&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbenlobberechtigte konnten &lt;strong&gt;innerhalb von 1 Jahr&lt;/strong&gt; das Gut &lt;strong&gt;von jedem Dritten&lt;/strong&gt; &lt;strong&gt;&lt;em&gt;ohne Gegenleistung&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;&lt;strong&gt;herausverlangen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eigentümer&lt;/strong&gt; wurde dann &lt;strong&gt;nicht Erblasser&lt;/strong&gt;, &lt;strong&gt;sondern&lt;/strong&gt; &lt;strong&gt;Erbenlobberechtigter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Entwicklung des Ehegatten&lt;strong&gt;erbrechts&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;heimisches Gewohnheitsrecht &lt;/em&gt;(&lt;strong&gt;älteres &lt;/strong&gt;Recht)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;kein Erbrecht&lt;/strong&gt; des Ehegatten, weil &lt;strong&gt;Eheschließung keine&lt;/strong&gt; &lt;strong&gt;Verwandtschaft &lt;/strong&gt;begründete&lt;/li&gt;&lt;li&gt;Wenn &lt;strong&gt;keine Verwandten&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Fiskus &lt;/strong&gt;erhält Erbgut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kein Bedürfnis &lt;/strong&gt;nach Ausgestaltung des &lt;strong&gt;Ehegattenerbrechts&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;MA&lt;/strong&gt; und &lt;strong&gt;frühe&lt;/strong&gt; &lt;strong&gt;Neuzeit&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Ehegüterrecht &lt;/em&gt;&lt;/strong&gt;für finanzielle Absicherung des Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ansätze &lt;/strong&gt;zur Ausgestaltung des &lt;strong&gt;Ehegattenerbr&lt;/strong&gt;.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ehegüterrechtl&lt;/strong&gt;. Ansprüche wurden mit &lt;strong&gt;Vorstellung von&lt;/strong&gt; &lt;strong&gt;Erbrecht&lt;/strong&gt; &lt;strong&gt;verbunden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;besonders im &lt;strong&gt;Bauernstand&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Üblich: &lt;strong&gt;Ehegatte &lt;/strong&gt;erhält &lt;strong&gt;Hälfte&lt;/strong&gt; der &lt;strong&gt;Errungenschaft &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wichtige &lt;strong&gt;Motivation&lt;/strong&gt;: &lt;strong&gt;unversorgte Witwen &lt;/strong&gt;mangels ehegüterrechtlicher Vereinbarungen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Rezeption &lt;/strong&gt;des gemeinsamen &lt;strong&gt;Ehegattenerbrechts &lt;/strong&gt;im &lt;strong&gt;18 JH&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ehegatte erhielt &lt;strong&gt;Erbrecht nach&lt;/strong&gt; &lt;strong&gt;allen Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;falls ehegüterr&lt;/strong&gt;. &lt;strong&gt;Vereinbarung&lt;/strong&gt;: Ehegatte hat &lt;strong&gt;Wahl &lt;/strong&gt;ob &lt;strong&gt;Ehegüter oder Erbe &lt;/strong&gt;antreten.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sonderstellung unbemittelter &lt;/strong&gt;Gatte: wenn &lt;strong&gt;gänzlich&lt;/strong&gt; &lt;strong&gt;unversorgt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;1/4 des Nachlasses&lt;/strong&gt; (oder &lt;em&gt;Kindeskopfteil &lt;/em&gt;bei &lt;em&gt;vier+ Kindern&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Josephinisches &lt;/strong&gt;&lt;em&gt;Erbfolgepatent &lt;/em&gt;&lt;strong&gt;1786&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehegatte &lt;/strong&gt;wird Erbfolger, &lt;strong&gt;wenn kein&lt;/strong&gt; &lt;strong&gt;Verwandter &lt;/strong&gt;in&lt;strong&gt; 6 Parentelen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Zusätzlich &lt;strong&gt;Fruchtgenussrecht &lt;/strong&gt;an &lt;strong&gt;1/4 des Vermögens &lt;/strong&gt;(&lt;em&gt;endet mit erneuter Ehe&lt;/em&gt;).&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;basierend&lt;/strong&gt; auf &lt;strong&gt;Josephinischem&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fruchtgenuss &lt;/strong&gt;zu unbeschränktem&lt;strong&gt; Eigentum&lt;/strong&gt; &lt;strong&gt;erweitert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;Kind 1/4&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;anderen Erben&lt;/strong&gt; &lt;strong&gt;1/2 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne Verwandte &lt;/strong&gt;in &lt;strong&gt;1+2. Linie&lt;/strong&gt; und &lt;strong&gt;ohne Großeltern&lt;/strong&gt;: &lt;strong&gt;ganze &lt;/strong&gt;Verlassenschaft&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;kein Pflichtteil&lt;/strong&gt;, aber &lt;strong&gt;Vorausvermächtnis &lt;/strong&gt;(&lt;em&gt;bewegliche Sachen &lt;/em&gt;des Haushalts)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;heutiges Ehegattenerbrecht&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;entstand aus &lt;strong&gt;Familienrechtsreform&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anhebung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Erbteils&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilanspruch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erben müssen Ehegatten &lt;strong&gt;verbleib in Wohnung &lt;/strong&gt;ermöglichen (&lt;strong&gt;Schuldrechtl&lt;/strong&gt;. &lt;strong&gt;Anspruch &lt;/strong&gt;des Ehegatten gegen Erben)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehegatte erhält &lt;strong&gt;haushaltszugehörige Sachen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;gewohnte Umgebung&lt;/strong&gt; behalten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der &lt;strong&gt;Freiteil&lt;/strong&gt; (&lt;strong&gt;Sohnesquote&lt;/strong&gt;) bei der Testierfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;das &lt;strong&gt;ganze&lt;/strong&gt; &lt;strong&gt;MA &lt;/strong&gt;hindurch &lt;strong&gt;dominant&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Kirche verlangte&lt;/strong&gt; vom Erblasser eine &lt;strong&gt;Quote &lt;/strong&gt;des &lt;strong&gt;Nachlasses &lt;/strong&gt;-&amp;gt; &lt;em&gt;Freiteil&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gedacht als &lt;strong&gt;Umverteilung &lt;/strong&gt;für die &lt;strong&gt;Armen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Unter &lt;strong&gt;Kaiser Augustinus &lt;/strong&gt;(&lt;em&gt;4./5. JH&lt;/em&gt;): &lt;strong&gt;Freiteilslehre&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine festgesetzte&lt;/strong&gt; Quote -&amp;gt; ein &lt;strong&gt;Sohnesteil &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei 2 Söhnen also 3 Teile -&amp;gt; 1 an Kirche&lt;/li&gt;&lt;li&gt;War im dt. Recht nur &lt;strong&gt;kirchl. Gebot&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber: &lt;strong&gt;Nichteinhaltung &lt;/strong&gt;von Kirche mit &lt;strong&gt;Sakraments&lt;/strong&gt;- und &lt;strong&gt;Begräbnisverweigerung &lt;/strong&gt;sanktioniert&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Besonderheit:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Es gab im &lt;strong&gt;MA ursprünglich keine&lt;/strong&gt; &lt;strong&gt;letztwillige &lt;/strong&gt;Verfügung&lt;/li&gt;&lt;li&gt;also nur &lt;strong&gt;geborene&lt;/strong&gt;, &lt;strong&gt;keine gekorenen Erben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher: &lt;strong&gt;Freiteil&lt;/strong&gt; als &lt;strong&gt;Schenkung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bedingte Schenkung &lt;/strong&gt;auf den &lt;strong&gt;Todesfall&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;oder &lt;strong&gt;sofortige Schenkung &lt;/strong&gt;unter &lt;strong&gt;Vorbehalt&lt;/strong&gt; von &lt;strong&gt;Nießbrauch&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Eherecht/gesetz 1938?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Gesetz zur Vereinheitlichung des Rechts der Eheschließung und der Ehescheidung in Österreich&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Derogierte &lt;/strong&gt;das &lt;strong&gt;Konkordat 1934, &lt;/strong&gt;sowie &lt;strong&gt;ABGB, Sondereherecht für Burgenland&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehe wird zur &lt;strong&gt;reinen Zivilehe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ehe wurde nur &lt;strong&gt;anerkannt&lt;/strong&gt;, &lt;strong&gt;wenn &lt;/strong&gt;alle &lt;strong&gt;gesetzlichen&lt;/strong&gt; &lt;strong&gt;Vorschriften eingehalten &lt;/strong&gt;wurden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Scheidung für alle&lt;/strong&gt; Staatsbürger möglich&lt;/li&gt;&lt;li&gt;umfassend &lt;strong&gt;Ehehindernisrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;klassische Regelungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber auch: Eheschließung zwischen &lt;strong&gt;Juden &lt;/strong&gt;und &lt;strong&gt;Staatsangehörigen&lt;/strong&gt; mit "&lt;strong&gt;deutschem&lt;/strong&gt;" oder "&lt;strong&gt;artverwandtem&lt;/strong&gt;" Blut &lt;strong&gt;verboten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie: &lt;strong&gt;zwischen &lt;/strong&gt;Personen mit &lt;strong&gt;ansteckenden Krankheiten&lt;/strong&gt;, &lt;strong&gt;entmündigten&lt;/strong&gt;, &lt;strong&gt;Geistes&lt;/strong&gt;- oder &lt;strong&gt;Erbkranken&lt;/strong&gt; &lt;strong&gt;verboten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Noch heute "&lt;strong&gt;entnazifiziert&lt;/strong&gt;" &lt;strong&gt;gültig &lt;/strong&gt;aber durch &lt;em&gt;große Familienrechtsreform&lt;/em&gt; der &lt;em&gt;1970er &lt;/em&gt;und &lt;em&gt;Eheänderungsgesetz&lt;/em&gt; &lt;em&gt;1999 &lt;/em&gt;abgeändert&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Mittelalterliche Testament?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Universalsukzession&lt;/strong&gt;, sondern &lt;strong&gt;Sammlung &lt;/strong&gt;von &lt;strong&gt;Singularsukzessionen &lt;/strong&gt;(&lt;em&gt;Legaten&lt;/em&gt;&lt;strong&gt;&lt;em&gt;=&lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Vermächtnissen&lt;/em&gt;) -&amp;gt; wird &lt;strong&gt;Vermächtnistestament &lt;/strong&gt;genannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;benötigte einen &lt;strong&gt;Testamentvollstrecker&lt;/strong&gt;, der &lt;strong&gt;Nachlass &lt;/strong&gt;als &lt;strong&gt;Treuhänder an &lt;/strong&gt;alle &lt;strong&gt;Erben verteilt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verfügung&lt;/strong&gt; zu &lt;strong&gt;frommen&lt;/strong&gt; &lt;strong&gt;Zwecken &lt;/strong&gt;(&lt;em&gt;Freiteilslehre&lt;/em&gt;) &lt;strong&gt;anerkannt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der &lt;strong&gt;Verfügungsfreiheit &lt;/strong&gt;standen &lt;strong&gt;im MA Bindungen des Vermögens&lt;/strong&gt; &lt;strong&gt;an &lt;/strong&gt;die &lt;strong&gt;Familie entgegen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ehefrau &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Kinder&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;mussten &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Inhalt zustimmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Liegenschaften &lt;/strong&gt;und &lt;strong&gt;Erbgut &lt;/strong&gt;konnten &lt;strong&gt;nicht letztwillig &lt;/strong&gt;verfügt werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;außerdem zahlreiche &lt;strong&gt;Verwandtschaftserbfolgeordnungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Testierfreiheit &lt;/strong&gt;also nur &lt;strong&gt;über bestimmte Vermögensmassen &lt;/strong&gt;(z.B.: &lt;em&gt;Kaufgut&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Oft mit &lt;strong&gt;&lt;em&gt;Unwiderruflichkeitsklauseln&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erst im &lt;strong&gt;späten MA&lt;/strong&gt; wurde Testament zu &lt;strong&gt;einseitiger widerruflicher letztwilliger Erklärung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was war das Josephinische Ehepatent von 1783?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anfänge &lt;/strong&gt;der &lt;strong&gt;staatl&lt;/strong&gt;. &lt;strong&gt;Ehegesetzgebung&lt;/strong&gt; schon unter &lt;strong&gt;Maria Theresia&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einschränkung &lt;/strong&gt;der &lt;strong&gt;kirchlichen Macht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;rechtl&lt;/strong&gt;. &lt;strong&gt;Wirkung &lt;/strong&gt;der Ehe &lt;strong&gt;fixiert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Grundlegender &lt;strong&gt;Wandel &lt;/strong&gt;unter&lt;strong&gt; Joseph II: Ehepatent 1783&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Trennung&lt;/strong&gt; zwischen &lt;strong&gt;Ehesakramenten&lt;/strong&gt; und &lt;strong&gt;Ehevertrag &lt;/strong&gt;("&lt;em&gt;Zurückeroberung der legitimen Rechte&lt;/em&gt;")&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kirchl&lt;/strong&gt;. Ehegesetze &lt;strong&gt;formell&lt;/strong&gt; &lt;strong&gt;derogiert &lt;/strong&gt;mit Vorlage eines &lt;strong&gt;bürgerlichen&lt;/strong&gt; &lt;strong&gt;Ehevertrags &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; d.h. &lt;strong&gt;kirchliche &lt;/strong&gt;Ehegesetzgebung &lt;strong&gt;unter bürgerlichen Ehevertrag &lt;/strong&gt;geordnet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bewirkte &lt;strong&gt;keine Umwandlung &lt;/strong&gt;in &lt;strong&gt;obligatorische Zivilehe&lt;/strong&gt;, &lt;strong&gt;geistliche &lt;/strong&gt;verstanden sich bei der &lt;strong&gt;Trauung &lt;/strong&gt;aber &lt;strong&gt;mehr &lt;/strong&gt;als &lt;strong&gt;Staatsdiener&lt;/strong&gt;, &lt;strong&gt;denn &lt;/strong&gt;als &lt;strong&gt;Religionsdiener&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit&lt;/strong&gt; bei &lt;strong&gt;staatlichen Gerichtshöfen &lt;/strong&gt;(&lt;em&gt;Staat DiözesenGH&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehefähigkeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Minderjährige benötigten &lt;/strong&gt;zur Eheschließung &lt;strong&gt;Einwilligung &lt;/strong&gt;von &lt;strong&gt;Vater &lt;/strong&gt;(oder falls dieser Tot: &lt;strong&gt;Großvater väterlicherseits&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehen &lt;strong&gt;ohne Einwilligung&lt;/strong&gt;: "&lt;em&gt;völlig ungültig&lt;/em&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wurde Einwilligung&lt;strong&gt; ohne erhebliche Gründe verweigert &lt;/strong&gt;-&amp;gt; v&lt;strong&gt;on Amts wegen Einwilligung &lt;/strong&gt;bekommen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Mittelalterliche Testament?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Universalsukzession&lt;/strong&gt;, sondern &lt;strong&gt;Sammlung &lt;/strong&gt;von &lt;strong&gt;Singularsukzessionen &lt;/strong&gt;(&lt;em&gt;Legaten&lt;/em&gt;) -&amp;gt; wird &lt;strong&gt;Vermächtnistestament &lt;/strong&gt;genannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;benötigte einen &lt;strong&gt;Testamentvollstrecker&lt;/strong&gt;, der &lt;strong&gt;Nachlass &lt;/strong&gt;als &lt;strong&gt;Treuhänder an &lt;/strong&gt;alle &lt;strong&gt;Erben verteilt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;Verfügungsfreiheit &lt;/strong&gt;standen &lt;strong&gt;im MA Bindungen des Vermögens&lt;/strong&gt; &lt;strong&gt;an &lt;/strong&gt;die &lt;strong&gt;Familie entgegen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Liegenschaften &lt;/strong&gt;und &lt;strong&gt;Erbgut &lt;/strong&gt;konnten &lt;strong&gt;nicht letztwillig &lt;/strong&gt;verfügt werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;außerdem zahlreiche &lt;strong&gt;Verwandtschaftserbfolgeordnungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Testierfreiheit &lt;/strong&gt;also nur &lt;strong&gt;über bestimmte Vermögensmassen &lt;/strong&gt;(z.B.: &lt;em&gt;Kaufgut&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehefrau &lt;/strong&gt;und &lt;strong&gt;Kinder &lt;/strong&gt;mussten &lt;strong&gt;Inhalt zustimmen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Erst im &lt;strong&gt;späten MA&lt;/strong&gt; wurde Testament zu &lt;strong&gt;einseitiger widerruflicher letztwilliger Erklärung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Eherecht/gesetz 1938?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Gesetz zur Vereinheitlichung des Rechts der Eheschließung und der Ehescheidung in Österreich&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Derogierte &lt;/strong&gt;das &lt;strong&gt;Konkordat 1934, &lt;/strong&gt;sowie &lt;strong&gt;ABGB, Sondereherecht für Burgenland&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ehe wurde nur &lt;strong&gt;anerkannt&lt;/strong&gt;, &lt;strong&gt;wenn &lt;/strong&gt;alle &lt;strong&gt;gesetzlichen&lt;/strong&gt; &lt;strong&gt;Vorschriften eingehalten &lt;/strong&gt;wurden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Scheidung für alle&lt;/strong&gt; Staatsbürger möglich&lt;/li&gt;&lt;li&gt;umfassend &lt;strong&gt;Ehehindernisrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;klassische Regelungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber auch: Eheschließung zwischen &lt;strong&gt;Juden &lt;/strong&gt;und &lt;strong&gt;Staatsangehörigen&lt;/strong&gt; mit "&lt;strong&gt;deutschem&lt;/strong&gt;" oder "&lt;strong&gt;artverwandtem&lt;/strong&gt;" Blut &lt;strong&gt;verboten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie: &lt;strong&gt;zwischen &lt;/strong&gt;Personen mit &lt;strong&gt;ansteckenden Krankheiten&lt;/strong&gt;, &lt;strong&gt;entmündigten&lt;/strong&gt;, &lt;strong&gt;Geistes&lt;/strong&gt;- oder &lt;strong&gt;Erbkranken&lt;/strong&gt; &lt;strong&gt;verboten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Noch heute "&lt;strong&gt;entnazifiziert&lt;/strong&gt;" &lt;strong&gt;gültig &lt;/strong&gt;aber durch &lt;em&gt;große Familienrechtsreform&lt;/em&gt; der &lt;em&gt;1970er &lt;/em&gt;und &lt;em&gt;Eheänderungsgesetz&lt;/em&gt; &lt;em&gt;1999 &lt;/em&gt;abgeändert&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der &lt;strong&gt;Freiteil&lt;/strong&gt; (&lt;strong&gt;Sohnesquote&lt;/strong&gt;) bei der Testierfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;das &lt;strong&gt;ganze&lt;/strong&gt; &lt;strong&gt;MA &lt;/strong&gt;hindurch &lt;strong&gt;dominant&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Kirche verlangte&lt;/strong&gt; vom Erblasser eine &lt;strong&gt;Quote &lt;/strong&gt;des &lt;strong&gt;Nachlasses &lt;/strong&gt;-&amp;gt; &lt;em&gt;Freiteil&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gedacht als &lt;strong&gt;Umverteilung &lt;/strong&gt;für die &lt;strong&gt;Armen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Unter &lt;strong&gt;Kaiser Augustinus  &lt;/strong&gt;(&lt;em&gt;4./5. JH&lt;/em&gt;): &lt;strong&gt;Freiteilslehre&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine festgesetzte&lt;/strong&gt; Quote -&amp;gt; ein &lt;strong&gt;Sohnesteil &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei 2 Söhnen also 3 Teile -&amp;gt; 1 an Kirche &lt;/li&gt;&lt;li&gt;War im dt. Recht nur &lt;strong&gt;kirchl. Gebot&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber: &lt;strong&gt;Nichteinhaltung &lt;/strong&gt;von Kirche mit &lt;strong&gt;Sakraments&lt;/strong&gt;- und &lt;strong&gt;Begräbnisverweigerung &lt;/strong&gt;sanktioniert&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Entwicklung des Ehegatten&lt;strong&gt;erbrechts&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;heimisches Gewohnheitsrecht &lt;/em&gt;(&lt;strong&gt;älteres &lt;/strong&gt;Recht)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;kein Erbrecht&lt;/strong&gt; des Ehegatten, weil &lt;strong&gt;Eheschließung keine&lt;/strong&gt; &lt;strong&gt;Verwandtschaft &lt;/strong&gt;begründete&lt;/li&gt;&lt;li&gt;Wenn &lt;strong&gt;keine Verwandten&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Fiskus &lt;/strong&gt;erhält Erbgut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kein Bedürfnis &lt;/strong&gt;nach Ausgestaltung des &lt;strong&gt;Ehegattenerbrechts&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;MA&lt;/strong&gt; und &lt;strong&gt;frühe&lt;/strong&gt; &lt;strong&gt;Neuzeit&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Ehegüterrecht &lt;/em&gt;&lt;/strong&gt;für finanzielle Absicherung des Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ansätze &lt;/strong&gt;zur Ausgestaltung des &lt;strong&gt;Ehegattenerbr&lt;/strong&gt;.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ehegüterrechtl&lt;/strong&gt;. Ansprüche wurden mit &lt;strong&gt;Vorstellung von&lt;/strong&gt; &lt;strong&gt;Erbrecht&lt;/strong&gt; &lt;strong&gt;verbunden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;besonders im &lt;strong&gt;Bürger&lt;/strong&gt;- und &lt;strong&gt;Bauernstand&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Üblich: &lt;strong&gt;Ehegatte &lt;/strong&gt;erhält &lt;strong&gt;Hälfte&lt;/strong&gt; der &lt;strong&gt;Errungenschaft &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wichtige &lt;strong&gt;Motivation&lt;/strong&gt;: &lt;strong&gt;unversorgte Witwen &lt;/strong&gt;mangels ehegüterrechtlicher Vereinbarungen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Rezeption &lt;/strong&gt;des gemeinsamen &lt;strong&gt;Ehegattenerbrechts &lt;/strong&gt;im &lt;strong&gt;18 JH&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ehegatte erhielt &lt;strong&gt;Erbrecht nach&lt;/strong&gt; &lt;strong&gt;allen Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;falls ehegüterr&lt;/strong&gt;. &lt;strong&gt;Vereinbarung&lt;/strong&gt;: Ehegatte hat &lt;strong&gt;Wahl &lt;/strong&gt;ob &lt;strong&gt;Ehegüter oder Erbe &lt;/strong&gt;antreten.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sonderstellung unbemittelter &lt;/strong&gt;Gatte: wenn &lt;strong&gt;gänzlich&lt;/strong&gt; &lt;strong&gt;unversorgt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;1/4 des Nachlasses&lt;/strong&gt; (oder &lt;em&gt;Kindeskopfteil &lt;/em&gt;bei &lt;em&gt;vier+ Kindern&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Josephinisches &lt;/strong&gt;&lt;em&gt;Erbfolgepatent &lt;/em&gt;&lt;strong&gt;1786&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehegatte &lt;/strong&gt;wird Erbfolger, &lt;strong&gt;wenn kein&lt;/strong&gt; &lt;strong&gt;Verwandter &lt;/strong&gt;in&lt;strong&gt; 6 Parentelen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Zusätzlich &lt;strong&gt;Fruchtgenussrecht &lt;/strong&gt;an &lt;strong&gt;1/4 des Vermögens &lt;/strong&gt;(&lt;em&gt;endet mit erneuter Ehe&lt;/em&gt;).&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;basierend&lt;/strong&gt; auf &lt;strong&gt;Josephinischem&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fruchtgenuss &lt;/strong&gt;zu unbeschränktem&lt;strong&gt; Eigentum&lt;/strong&gt; &lt;strong&gt;erweitert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;Kind 1/4&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;anderen Erben&lt;/strong&gt; &lt;strong&gt;1/2 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne Verwandte &lt;/strong&gt;in &lt;strong&gt;1+2. Linie&lt;/strong&gt; und &lt;strong&gt;ohne Großeltern&lt;/strong&gt;: &lt;strong&gt;ganze &lt;/strong&gt;Verlassenschaft&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;kein Pflichtteil&lt;/strong&gt;, aber &lt;strong&gt;Vorausvermächtnis &lt;/strong&gt;(&lt;em&gt;bewegliche Sachen &lt;/em&gt;des Haushalts)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;heutiges Ehegattenerbrecht&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;entstand aus &lt;strong&gt;Familienrechtsreform&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anhebung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Erbteils&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilanspruch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erben müssen Ehegatten &lt;strong&gt;verbleib in Wohnung &lt;/strong&gt;ermöglichen (&lt;strong&gt;Schuldrechtl&lt;/strong&gt;. &lt;strong&gt;Anspruch &lt;/strong&gt;des Ehegatten gegen Erben)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehegatte erhält &lt;strong&gt;haushaltszugehörige Sachen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;gewohnte Umgebung&lt;/strong&gt; behalten&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Parentelensystem?&lt;/p&gt;&lt;p&gt;Was meint man mit &lt;strong&gt;formell&lt;/strong&gt;/&lt;strong&gt;materiell&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Parentelen&lt;/strong&gt;: sind &lt;strong&gt;Verwandte&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;nähere &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verwandte &lt;/span&gt;des &lt;strong&gt;Erblassers &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;schließen &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;weitere aus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;neuzeitliches &lt;/strong&gt;System geht auf Kaiser &lt;strong&gt;Joseph II&lt;/strong&gt; zurück&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Parentelensystem &lt;/strong&gt;ist Teil der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;gesetzlichen &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbfolge&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;also &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;subsidiär&lt;/strong&gt;, &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;wenn &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;keine letztwillige &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verfügung&lt;/span&gt;!&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;neben Parentelensystem, &lt;/strong&gt;ab &lt;em&gt;ABGB 1811&lt;/em&gt;: &lt;strong&gt;Ehegatte &lt;/strong&gt;steht &lt;strong&gt;gesetzliches&lt;/strong&gt; &lt;strong&gt;Vorausvermächtnis &lt;/strong&gt;zu (&lt;strong&gt;bewegliche Sachen &lt;/strong&gt;aus Haushalt, heute auch: Verbleib in &lt;strong&gt;ehelicher Wohnung&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;System Kaiser &lt;strong&gt;Josephs&lt;/strong&gt;: &lt;strong&gt;6 Parentelen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ABGB 1811&lt;/strong&gt;: Grenze bei &lt;strong&gt;4. Parentele&lt;/strong&gt;, d.h. in der &lt;strong&gt;vierten &lt;/strong&gt;Linie &lt;strong&gt;kein Repräsentationsrecht &lt;/strong&gt;der &lt;strong&gt;Nachkommen &lt;/strong&gt;mehr&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Parentelen:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1&lt;/strong&gt;. Parentele: &lt;strong&gt;Deszendenten &lt;/strong&gt;(Kinder) des Erblassers&lt;/li&gt;&lt;li&gt;&lt;strong&gt;2&lt;/strong&gt;. Parentele: &lt;strong&gt;Eltern &lt;/strong&gt;+ &lt;strong&gt;Nachkommen &lt;/strong&gt;(&lt;em&gt;Geschwister&lt;/em&gt;, &lt;em&gt;Nichten,&lt;/em&gt; &lt;em&gt;Neffen&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;3&lt;/strong&gt;. Parentele: &lt;strong&gt;Großeltern &lt;/strong&gt;+ &lt;strong&gt;Nachkommen&lt;/strong&gt; (&lt;em&gt;Tante&lt;/em&gt;, &lt;em&gt;Onkel&lt;/em&gt;, &lt;em&gt;Cousins&lt;/em&gt;, &lt;em&gt;Cousinen&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;4&lt;/strong&gt;. Parentele: nur &lt;strong&gt;Urgroßeltern &lt;/strong&gt;(keine Nachkommen!)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;formell&lt;/em&gt;: &lt;strong&gt;Eintrittsrecht&lt;/strong&gt;/&lt;strong&gt;Repräsentationsrecht &lt;/strong&gt;des Erben &lt;strong&gt;in&lt;/strong&gt; &lt;strong&gt;Erbfolge&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;materiell&lt;/em&gt;: &lt;strong&gt;zustehender Anteil &lt;/strong&gt;(&lt;em&gt;Viertel&lt;/em&gt;, &lt;em&gt;Drittel&lt;/em&gt;, ...) an der &lt;strong&gt;Erbmasse&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war Erbenlaub/Erbenlob?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zustimmung &lt;/strong&gt;des nächsten &lt;strong&gt;Erben &lt;/strong&gt;zu &lt;strong&gt;Rechtsgeschäften über Erbgut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;dinglich &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;wirkendes Wartrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erbgut&lt;/strong&gt;: hat man &lt;strong&gt;selbst vererbt &lt;/strong&gt;bekommen, wird &lt;strong&gt;familiär weitergegeben&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaufgut&lt;/strong&gt;: &lt;strong&gt;selbst erwirtschaftetes &lt;/strong&gt;Vermögen zur &lt;strong&gt;freien Verfügung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Reallasten, Rentenkauf?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Modernes Recht&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reallast: dinglich wirkende Belastung&lt;/strong&gt; eines &lt;strong&gt;Grundstücks&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;für &lt;strong&gt;bestimmte&lt;/strong&gt;, idR &lt;strong&gt;wiederkehrende&lt;/strong&gt; &lt;strong&gt;Leistungen &lt;/strong&gt;des &lt;strong&gt;Eigentümers&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;Leistungsverpflichtete &lt;/strong&gt;wird also über das &lt;strong&gt;Eigentum &lt;/strong&gt;am Grundstück &lt;strong&gt;bestimmt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wesentlich&lt;strong&gt;: sachliche Haftung&lt;/strong&gt; -&amp;gt; &lt;strong&gt;verdinglichte&lt;/strong&gt; &lt;strong&gt;Leistungspflicht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Haftung &lt;/strong&gt;auch &lt;strong&gt;persönlich &lt;/strong&gt;für fällig gewordenen &lt;strong&gt;Leistungen!&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Arten:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dienstleistungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgabe von &lt;strong&gt;Produkten&lt;/strong&gt; des &lt;strong&gt;Grundstücks&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geldrenten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Einschränkung&lt;/strong&gt;: &lt;strong&gt;Leistung &lt;/strong&gt;und &lt;strong&gt;wirtschaftliche Beschaffenheit &lt;/strong&gt;des &lt;strong&gt;GS &lt;/strong&gt;müssen &lt;strong&gt;zusammenhängen&lt;/strong&gt; (&lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;willkürlichen &lt;/strong&gt;Verpflichtungen)&lt;/li&gt;&lt;li&gt;In Ö: keine geschlossene gesetzliche Regelung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Älteres Recht: &lt;/em&gt;Viele&lt;/strong&gt; Arten der Reallasten&lt;/p&gt;&lt;p&gt;&lt;strong&gt;→ Obrigkeitliche&lt;/strong&gt; Reallasten:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;in Form von &lt;strong&gt;Grundzins&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eigentümliche Verknüpfung &lt;/strong&gt;von &lt;strong&gt;herrschaftlichen&lt;/strong&gt; und &lt;strong&gt;wirtschaftlichen&lt;/strong&gt; &lt;strong&gt;Abhängigkeitsverhältnissen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;→ privatrechtliche &lt;/strong&gt;Reallasten:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;seit &lt;strong&gt;hohem MA&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ältere &lt;/strong&gt;Reallast: &lt;strong&gt;wiederkehrende Abgaben&lt;/strong&gt; des &lt;strong&gt;Gewere&lt;/strong&gt;inhabers an &lt;strong&gt;Träger &lt;/strong&gt;geistlicher und weltlicher &lt;strong&gt;Hoheitsgewalt &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Neuere &lt;/strong&gt;Reallast:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;entsprach &lt;strong&gt;Kredit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;begründet durch &lt;strong&gt;dingliche Einigung&lt;/strong&gt; der Vertragspartner vor &lt;strong&gt;Gericht &lt;/strong&gt;+ &lt;strong&gt;Eintragung &lt;/strong&gt;in &lt;strong&gt;öffentliche Bücher&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rentenkäufer &lt;/strong&gt;bekommt &lt;strong&gt;Grundrente &lt;/strong&gt;aus &lt;strong&gt;Teil &lt;/strong&gt;des &lt;strong&gt;Ertragswertes&lt;/strong&gt; der Liegenschaft&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eigentümer (&lt;strong&gt;Reallastverpflichteter&lt;/strong&gt;) leistet &lt;strong&gt;Natural&lt;/strong&gt;-, &lt;strong&gt;Dienst&lt;/strong&gt;- oder &lt;strong&gt;Geldleistungen&lt;/strong&gt; an &lt;strong&gt;Rentenkäufer&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bei &lt;strong&gt;Nichterbringung&lt;/strong&gt;: &lt;strong&gt;Haftung &lt;/strong&gt;mit &lt;strong&gt;Grundstück&lt;/strong&gt;, aber &lt;strong&gt;nicht persönlich&lt;/strong&gt; oder mit übrigem &lt;strong&gt;Vermögen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;reine&lt;/strong&gt; &lt;strong&gt;Sachhaftung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Befriedigung &lt;/strong&gt;aus dem belasteten Grundstück&lt;/li&gt;&lt;li class="ql-indent-1"&gt;im &lt;strong&gt;Hochmittelalter&lt;/strong&gt;: &lt;strong&gt;eigenständige &lt;/strong&gt;Verpfändung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ausgehendes &lt;/strong&gt;Mittelalter: &lt;strong&gt;gerichtliche &lt;/strong&gt;Verpfändung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Güterstand ABGB 1811?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Gütertrennung&lt;/strong&gt; in der &lt;strong&gt;Ehe &lt;/strong&gt;-&amp;gt; jeder hatte sein &lt;strong&gt;eigenes Vermögen&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aber: &lt;strong&gt;Zweifelsregelungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sogn. "&lt;strong&gt;verschämte&lt;/strong&gt; &lt;strong&gt;Gütergemeinschaft&lt;/strong&gt;" bzw "&lt;strong&gt;vermutete Verwaltungsgemeinschaft&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Im&lt;/strong&gt; &lt;strong&gt;Zweifel &lt;/strong&gt;wird vermutet:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dass &lt;strong&gt;Erwerb vom&lt;/strong&gt; &lt;strong&gt;Mann &lt;/strong&gt;stammt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dass Frau &lt;strong&gt;bis auf&lt;/strong&gt; &lt;strong&gt;Widerruf &lt;/strong&gt;die &lt;strong&gt;Verwaltung &lt;/strong&gt;des &lt;strong&gt;Vermögens &lt;/strong&gt;dem &lt;strong&gt;Mann&lt;/strong&gt; anvertraut hat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mann haftet &lt;/strong&gt;als Verwalter des Frauenvermögens für &lt;strong&gt;Stammgut &lt;/strong&gt;und &lt;strong&gt;Kapital&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind ältere und jüngere Satzung? (Altes/Neues Pfandrecht)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ältere Satzung: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Hingabe &lt;/strong&gt;einer Liegenschaft in die &lt;strong&gt;leibliche Gewere des Gläubigers&lt;/strong&gt; zur &lt;strong&gt;Sicherung &lt;/strong&gt;oder vorläufigen &lt;strong&gt;Tilgung&lt;/strong&gt; einer &lt;strong&gt;Schuld&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Jüngere Satzung: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Liegenschaftspfand ohne Übertragung&lt;/strong&gt; der Sache &lt;strong&gt;in die leibliche Gewere des Gläubigers.&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eigentum &lt;/strong&gt;und &lt;strong&gt;leibliche Gewere &lt;/strong&gt;verbleiben &lt;strong&gt;beim Schuldner&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;erhält &lt;strong&gt;anwartschaftliche Gewere&lt;/strong&gt;, &lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;bei Nichtleistung &lt;/strong&gt;kann er sich aus dem &lt;strong&gt;Pfandgut befriedigen&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: lime;"&gt;Was ist die Muntehe oder auch Sittenvertragsehe?&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;im &lt;strong&gt;älteren Recht &lt;/strong&gt;die &lt;strong&gt;ausgeprägteste Form&lt;/strong&gt; &lt;strong&gt;der Ehe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;germanische Rechtsordnung &lt;/strong&gt;stark an der &lt;strong&gt;Sippe ausgerichtet &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; in älterer Zeit &lt;strong&gt;auch Ehe zwischen Sippen abgemacht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Willensbildung &lt;/strong&gt;der &lt;strong&gt;Frau kaum &lt;/strong&gt;vorhanden&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Muntgewalt?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gewalt des Hausvaters&lt;/strong&gt; über &lt;strong&gt;alle im Haus lebenden Personen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;gegliedert in &lt;strong&gt;Herrschafts&lt;/strong&gt;- und &lt;strong&gt;Schutzverhältnis&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dritten &lt;/strong&gt;gegenüber übernahm der Munt(walt) eine &lt;strong&gt;Schutzfunktion&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;im &lt;strong&gt;Innenverhältnis &lt;/strong&gt;stand der &lt;strong&gt;Herrschaftsaspekt &lt;/strong&gt;im Vordergrund. &lt;/li&gt;&lt;li&gt;Die Muntgewalt zerfiel ferner in die &lt;strong&gt;väterliche&lt;/strong&gt;, &lt;strong&gt;eheliche &lt;/strong&gt;und &lt;strong&gt;gesinderechtliche und/oder vormundschaftsrechtliche Munt&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Munt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leitungs- und Ordnungsmacht des Hausvaters&lt;/strong&gt; über alle &lt;strong&gt;im Haus lebenden Personen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Muntlinge &lt;/strong&gt;unterstanden der&lt;strong&gt; Herrschaft des Muntwalts&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;konnten nur &lt;strong&gt;über seine Vermittlung am Rechtsleben teilnehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;hatten also lediglich &lt;strong&gt;beschränkte Geschäftsfähigkeit&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Dritthandverfahren?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Teil der &lt;strong&gt;Anefangklage &lt;/strong&gt;(mittelalterlicher &lt;strong&gt;Rechtsbehelf &lt;/strong&gt;gegen eine &lt;strong&gt;abhandengekommene Sache &lt;/strong&gt;war)&lt;/li&gt;&lt;li&gt;Für die &lt;strong&gt;Klageerhebung &lt;/strong&gt;war das &lt;strong&gt;außergerichtliche Anfassen &lt;/strong&gt;der beweglichen Sache (&lt;strong&gt;Fahrnis&lt;/strong&gt;) zwingend &lt;strong&gt;erforderlich &lt;/strong&gt;(diese Handlung bezeichnete genau die Sache, die abhandengekommen war)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dadurch wurde &lt;strong&gt;klar&lt;/strong&gt;, dass die &lt;strong&gt;Sache dem Kläger abhandengekommen &lt;/strong&gt;ist.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;aktuelle Besitzer &lt;/strong&gt;musste zur &lt;strong&gt;Exkulpation &lt;/strong&gt;einen &lt;strong&gt;Dritten &lt;/strong&gt;bzw einen &lt;strong&gt;Vormann &lt;/strong&gt;öffentlich &lt;strong&gt;benennen&lt;/strong&gt;,&lt;/li&gt;&lt;li class="ql-indent-2"&gt;von dem sich seine &lt;strong&gt;rechtmäßige&lt;/strong&gt; &lt;strong&gt;Gewere ableitet&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Konnte &lt;/strong&gt;er das &lt;strong&gt;nicht&lt;/strong&gt;, war er als &lt;strong&gt;Dieb &lt;/strong&gt;überführt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Deshalb &lt;/strong&gt;heißt das Verfahren auch &lt;strong&gt;Dritthandverfahren&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was bedeutet „Hand wahre Hand“?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;War die Sache bereits in die &lt;strong&gt;Hand eines Dritten gelangt&lt;/strong&gt;, so galt das mittelalterliche &lt;strong&gt;Rechtssprichwort &lt;/strong&gt;„&lt;em&gt;Wo du deinen Glauben gelassen hast, dort sollst du ihn auch suchen&lt;/em&gt;“ oder „&lt;em&gt;Hand wahre Hand&lt;/em&gt;“. &lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;Eigentümer einer beweglichen &lt;/strong&gt;Sache, der diese einem &lt;strong&gt;anderen anvertraut &lt;/strong&gt;hat, kann diese &lt;strong&gt;nur von diesem&lt;/strong&gt;, nicht von einem Dritten &lt;strong&gt;herausverlangen&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;basierend auf &lt;strong&gt;Publizitätsgedanken &lt;/strong&gt;des &lt;strong&gt;Fahrnisrecht&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;der &lt;strong&gt;Dritte kennt&lt;/strong&gt; den &lt;strong&gt;Besitz &lt;/strong&gt;(&lt;em&gt;leibliche Gewere&lt;/em&gt;) des Entlehners,&lt;strong&gt; aber nicht den Rechtsmangel&lt;/strong&gt; des Vertrauensmannes&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Heute: &lt;strong&gt;gutgläubiger Erwerb vom Nichtberechtigten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche 8 Liegenschaftsgewere werden unterschieden? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Unmittelbare Gewere (leiheberechtigter Bauer)&lt;/li&gt;&lt;li&gt;Mittelbare Gewere (Grundherr)&lt;/li&gt;&lt;li&gt;Eigengewere (Umfassendes Herrschaftsrecht)&lt;/li&gt;&lt;li&gt;Beschränktes Gewere (Gewere zur rechten Vormundschaft)&lt;/li&gt;&lt;li&gt;Leibliche Gewere (körperliche Gewere)&lt;/li&gt;&lt;li&gt;Ideelle Gewere (besitzlose Gewere im Liegenschaftsrecht)&lt;/li&gt;&lt;li&gt;Ruhende Gewere (Pfandschuldner)&lt;/li&gt;&lt;li&gt;Anwartschaftliche Gewere (Schenkung auf den Todesfall)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind Fahrnisgewere?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gewere an &lt;strong&gt;beweglicher Sache &lt;/strong&gt;(Fahrnis) untrennbar &lt;strong&gt;an&lt;/strong&gt; &lt;strong&gt;körperliche Innehabung gebunden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erworben &lt;/strong&gt;durch &lt;strong&gt;Ergreifen &lt;/strong&gt;oder &lt;strong&gt;Übergabe von Hand zu Hand&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geht mit &lt;strong&gt;Verlust &lt;/strong&gt;der &lt;strong&gt;körperlichen Herrschaft verloren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Recht der &lt;strong&gt;Fahrnisverfolgung im älteren Recht&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Strenge &lt;strong&gt;Unterscheidung &lt;/strong&gt;zwischen &lt;strong&gt;freiwilliger&lt;/strong&gt; &lt;strong&gt;Besitzaufgabe&lt;/strong&gt; (&lt;em&gt;Hand wahre Hand&lt;/em&gt;) und &lt;strong&gt;unfreiwilligem Besitzverlust &lt;/strong&gt;(&lt;em&gt;Anefangsklage, Dritthandverfahren&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Liegenschaftsgewere?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Fahrnisgewere &lt;/strong&gt;nur auf Fälle &lt;strong&gt;unmittelbarer Sachherrschaft &lt;/strong&gt;beschränkt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Liegenschaftsgewere &lt;/strong&gt;auch für &lt;strong&gt;mittelbare &lt;/strong&gt;Nutzung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sachherrschaft über Liegenschaften eine von zwei Formen: Nutzen oder Brauchen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind ideelle Gewere?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Gewere &lt;/strong&gt;war ein Zentralinstitut des &lt;strong&gt;mittelalterlichen deutschen Rechts&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ein &lt;strong&gt;sachenrechtlicher Vorgang &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;definiert &lt;strong&gt;Verhältnis &lt;/strong&gt;einer &lt;strong&gt;Person &lt;/strong&gt;zu einer &lt;strong&gt;Sache &lt;/strong&gt;oder einem &lt;strong&gt;Amt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Träger &lt;/strong&gt;kann &lt;strong&gt;rechtswidrige Zugriffe &lt;/strong&gt;auf die Sache &lt;strong&gt;abwehren&lt;/strong&gt;, und nach &lt;strong&gt;Wegnahme herausverlangen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Im Kern: &lt;strong&gt;Keine&lt;/strong&gt; &lt;strong&gt;Differenzierung &lt;/strong&gt;zwischen &lt;strong&gt;Besitz&lt;/strong&gt; und &lt;strong&gt;Eigentum&lt;/strong&gt;, sondern es &lt;strong&gt;ging um die Verfügungsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ideelle &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bestanden an&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;rechtswidrig entzogenem Gut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;rechtmäßigem Erbteil&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sind &lt;strong&gt;besitzlose Gewere &lt;/strong&gt;im &lt;strong&gt;Liegenschaftsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Unterscheidung zwischen &lt;strong&gt;Fahrnis&lt;/strong&gt;- und &lt;strong&gt;Liegenschaftsgewere&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch wenn die Grundstücksnutzung zur &lt;strong&gt;Gänze entzogen &lt;/strong&gt;wurde, &lt;strong&gt;bleibt die ideelle Gewere&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anfänge &lt;/strong&gt;der &lt;strong&gt;staatl&lt;/strong&gt;. &lt;strong&gt;Ehegesetzgebung&lt;/strong&gt; schon unter &lt;strong&gt;Maria Theresia&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einschränkung &lt;/strong&gt;der &lt;strong&gt;kirchlichen Macht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;rechtl&lt;/strong&gt;. &lt;strong&gt;Wirkung &lt;/strong&gt;der Ehe &lt;strong&gt;fixiert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Grundlegender &lt;strong&gt;Wandel &lt;/strong&gt;unter&lt;strong&gt; Joseph II: Ehepatent 1783&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Trennung&lt;/strong&gt; zwischen &lt;strong&gt;Ehesakramenten&lt;/strong&gt; und &lt;strong&gt;Ehevertrag &lt;/strong&gt;("&lt;em&gt;Zurückeroberung der legitimen Rechte&lt;/em&gt;")&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;fomelle Derogation &lt;/strong&gt;der &lt;em&gt;kirchl&lt;/em&gt;. &lt;em&gt;Ehegesetzedurch&lt;/em&gt; Vorlage eines &lt;strong&gt;bürgerlichen&lt;/strong&gt; &lt;strong&gt;Ehevertrags &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; d.h. &lt;strong&gt;kirchliche &lt;/strong&gt;Ehegesetzgebung &lt;strong&gt;unter bürgerlichen Ehevertrag &lt;/strong&gt;geordnet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bewirkte &lt;strong&gt;keine Umwandlung &lt;/strong&gt;in &lt;strong&gt;obligatorische Zivilehe&lt;/strong&gt;, &lt;strong&gt;geistliche &lt;/strong&gt;verstanden sich bei der &lt;strong&gt;Trauung &lt;/strong&gt;aber &lt;strong&gt;mehr &lt;/strong&gt;als &lt;strong&gt;Staatsdiener&lt;/strong&gt;, &lt;strong&gt;denn &lt;/strong&gt;als &lt;strong&gt;Religionsdiener&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit&lt;/strong&gt; bei &lt;strong&gt;staatlichen Gerichtshöfen &lt;/strong&gt;(&lt;em&gt;Staat DiözesenGH&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehefähigkeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Minderjährige benötigten &lt;/strong&gt;zur Eheschließung &lt;strong&gt;Einwilligung &lt;/strong&gt;von &lt;strong&gt;Vater &lt;/strong&gt;(oder falls dieser Tot: &lt;strong&gt;Großvater väterlicherseits&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehen &lt;strong&gt;ohne Einwilligung&lt;/strong&gt;: "&lt;em&gt;völlig ungültig&lt;/em&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wurde Einwilligung&lt;strong&gt; ohne erhebliche Gründe verweigert &lt;/strong&gt;-&amp;gt; v&lt;strong&gt;on Amts wegen Einwilligung &lt;/strong&gt;bekommen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Eintrittsrecht?&lt;/p&gt;&lt;p&gt;Was bedeutet &lt;strong&gt;formell&lt;/strong&gt;/&lt;strong&gt;materiell &lt;/strong&gt;hier? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;das &lt;strong&gt;Recht zu Erben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;kann&lt;strong&gt; innerhalb der ersten 3 Parentelen&lt;/strong&gt; der dem toten &lt;strong&gt;Gradnächste nicht erben &lt;/strong&gt;(&lt;em&gt;tot &lt;/em&gt;oder &lt;em&gt;erbunwürdig&lt;/em&gt;) -&amp;gt; Erbschaft geht an &lt;strong&gt;Nachkommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dieser &lt;strong&gt;Nachkomme repräsentiert&lt;/strong&gt; den &lt;strong&gt;Gradnächsten&lt;/strong&gt; -&amp;gt; &lt;em&gt;Repräsentionsrecht&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;formell vs materiell Repräsentationsrecht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erbt &lt;/strong&gt;der Eintrittsberechtigte aufgrund seines &lt;strong&gt;eigenen Rechts&lt;/strong&gt;, oder übt er das &lt;strong&gt;Erbrecht des Repräsentierten &lt;/strong&gt;aus?&lt;/li&gt;&lt;li&gt;&lt;strong&gt;formell&lt;/strong&gt;: &lt;strong&gt;eigenes&lt;/strong&gt; Recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur &lt;strong&gt;Anteil &lt;/strong&gt;wird von der repräsentierten Person &lt;strong&gt;abgeleitet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbausschluss&lt;/strong&gt; des &lt;strong&gt;Repräsentierten &lt;/strong&gt;ist &lt;strong&gt;unerheblich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;materiel&lt;/strong&gt;: Recht des &lt;strong&gt;Erbberechtigten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Recht &lt;/strong&gt;auf &lt;strong&gt;Erbe &lt;/strong&gt;von repräsentierter Person &lt;strong&gt;abgeleitet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;fehlende Erbberechtigung &lt;/strong&gt;(&lt;em&gt;Erbunfähigkeit&lt;/em&gt;- oder &lt;em&gt;Verzicht&lt;/em&gt;) des Repräsentierten -&amp;gt; Repräsentant kann auch &lt;strong&gt;nicht erben&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Erbenhaftung? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;Älteres Recht/Älteste Zeit&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;keine vererbbaren&lt;/strong&gt; &lt;strong&gt;Schulden &lt;/strong&gt;-&amp;gt; Schuld &lt;strong&gt;strafrechtlich persönlich &lt;/strong&gt;auf &lt;strong&gt;Schuldner &lt;/strong&gt;bezogen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sippenhaftung &lt;/strong&gt;-&amp;gt; &lt;strong&gt;nicht erblich&lt;/strong&gt;, sondern &lt;strong&gt;Gefahrengemeinschaft&lt;/strong&gt; aller &lt;strong&gt;Sippengenossen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Deliktsschulden unvererblich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vertragsschulden&lt;/strong&gt;: &lt;strong&gt;beschränkte &lt;/strong&gt;Erbenhaftung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbe &lt;strong&gt;haftet nur&lt;/strong&gt;, wenn &lt;strong&gt;Vertragspartner &lt;/strong&gt;des Erblassers &lt;strong&gt;schon geleistet &lt;/strong&gt;hat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbe haftet mit &lt;strong&gt;Fahrnissen&lt;/strong&gt;, aber &lt;strong&gt;nicht mit Liegenschaften &lt;/strong&gt;des &lt;strong&gt;Nachlasses&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;SpMA&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erbe haftet für &lt;strong&gt;alle Schulden &lt;/strong&gt;des Erblassers, &lt;strong&gt;außer höchstpersönliche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sachhaftung &lt;/strong&gt;-&amp;gt; "&lt;strong&gt;Nachlass&lt;/strong&gt;" &lt;strong&gt;haftet &lt;/strong&gt;für Schulde, &lt;strong&gt;nicht &lt;/strong&gt;der &lt;strong&gt;Erbe &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Neuzeitliche Entwicklung&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;durch &lt;strong&gt;Rezeption&lt;/strong&gt;: &lt;strong&gt;unbeschränkte &lt;/strong&gt;Erbenhaftung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wegen &lt;strong&gt;röm. rechtlicher&lt;/strong&gt; Ansicht, dass &lt;strong&gt;Erblasser &lt;/strong&gt;und &lt;strong&gt;Erbe gleich &lt;/strong&gt;zu behandeln sind&lt;/li&gt;&lt;li&gt;Erbe konnte im &lt;strong&gt;gemeinen Recht &lt;/strong&gt;aber &lt;strong&gt;Liste &lt;/strong&gt;aller &lt;strong&gt;Erbschaftsgegenstände &lt;/strong&gt;erstellen -&amp;gt; dadurch &lt;strong&gt;Sachhaftung &lt;/strong&gt;erwirken&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;klärt &lt;strong&gt;beschränkte Erbenhaftung nicht genau&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Auslegung&lt;/strong&gt;: Erben haften &lt;strong&gt;nur &lt;/strong&gt;mit &lt;strong&gt;Nachlassaktiva&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Heute&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;umfanglich beschränkte &lt;/strong&gt;Erbenhaftung &lt;strong&gt;üblich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Da mit &lt;strong&gt;Eintreten&lt;/strong&gt; in Erbe &lt;strong&gt;Zugriff &lt;/strong&gt;der &lt;strong&gt;Gläubiger&lt;/strong&gt; auf &lt;strong&gt;Nachlassvermögen verhindert &lt;/strong&gt;wird&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nachlassseparation &lt;/strong&gt;auf &lt;strong&gt;Antrag &lt;/strong&gt;der &lt;strong&gt;Gläubiger&lt;/strong&gt; führt zu &lt;strong&gt;Sachhaftung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Real/Formal/Konsensual/Arrhalverträge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur &lt;strong&gt;Formal&lt;/strong&gt;- und &lt;strong&gt;Realverträge &lt;/strong&gt;(+ Sonderform &lt;strong&gt;Arrhalvertrag&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Formalvertrag&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wichtig: &lt;strong&gt;Hör- und Sichtbarkeit&lt;/strong&gt; von Abgabe und Annahme des &lt;strong&gt;Versprechens&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Daher b&lt;strong&gt;estimmte Gesten/ritualisierte Formeln &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Begründen &lt;strong&gt;Schuld&lt;/strong&gt;- und &lt;strong&gt;Haftungsverhältnisse&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Realvertrag&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Austauschgeschäfte&lt;/strong&gt; waren in ältester Zeit Bar (&lt;strong&gt;Zug-um-Zug&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit &lt;strong&gt;Kreditkauf&lt;/strong&gt; kam &lt;strong&gt;auseinanderfallen &lt;/strong&gt;der &lt;strong&gt;Leistungszeitpunkte&lt;/strong&gt; und damit &lt;strong&gt;Haftungsprobleme&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Lösung: &lt;strong&gt;Vertrag&lt;/strong&gt; &lt;strong&gt;nicht &lt;/strong&gt;mit &lt;strong&gt;Willensübereinkunft&lt;/strong&gt;, &lt;strong&gt;sondern &lt;/strong&gt;mit &lt;strong&gt;Leistung&lt;/strong&gt; &lt;strong&gt;abgeschlossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verpflichtete&lt;/strong&gt; nur den &lt;strong&gt;Annehmer &lt;/strong&gt;-&amp;gt; Der &lt;strong&gt;Geber &lt;/strong&gt;hat mit Leistung schon &lt;strong&gt;Schuld erfüllt &lt;/strong&gt;(&lt;strong&gt;&lt;em&gt;Kauf, Tausch&lt;/em&gt;&lt;/strong&gt;, ...)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Arrhalvertrag&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wie Realvertrag, jedoch&lt;strong&gt; nur Anzahlung statt voller Leistung&lt;/strong&gt; -&amp;gt; &lt;em&gt;Arrha&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anfangs relevanter Teil &lt;/strong&gt;der Leistung, &lt;strong&gt;später symbolisch&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;röm&lt;/strong&gt;. &lt;strong&gt;rechtlicher&lt;/strong&gt; &lt;strong&gt;Einfluss&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Konsensualverträge&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Kauf&lt;/em&gt;&lt;/strong&gt;, &lt;em&gt;Miete &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;entstehen durch &lt;strong&gt;übereinstimmende Willenserklärungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;kanonischer Einfluss&lt;/strong&gt;: &lt;strong&gt;Formfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Formvorgaben waren die Ausnahme&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;hauptsächlich Konsensualverträge&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;wenige Realverträge&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;allgemein &lt;strong&gt;Formfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Formvorschriften &lt;/strong&gt;bei &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Bürgschaft&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Schenkungsversprechen&lt;/em&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Ratengeschäften&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Ehepakten &lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Vermögenswirkung der Ehe/Das Ehegüterrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehegüterrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Zwei Ausprägungen&lt;strong&gt;: &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;reine Gütertrennung &lt;/strong&gt;(&lt;em&gt;keine eherechtlichen Folgen&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;umfassende Gütergemeinschaft &lt;/strong&gt;(gesamtes &lt;strong&gt;Vermögen &lt;/strong&gt;wird zur &lt;strong&gt;Einheit&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mischformen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Primäre &lt;strong&gt;Aufgabe&lt;/strong&gt;: &lt;strong&gt;Versorgung &lt;/strong&gt;des &lt;strong&gt;Überlebenden &lt;/strong&gt;und &lt;strong&gt;Aufteilung&lt;/strong&gt; der &lt;strong&gt;finanziellen Lasten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Entwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Älteres Recht: &lt;/em&gt;Vermögenstrennung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Karte&lt;/li&gt;&lt;li&gt;&lt;em&gt;Mittelalter: &lt;/em&gt;Mischformen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Karte "Güterstand im Mittelalter"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeit (Rezeption)&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;prinzipiell&lt;/strong&gt; &lt;strong&gt;Gütertrennung &lt;/strong&gt;wie MA&lt;/li&gt;&lt;li&gt;aber &lt;strong&gt;Vielzahl vertraglicher Gütergemeinschaftstypen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gütertrennung &lt;/strong&gt;(außer &lt;strong&gt;vertragliche &lt;/strong&gt;Vereinbarung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zweifelsregelungen &lt;/strong&gt;zugunsten des &lt;strong&gt;Mannes&lt;/strong&gt;! &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gütertrennung &lt;/strong&gt;- außer &lt;strong&gt;vertragliche &lt;/strong&gt;Vereinbarung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Eherecht im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundsätze &lt;/strong&gt;von Josephinischen &lt;strong&gt;Ehepatent&lt;/strong&gt; &lt;strong&gt;1783 übernommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber: &lt;strong&gt;dreifach gegliedertes &lt;/strong&gt;Eherecht für &lt;strong&gt;Protestanten&lt;/strong&gt;, &lt;strong&gt;Juden&lt;/strong&gt;, &lt;strong&gt;Katholiken&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Katholiken&lt;/strong&gt; konnten sich &lt;strong&gt;nicht Scheiden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Güterstand: &lt;strong&gt;Gütertrennung &lt;/strong&gt;(außer Vertragl.) &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mann&lt;/strong&gt; zwingend &lt;strong&gt;Haupt &lt;/strong&gt;der Familie&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehefrau&lt;/strong&gt; hat &lt;strong&gt;Unterhaltsanspruch&lt;/strong&gt; und &lt;strong&gt;Folgepflichten &lt;/strong&gt;ggü. Mann&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Arten der Ehe gab es im Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;Muntehe&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;auch &lt;strong&gt;Sippenvertragsehe &lt;/strong&gt;oder &lt;strong&gt;Kaufehe &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;häufigste Form &lt;/strong&gt;der Ehe im &lt;strong&gt;älteren Recht&lt;/strong&gt;, &lt;strong&gt;gemeinsam &lt;/strong&gt;mit &lt;strong&gt;Konsensehe einzige &lt;/strong&gt;von der &lt;strong&gt;Kirche&lt;/strong&gt; &lt;strong&gt;anerkannte &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vertrag&lt;/strong&gt; zwischen &lt;strong&gt;Bräutigam &lt;/strong&gt;und &lt;strong&gt;Muntwalt&lt;/strong&gt; &lt;strong&gt;der Braut&lt;/strong&gt;, oft Mitwirkung der Verwandten&lt;/li&gt;&lt;li&gt;Geschlossen mit &lt;strong&gt;Eheschließung &lt;/strong&gt;+ &lt;strong&gt;Hochzeitsnacht &lt;/strong&gt;(Vollziehung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;alleinige &lt;strong&gt;Verfügungsgewalt &lt;/strong&gt;über &lt;strong&gt;Vermögen&lt;/strong&gt;, &lt;strong&gt;Frau &lt;/strong&gt;und &lt;strong&gt;Kinder&lt;/strong&gt;, sowie &lt;em&gt;alleiniges&lt;/em&gt; &lt;em&gt;Scheidungsrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Mann&lt;strong&gt; &lt;/strong&gt;muss &lt;strong&gt;Frau schützen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Friedelehe&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mann hatte &lt;strong&gt;keine Muntgewalt &lt;/strong&gt;über Frau&lt;/li&gt;&lt;li&gt;Geschlossen durch &lt;strong&gt;Willensübereinkunft Mann+Frau &lt;/strong&gt;+ &lt;strong&gt;Hochzeitsnacht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Üblich wenn:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbtocher &lt;/strong&gt;Mann mit &lt;strong&gt;niedrigerem&lt;/strong&gt; &lt;strong&gt;Stand heiratete&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Adeliger Zweitehe &lt;/strong&gt;eingeht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weil: Person &lt;strong&gt;niedrigeren Standes rückt nicht &lt;/strong&gt;in höheren auf, und &lt;strong&gt;kein Erbrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;In Neuzeit "&lt;strong&gt;morganatische Ehe&lt;/strong&gt;" genannt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Kebsehe&lt;/em&gt; &lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Eheähnliches &lt;/strong&gt;Verhältnis&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unfreie Frau &lt;/strong&gt;von &lt;strong&gt;freiem Mann &lt;/strong&gt;dazu &lt;strong&gt;gezwungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Mann konnte &lt;strong&gt;mehrere Kebsehen &lt;/strong&gt;haben&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kinder&lt;/strong&gt;, ungeachtet der Stellung des Vaters als &lt;strong&gt;Leibeigene &lt;/strong&gt;geboren&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Raubehe/Entführungsehe&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Unterschied: Bei &lt;strong&gt;Raubehe Braut nicht Einverstanden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erlaubnis &lt;/strong&gt;des &lt;strong&gt;Muntwalt nicht &lt;/strong&gt;eingeholt -&amp;gt; ist ein &lt;strong&gt;Verbrechen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Braut&lt;/strong&gt; muss &lt;strong&gt;zurückgegeben &lt;/strong&gt;werden, &lt;strong&gt;Bräutigam &lt;/strong&gt;zahlt &lt;strong&gt;Buße&lt;/strong&gt; an &lt;strong&gt;Vormund&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ohne Anfehdung &lt;/strong&gt;von Brautfamilie blieb sie &lt;strong&gt;bestehen&lt;/strong&gt;. &lt;strong&gt;Gültig &lt;/strong&gt;aber erst mit &lt;strong&gt;Eheschließung &lt;/strong&gt;-&amp;gt; &lt;strong&gt;meist Friedelehe&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Konsensehe&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;kanonistischer Begriff&lt;/strong&gt;, beschreibt in erster Linie, dass ehe durch &lt;strong&gt;gegenseitige Willenserklärung vor Zeugen zustande &lt;/strong&gt;kommt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nicht &lt;/strong&gt;durch &lt;strong&gt;priesterlichen&lt;/strong&gt; &lt;strong&gt;Segen&lt;/strong&gt;, &lt;strong&gt;oder&lt;/strong&gt; &lt;strong&gt;Beischlaf&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Also: &lt;strong&gt;Unterscheidung&lt;/strong&gt; zwischen&lt;strong&gt; röm-kath. &lt;/strong&gt;Auffassung und &lt;strong&gt;alt/ostkirchlichen&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;röm&lt;/em&gt;-&lt;em&gt;kath&lt;/em&gt;: &lt;strong&gt;Priester &lt;/strong&gt;ist zwar einer der&lt;strong&gt; &lt;/strong&gt;Zeugen, aber &lt;strong&gt;Eheleute&lt;/strong&gt; &lt;strong&gt;stiften &lt;/strong&gt;Ehe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ostkirchlich&lt;/em&gt;: &lt;strong&gt;Priester stiftet &lt;/strong&gt;ehe.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;altrömisch&lt;/strong&gt;/altkirchlich: &lt;strong&gt;Ehe &lt;/strong&gt;gilt mit &lt;strong&gt;Beischlaf&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Konsensehe&lt;/strong&gt;: &lt;strong&gt;Beischlaf festigt &lt;/strong&gt;ehe nur&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gültig auch ohne &lt;/strong&gt;Beischlaf&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kann aber &lt;strong&gt;unter &lt;/strong&gt;bestimmten &lt;strong&gt;Voraussetzungen gelöst &lt;/strong&gt;werden&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Geschichte der Stellung der &lt;strong&gt;ehelichen &lt;/strong&gt;Kinder?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;keine Unterschiede &lt;/strong&gt;zwischen &lt;strong&gt;ehelich &lt;/strong&gt;und &lt;strong&gt;unehelich &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es zählte &lt;strong&gt;Aufnahme &lt;/strong&gt;in &lt;strong&gt;Hausgemeinschaft &lt;/strong&gt;durch &lt;strong&gt;Muntwalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Stellung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein Schutz&lt;/strong&gt; im Hauswesen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Züchtigungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;väterliche &lt;strong&gt;Munt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kinder folgten &lt;strong&gt;Stamm &lt;/strong&gt;von &lt;strong&gt;schlechter &lt;/strong&gt;gestelltem &lt;strong&gt;Elternteil&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Frühe Neuzeit&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vernachlässigung &lt;/strong&gt;durch Eltern wurde &lt;strong&gt;bestraft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;erste Ansätze von &lt;strong&gt;Jugendschutzgesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eheliche Kinder &lt;/strong&gt;erhielten &lt;strong&gt;Namen&lt;/strong&gt;, &lt;strong&gt;Familie &lt;/strong&gt;und &lt;strong&gt;Stand &lt;/strong&gt;des &lt;strong&gt;Vaters&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Vater war &lt;strong&gt;gesetzlicher Vormund&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Väterliche&lt;/strong&gt; &lt;strong&gt;Unterhaltspflicht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Josephinische Gesetzbuch&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erste Bestimmungen für &lt;strong&gt;Unterhaltspflicht &lt;/strong&gt;der &lt;strong&gt;Mutter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Vater durfte &lt;strong&gt;keinen Nutzen&lt;/strong&gt; aus &lt;strong&gt;Kindesvermögen &lt;/strong&gt;ziehen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erziehungsgewalt &lt;/strong&gt;des Vaters genau &lt;strong&gt;geregelt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Wohl &lt;/strong&gt;des Kindes&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vater Unterhalt&lt;/strong&gt;, &lt;em&gt;Mutter Pflege&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kindesvermögen&lt;/strong&gt; weiterhin &lt;strong&gt;nicht nutzen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater vertritt&lt;/strong&gt; Kind im &lt;strong&gt;Rechtsverkehr&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gemeinsame Rechte, aber &lt;strong&gt;letzte Entscheidung&lt;/strong&gt; bei &lt;strong&gt;Vater&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vertretung &lt;/strong&gt;des Kindes durch &lt;strong&gt;beide&lt;/strong&gt; &lt;strong&gt;Eltern &lt;/strong&gt;möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übertragung auf &lt;strong&gt;Großeltern möglich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kinderrechtsnovelle 1989 &lt;em&gt;verbietet körperliche Gewalt&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Geschichte der Stellung der &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;&lt;em&gt;un&lt;/em&gt;ehelichen &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Kinder?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;bis &lt;strong&gt;13 Jhd gleich wie eheliche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Christlicher Einfluss&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aberkennung Erbrecht &lt;/strong&gt;gegen &lt;strong&gt;Vater &lt;/strong&gt;(&lt;strong&gt;nicht verwandt&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ausschluss &lt;/strong&gt;von &lt;strong&gt;best&lt;/strong&gt;. &lt;strong&gt;Berufen &lt;/strong&gt;und von &lt;strong&gt;allen Zünften&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;keine kirchlichen &lt;/strong&gt;Ämter&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Rezeption &lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Unterscheidung &lt;/strong&gt;zwischen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;natürlichen &lt;/strong&gt;Kindern (&lt;strong&gt;Eltern &lt;/strong&gt;konnten &lt;strong&gt;heiraten&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehebruchskindern &lt;/strong&gt;(&lt;strong&gt;Zugehörigkeit &lt;/strong&gt;zu &lt;strong&gt;mütterlicher &lt;/strong&gt;Familie &lt;strong&gt;verwehrt&lt;/strong&gt;) &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Josephinische Gesetzgebung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleichstellung &lt;/strong&gt;uneheliche und eheliche Kinder&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehebruchskinder Unterhaltsanspruch beschränkt&lt;/strong&gt; und &lt;strong&gt;keine verwandschaftlichen &lt;/strong&gt;Rechte zu &lt;strong&gt;Mutter &lt;/strong&gt;und &lt;strong&gt;Vater&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;uneheliche nur mit Mutter verwandt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Milderung&lt;/strong&gt; mit Novelle &lt;strong&gt;1914&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;uneheliche gleiche &lt;/strong&gt;Rechte&lt;strong&gt; ggü Mutter &lt;/strong&gt;wie eheliche &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Alimenteanspruch &lt;/strong&gt;und &lt;strong&gt;Recht &lt;/strong&gt;auf &lt;strong&gt;pers&lt;/strong&gt;. &lt;strong&gt;Verkehr &lt;/strong&gt;mit &lt;strong&gt;Vater&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;weitgehende &lt;strong&gt;Angleichung ehelich&lt;/strong&gt;/&lt;strong&gt;unehelich &lt;/strong&gt;mit &lt;strong&gt;Familienrechtsreform 1970er&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Benachteiligung &lt;/strong&gt;im &lt;strong&gt;Erbrecht&lt;/strong&gt; &lt;strong&gt;beseitigt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Unterschied im &lt;strong&gt;Namensrecht&lt;/strong&gt;: &lt;em&gt;Name der Mutter&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Stellung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bestmögliches Kindeswohl&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eltern gleiche Rechte &lt;/strong&gt;und &lt;strong&gt;Pflichten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pflicht&lt;/strong&gt; zu &lt;strong&gt;Unterhalt &lt;/strong&gt;und &lt;strong&gt;Obsorge &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Leibzucht/Leibgedinge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eingerichtet &lt;strong&gt;wegen Vermögenstrennung &lt;/strong&gt;in der Ehe&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehegatte &lt;/strong&gt;erhielt &lt;strong&gt;nach Tod&lt;/strong&gt; von Partner &lt;strong&gt;Nutzungsrecht auf Lebenszeit &lt;/strong&gt;an &lt;strong&gt;einem &lt;/strong&gt;oder &lt;strong&gt;mehreren Objekten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesicherte Rechtsstellung &lt;/strong&gt;- &lt;strong&gt;Leibgedingeurkunde &lt;/strong&gt;konnte nur mit &lt;strong&gt;Zustimmung&lt;/strong&gt; &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;Berechtigten aufgehoben &lt;/strong&gt;werden&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der gewohnheitsrechtliche Beisitz der Witwe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ältestes Institut der &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Witwe &lt;/strong&gt;und &lt;strong&gt;Kinder&lt;/strong&gt; setzten&lt;strong&gt; Haus- und Vermögensgemeinschaft fort&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Witwe kann dadurch &lt;strong&gt;Kindesvermögen&lt;/strong&gt; &lt;strong&gt;verwalten &lt;/strong&gt;und &lt;strong&gt;nutzen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Beisitz &lt;strong&gt;endete &lt;/strong&gt;mit &lt;strong&gt;Wiederverheiratung&lt;/strong&gt; oder &lt;strong&gt;Ausscheiden &lt;/strong&gt;der Kinder aus der &lt;strong&gt;Hausgemeinschaft &lt;/strong&gt;(&lt;strong&gt;Abschichtung&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Möglichkeiten der letztwilligen Verfügung gab es im MA neben dem Testament?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Fränkische Affatomie/langobradische Thinx&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Wenn &lt;strong&gt;Erblasser keine&lt;/strong&gt; &lt;strong&gt;Erben &lt;/strong&gt;hatte, konnte er mit &lt;strong&gt;Zustimmung&lt;/strong&gt; &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;Kaisers&lt;/strong&gt; sein &lt;strong&gt;Gut jemand "Fremden" vermachen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Erbverbrüderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Um das &lt;strong&gt;Aussterben regierender&lt;/strong&gt; &lt;strong&gt;Häuser &lt;/strong&gt;zu &lt;strong&gt;vermeiden&lt;/strong&gt;, schloss man mit anderen Häusern sog. &lt;strong&gt;Hausverträge&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Häuser beerben sich bei aussterben gegenseitig&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verindert Lehensrückfall&lt;/strong&gt; zu Kaiser&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erlaubt &lt;strong&gt;einfachen Gebietsgewinn&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Benötigte &lt;strong&gt;Zustimmung&lt;/strong&gt; &lt;strong&gt;des Kaisers&lt;/strong&gt;, &lt;strong&gt;wenn&lt;/strong&gt; &lt;strong&gt;Lehensgut &lt;/strong&gt;betroffen war&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ehegemächt&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;sachenrechtliche Übertragung &lt;/strong&gt;des &lt;strong&gt;gesamten&lt;/strong&gt; &lt;strong&gt;Ehevermögens&lt;/strong&gt; des einen Gatten &lt;strong&gt;an den anderen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Einkindschaftsvertrag&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;erbrechtliche Gleichstellung&lt;/strong&gt; von &lt;strong&gt;Stiefgeschwistern&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das SC Vallejanum? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schließt Frauen &lt;/strong&gt;von &lt;strong&gt;Sicherstellung fremder Verbindlichkeiten &lt;/strong&gt;(&lt;em&gt;Bürgschaft&lt;/em&gt;, &lt;em&gt;Verpfändung&lt;/em&gt;, ... ) &lt;strong&gt;aus&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;In viele &lt;strong&gt;neuzeitliche Land&lt;/strong&gt;- und &lt;strong&gt;Stadtrechtsordnungen&lt;/strong&gt; aufgenommen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Entwicklung des Grundbuches?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ab &lt;/em&gt;&lt;strong&gt;&lt;em&gt;12 Jhdt&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schreinwesen&lt;/strong&gt;: Grundstücksgeschäfte in Städten auf &lt;strong&gt;Pergament &lt;/strong&gt;in Schreinen aufgehängt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ab &lt;/em&gt;&lt;strong&gt;&lt;em&gt;13 Jhdt&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Stadtbücher&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;zuerst kein Beweiswert&lt;/strong&gt;, dann 2 Varianten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Realfolien&lt;/strong&gt;: Eintragung nach &lt;strong&gt;Grundstück&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Personalfolien&lt;/strong&gt;: Eintragung nach &lt;strong&gt;Eigentümer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ab 13/14 Jhdt&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Landtafeln&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;für &lt;em&gt;adelige Liegenschaften&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eintragungszwang &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; keine &lt;strong&gt;dinglichen Rechte &lt;/strong&gt;ohne Eintragung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundbuch &lt;/strong&gt;im &lt;strong&gt;engeren Sinn: &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;für &lt;em&gt;bäuerliche Grundstücke&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundherr musste &lt;strong&gt;Grund &lt;/strong&gt;+ &lt;strong&gt;Pflichten &lt;/strong&gt;der &lt;strong&gt;Grunduntertanen &lt;/strong&gt;verzeichnen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;verwies auf &lt;strong&gt;Landtafeln &lt;/strong&gt;und &lt;strong&gt;Grundbücher&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Allg&lt;/em&gt;. &lt;strong&gt;&lt;em&gt;Grundbuchgesetz 1871&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;alle Liegenschaften &lt;/strong&gt;mussten &lt;strong&gt;verzeichnet &lt;/strong&gt;werden&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Teil &lt;strong&gt;ABGB&lt;/strong&gt;, Teil &lt;strong&gt;Sondergesetze &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie war das Grundbuch gegliedert?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;bis &lt;/em&gt;&lt;strong&gt;&lt;em&gt;18 Jhdt&lt;/em&gt;&lt;/strong&gt;&lt;em&gt;:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dreibuchsystem&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grundbuch&lt;/strong&gt;: &lt;strong&gt;Bezeichnung &lt;/strong&gt;von Gut&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gewerebuch&lt;/strong&gt;: Urkunden für &lt;strong&gt;Eigentum&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Satzbuch&lt;/strong&gt;: dingliche &lt;strong&gt;Belastungen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Änderungen im 18 Jhdt:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1. Buch&lt;/strong&gt; wurde &lt;strong&gt;Hauptbuch&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dreiteilung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Bezeichnung &lt;/strong&gt;Liegenschaft&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Eigentümer&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Eintragung der &lt;strong&gt;Lasten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;2&lt;strong&gt; &lt;/strong&gt;Urkundenbücher&lt;strong&gt;: Belegsammlungen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Prinzipien des Grundbuchrechts?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;em&gt;Intabulationsprinzip&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;ab&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;18. JH&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dingliche Rechte nur durch&lt;/strong&gt; &lt;strong&gt;Eintragung &lt;/strong&gt;im Grundbuch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bücherl. Vormann&lt;/strong&gt; -&amp;gt; Recht des Vormannes muss eingetragen werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eintragung benötigt &lt;strong&gt;gültigen Titel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Vertrauensgrundsatz&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gutgläubiger Erwerber &lt;/strong&gt;darf auf Grundbuch &lt;strong&gt;vertrauen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nicht&lt;/strong&gt; &lt;strong&gt;eingetragene RG &lt;/strong&gt;haben &lt;strong&gt;keine Wirkung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;: Nur für nachträgliche außerbücherliche Rechtsänderungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Später&lt;/em&gt;: auch für anfangs fehlerhafte Eintragungen&lt;/li&gt;&lt;li&gt;&lt;em&gt;Prioritätsprinzip&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;zeitlich &lt;/strong&gt;frühere Antrag geht &lt;strong&gt;vor dem späteren -&amp;gt; &lt;/strong&gt;maßgebend&lt;strong&gt;: &lt;/strong&gt;Zeitpunkt des &lt;strong&gt;Gesuchseingangs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Im &lt;em&gt;GrundbuchG 1871&lt;/em&gt;: Zeitpunkt der &lt;strong&gt;Eintragung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Spezialitätsprinzip&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bürgerliche Rechte &lt;/strong&gt;nur an &lt;strong&gt;bestimmten Grundbuchskörpern&lt;/strong&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Dispensehe bzw. Severehe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ab &lt;strong&gt;1919 &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Katholiken &lt;/strong&gt;konnten trotz &lt;strong&gt;bestehender Ehe &lt;/strong&gt;auf &lt;strong&gt;staatlichem&lt;/strong&gt; &lt;strong&gt;Weg &lt;/strong&gt;(&lt;em&gt;wieder&lt;/em&gt;) &lt;strong&gt;Heiraten &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ansuchen beim &lt;strong&gt;Landeshauptmann &lt;/strong&gt;um &lt;strong&gt;Dispens &lt;/strong&gt;(&lt;strong&gt;Befreiung &lt;/strong&gt;von geltenden &lt;strong&gt;Vorschriften&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Solange &lt;strong&gt;gültig bis&lt;/strong&gt; vom &lt;strong&gt;Gericht &lt;/strong&gt;für &lt;strong&gt;ungültig &lt;/strong&gt;erklärt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Rechtsbrauch des Dreißigsten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nach &lt;strong&gt;Tod &lt;/strong&gt;von &lt;strong&gt;Familienoberhaupt &lt;/strong&gt;mussten alle &lt;strong&gt;Hausgenossen&lt;/strong&gt; &lt;strong&gt;30 Tage &lt;/strong&gt;wie bisher &lt;strong&gt;versorgt &lt;/strong&gt;werden&lt;/li&gt;&lt;li&gt;der &lt;strong&gt;Tote lebte rechtlich 30 Tage &lt;/strong&gt;weiter und &lt;strong&gt;behielt&lt;/strong&gt; &lt;strong&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;erst &lt;strong&gt;danach Erbe aufgeteilt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Nasciturus iVm Rechtsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;Mittelalter&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei &lt;strong&gt;Erbanspruch &lt;/strong&gt;wurde &lt;strong&gt;Erbverteilung &lt;/strong&gt;bei &lt;strong&gt;Tode des Vaters bis &lt;/strong&gt;zur &lt;strong&gt;Geburt &lt;/strong&gt;des Kindes &lt;strong&gt;aufgeschoben&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Rezeption &lt;/em&gt;&lt;/strong&gt;(&lt;strong&gt;neuzeitliche &lt;/strong&gt;Rechtsentwicklung)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Beginn der &lt;strong&gt;Rechtsfähigkeit&lt;/strong&gt; &lt;strong&gt;mit Geburt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aber: Wenn es um &lt;strong&gt;Rechte &lt;/strong&gt;geht, ab &lt;strong&gt;Zeugung -&amp;gt; Nasciturus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;ausgehend von &lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;bedingte&lt;/strong&gt; und &lt;strong&gt;beschränkte&lt;/strong&gt; &lt;strong&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;unter &lt;strong&gt;Voraussetzung&lt;/strong&gt; einer &lt;strong&gt;Lebendgeburt &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;ausschließlich&lt;/strong&gt; zum &lt;strong&gt;Vorteil &lt;/strong&gt;des Nasciturus&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren verzigene und unverzigene Töchter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Rezeption &lt;/strong&gt;(&lt;strong&gt;neuzeitliche &lt;/strong&gt;Rechtsentwicklung)&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Verzigene&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei &lt;strong&gt;Heirat &lt;/strong&gt;mussten &lt;strong&gt;Töchter&lt;/strong&gt; auf &lt;strong&gt;väterliches Erbe Verzichten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;als &lt;strong&gt;Entschädigung: Heiratsgut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verblieb &lt;/strong&gt;der Verzicht, wurde &lt;strong&gt;so getan als gäbe &lt;/strong&gt;es ihn&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Unverzigene&lt;/strong&gt; &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vater und Brüder konnten Erbverzicht erlassen&lt;/li&gt;&lt;li&gt;Dann waren Töchter neben Brüdern zur Erbschaft zugelassen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war &lt;em&gt;Usus modernus pandectarum&lt;/em&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ziel: &lt;strong&gt;röm-kan. Recht allgemein Anwendbar&lt;/strong&gt; machen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ohne Errungenschaften heimischer Rechtskultur &lt;/strong&gt;zu &lt;strong&gt;verlieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Stände im Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;MA Gesellschaft nach Ständen &lt;/strong&gt;geordnet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Personengruppen &lt;/strong&gt;mit &lt;strong&gt;eigenen&lt;/strong&gt; &lt;strong&gt;Verhaltensnormen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Beseitigung &lt;strong&gt;extremer Unterschiede&lt;/strong&gt;: &lt;strong&gt;18 JH&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Anpassung &lt;strong&gt;Ungleichheiten&lt;/strong&gt;: &lt;strong&gt;19 JH&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufhebung&lt;/strong&gt;: &lt;strong&gt;20 JH&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Dreiständelehre:&lt;/em&gt;&lt;strong&gt;&lt;em&gt; &lt;/em&gt;Adel, Klerus, Bauern&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mit Urbanisierung&lt;strong&gt;&lt;em&gt; 4. Stand: &lt;/em&gt;Bürger&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Adel&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sonderstellungen &lt;/strong&gt;im öffentlichen und bürgerlichen Recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Privatfürstenrecht&lt;/strong&gt;: &lt;strong&gt;Haus &lt;/strong&gt;und &lt;strong&gt;Famlienangelegenheiten verbindend regeln&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Bürgerstand&lt;/em&gt;&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;strong&gt;Stadtluft macht Frei&lt;/strong&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grundlage&lt;/strong&gt; für das Zusammenleben bildete &lt;strong&gt;jeweilige Stadtverfassung&lt;/strong&gt; bzw. &lt;strong&gt;Stadtrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Bauern&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;starke Einschränkung &lt;/strong&gt;der &lt;strong&gt;Rechtsfähigkeiten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Karte zu Abhängigkeiten der Bauern&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Prinzip der Ebenbürtigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bestimmte &lt;strong&gt;Rechtsbeziehungen nur &lt;/strong&gt;zwischen &lt;strong&gt;Standesgenossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;v.a. &lt;strong&gt;Eherecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber auch &lt;strong&gt;Vertrags&lt;/strong&gt;- und &lt;strong&gt;Erbrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ungenossen&lt;/strong&gt; waren von &lt;strong&gt;Rechtsgemeinschaft &lt;/strong&gt;eines Standes &lt;strong&gt;ausgeschlossen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Heimfallsrecht? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;bei &lt;strong&gt;erblosem Nachlass&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Heimfall&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;keine &lt;/strong&gt;zur &lt;strong&gt;Erbfolge berechtigte &lt;/strong&gt;Personen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;oder &lt;strong&gt;erbberechtigte Personen &lt;/strong&gt;Erbschaft &lt;strong&gt;nicht antreten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Viele &lt;strong&gt;Heimfallberechtigte &lt;/strong&gt;Subjekte: &lt;strong&gt;Sippe&lt;/strong&gt;, &lt;strong&gt;Gemeinde&lt;/strong&gt;, &lt;strong&gt;Kirche&lt;/strong&gt;, &lt;strong&gt;König&lt;/strong&gt;, &lt;strong&gt;Staat &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber auch Universität, Gefängnisse, Spitäler, ...&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Besonders &lt;/strong&gt;wichtig: &lt;strong&gt;&lt;em&gt;König&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Oft &lt;strong&gt;gegen entfernte Verwandte &lt;/strong&gt;oder &lt;strong&gt;Ehegatten &lt;/strong&gt;durchgesetzt mit Begründung: &lt;strong&gt;Gemeinschaftsinteressen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Auch &lt;strong&gt;Regelungen &lt;/strong&gt;für &lt;strong&gt;Heimfall nur bei bestimmten Erblassern &lt;/strong&gt;(&lt;em&gt;Hingerichtete&lt;/em&gt;, &lt;em&gt;Sträflinge&lt;/em&gt;, ... )&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ältere &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Ansicht: &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Heimfallsrecht &lt;/strong&gt;als &lt;strong&gt;Aneignung herrenloser&lt;/strong&gt; &lt;strong&gt;Sachen &lt;/strong&gt;durch &lt;strong&gt;Fiskus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Jüngere &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Ansicht:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Staat &lt;/strong&gt;als &lt;strong&gt;Universalsukzessor &lt;/strong&gt;(&lt;strong&gt;haftet &lt;/strong&gt;für &lt;strong&gt;Schulden&lt;/strong&gt;!)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Berechtigte&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zunächst &lt;strong&gt;König &lt;/strong&gt;oder &lt;strong&gt;Landesherr&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch Ansprüche von &lt;strong&gt;Städten &lt;/strong&gt;und &lt;strong&gt;Grundherren&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;später und &lt;strong&gt;heute&lt;/strong&gt;: &lt;strong&gt;Staat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Gewährleistung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einstehenmüssen &lt;/strong&gt;des Schuldners für &lt;strong&gt;Sach/Rechtsmängel &lt;/strong&gt;der Leistung&lt;strong&gt; im Zeitpunkt des Erbringens&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;va bei &lt;strong&gt;entgeltlichen Rechtsgeschäften&lt;/strong&gt; &lt;strong&gt;gesetzlich angeordnet&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verschuldensunabhängig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;müssen &lt;strong&gt;innerhalb bestimmter Frist &lt;/strong&gt;durch &lt;strong&gt;Klage &lt;/strong&gt;oder &lt;strong&gt;Einrede &lt;/strong&gt;zur Geltung gebracht werden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Rechtsfolgen&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Verbesserung&lt;/em&gt;&lt;/strong&gt;/&lt;em&gt;Austausch&lt;/em&gt;, &lt;em&gt;Preisminderung&lt;/em&gt;/&lt;em&gt;Wandlung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Fallrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Hatte der &lt;strong&gt;Erblasser&lt;/strong&gt; &lt;strong&gt;keine Nachkommen&lt;/strong&gt;, fielen &lt;strong&gt;Liegenschaften&lt;/strong&gt; in &lt;strong&gt;Manneslinie &lt;/strong&gt;zurück &lt;/li&gt;&lt;li&gt;Liegenschaften der &lt;strong&gt;weiblichen Linie &lt;/strong&gt;fielen erst an &lt;strong&gt;Manneslinie&lt;/strong&gt;, &lt;strong&gt;wenn &lt;/strong&gt;es &lt;strong&gt;gar keine Erben&lt;/strong&gt; gab.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Entwicklung der Sachmangelhaftung? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;älteres Recht &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;keine Gewährleistung &lt;/strong&gt;für Sachmängel, Käufer muss &lt;strong&gt;Sache selbst prüfen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ausgenommen: &lt;strong&gt;Hauptmängel &lt;/strong&gt;(&lt;strong&gt;Gravierend &lt;/strong&gt;oder &lt;strong&gt;arglistig&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;im &lt;em&gt;dt.&lt;/em&gt; Recht: &lt;strong&gt;Viehkauf&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;Dort Beweisumkehr&lt;/em&gt;: Verkäufer &lt;/strong&gt;musste &lt;strong&gt;beweisen&lt;/strong&gt;, dass &lt;strong&gt;Vieh gesund &lt;/strong&gt;ist&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;fehlen &lt;/strong&gt;einer &lt;strong&gt;zugesicherten Eigenschaft&lt;/strong&gt;: &lt;em&gt;actio empti&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Naturrecht &lt;/em&gt;(&lt;strong&gt;ab 18 JH&lt;/strong&gt;)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Äquivalenzprinzip &lt;/strong&gt;-&amp;gt; &lt;strong&gt;umfassendes&lt;/strong&gt; &lt;strong&gt;System&lt;/strong&gt; der &lt;strong&gt;Sachmängel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gleichgewicht &lt;/strong&gt;zwischen den Werten von &lt;strong&gt;Leistung&lt;/strong&gt; und &lt;strong&gt;Gegenleistung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;ABGB&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gewährleistung &lt;/strong&gt;wurde &lt;strong&gt;allgemeines&lt;/strong&gt; &lt;strong&gt;Prinzip &lt;/strong&gt;im Vertragsrecht&lt;/li&gt;&lt;li&gt;&lt;em&gt;Rechtsbehelfe&lt;/em&gt;: &lt;strong&gt;Preisminderung&lt;/strong&gt;, &lt;strong&gt;Wandlung&lt;/strong&gt;, &lt;strong&gt;Verbesserung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur bei &lt;strong&gt;Arglist Klage&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Entwicklung der Rechtsmangelhaftung?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verkäufer bringt Käufer&lt;strong&gt; nicht in die abgemachte rechtliche Position &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;röm Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verschaffung &lt;strong&gt;ungestörten Besitzes&lt;/strong&gt; mit &lt;strong&gt;Ersitzungsmöglichkeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verkäufer &lt;/strong&gt;musste &lt;strong&gt;in Prozess eintreten&lt;/strong&gt;, wenn &lt;strong&gt;Käufer &lt;/strong&gt;von Dritten &lt;strong&gt;geklagt &lt;/strong&gt;wird&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Acht&lt;/strong&gt;/&lt;strong&gt;Friedlosigkeit &lt;/strong&gt;wenn er &lt;strong&gt;nicht aufscheint&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;ABGB&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Muss &lt;strong&gt;Eigentum&lt;/strong&gt; &lt;strong&gt;verschaffen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wurden Todeserklärungen gehandhabt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Verschollenheit: &lt;/em&gt;Rechtsnachfolge &lt;/strong&gt;des vermutlich Toten mit &lt;strong&gt;Verschweigung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erben &lt;/strong&gt;bekamen Vermögen in t&lt;strong&gt;reuhänderisches Gewere&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Wandlung&lt;/strong&gt; in Eigentum mit Todesbeweis&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;oberitalisch&lt;/em&gt;: &lt;strong&gt;100&lt;/strong&gt;. LJ&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;sächsische &lt;/em&gt;Praxis: &lt;strong&gt;70&lt;/strong&gt;. LJ&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;schlesisches &lt;/em&gt;System: &lt;strong&gt;reduziert Alter &lt;/strong&gt;und &lt;strong&gt;kombiniert &lt;/strong&gt;mit &lt;strong&gt;Dauer&lt;/strong&gt; der &lt;strong&gt;Verschollenheit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;verwendet &lt;strong&gt;schlesisches&lt;/strong&gt; &lt;strong&gt;System&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;führt &lt;strong&gt;Todeserklärungsverfahren &lt;/strong&gt;ein&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beweis früheren&lt;/strong&gt; oder &lt;strong&gt;späteren Sterbedatums &lt;/strong&gt;möglich&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Todeserklärungsgesetz 1950&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;&lt;p&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Wann &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;gab es &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Schritte&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; der Entwicklung der Rechtsfähigkeit?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Fähigkeit Träger &lt;/strong&gt;von &lt;strong&gt;Rechten &lt;/strong&gt;und &lt;strong&gt;Pflichten &lt;/strong&gt;zu sein&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Rezeption&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;NS Zeit&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Rechtsfähigkeit im MA?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;Beginn&lt;/em&gt;&lt;/strong&gt;: &lt;strong&gt;Aufnahme &lt;/strong&gt;in &lt;strong&gt;Sippe &lt;/strong&gt;durch &lt;strong&gt;Vater&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Davor&lt;/strong&gt; &lt;strong&gt;Aussetzung &lt;/strong&gt;möglich&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Lebensfähig&lt;/strong&gt;, wenn es &lt;strong&gt;schaut &lt;/strong&gt;und &lt;strong&gt;schreit &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Stände&lt;/em&gt;&lt;/strong&gt;: &lt;strong&gt;Personen mit unterschiedlichen Rechten und Pflichten&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Frauen&lt;/em&gt;&lt;/strong&gt;: &lt;strong&gt;Muntgewalt unterworfen&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;im &lt;strong&gt;SMA &lt;em&gt;Beschränkungen gelockert&lt;/em&gt;&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vermögen &lt;/strong&gt;selbst &lt;strong&gt;verfügen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;über &lt;strong&gt;Ehegut verfügen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nach &lt;strong&gt;Tod &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;geht &lt;strong&gt;Muntgewalt an Frau&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kauffrau&lt;/strong&gt;: Berechtigt &lt;strong&gt;wie Mann&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Andersgläubige&lt;/em&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ketzer&lt;/strong&gt; &lt;strong&gt;keine &lt;/strong&gt;Rechte&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Andersgläubige eingeschränkt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende&lt;/em&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;nicht automatisch &lt;/strong&gt;durch &lt;strong&gt;Tod&lt;/strong&gt;: Rechtsbrauch des &lt;strong&gt;Dreißigsten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verschollenheit&lt;/strong&gt;: Bis Tod sicher, &lt;strong&gt;Erben &lt;/strong&gt;&lt;em&gt;nur &lt;/em&gt;&lt;strong&gt;&lt;em&gt;treuhändisches &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Gewere&lt;/em&gt;&lt;strong&gt; (Verschweigung)&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Klosterbeitritt &lt;/strong&gt;-&amp;gt; "&lt;strong&gt;Klostertod&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;Für &lt;strong&gt;bestimmte&lt;/strong&gt; &lt;strong&gt;Verbrechen&lt;/strong&gt;: &lt;strong&gt;Friedlosigkeit&lt;/strong&gt;/&lt;strong&gt;Acht&lt;/strong&gt; oder &lt;strong&gt;Reichsacht &lt;/strong&gt;(durch &lt;em&gt;König&lt;/em&gt;/&lt;em&gt;Kaiser&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Rechtsfähigkeit in der Rezeption?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Beginn&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;bei &lt;strong&gt;freien &lt;/strong&gt;Menschen &lt;strong&gt;ab Geburt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nasciturus&lt;/strong&gt;:&lt;em&gt; Rechte ab Zeugung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Frauen&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückschritt &lt;/strong&gt;vom &lt;strong&gt;SMA&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;strong&gt;&lt;em&gt;natürliche Minderbegabung&lt;/em&gt;&lt;/strong&gt;" und "&lt;em&gt;Schutzbedürftigkeit&lt;/em&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geschlechtervormundschaft &lt;/strong&gt;lebte wieder auf&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Rechtliche Institutionen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rechtsbrauch des Dreißigsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wurde in &lt;strong&gt;erbrechtliches Institut umgewandelt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Reichsacht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wurde zum &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;bürgerlichen Tod&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;völlige &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zerstörung &lt;/strong&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kein &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Vermögen&lt;/strong&gt;, keine &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ehe&lt;/strong&gt;, keine &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Vormundschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mit &lt;strong&gt;Tod&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;bei &lt;strong&gt;Verschollenheit &lt;/strong&gt;entweder:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ab &lt;strong&gt;100 &lt;/strong&gt;LJ oder &lt;strong&gt;70 &lt;/strong&gt;LJ&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;schlesisches &lt;/strong&gt;System: rechnet &lt;strong&gt;Alter und Dauer &lt;/strong&gt;auf&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Rechtsfähigkeit im ABGB 1811?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Beginn&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;ab &lt;strong&gt;Geburt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nachweis &lt;/strong&gt;der &lt;strong&gt;Lebensfähigkeit nicht notwendig&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Nasciturus&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;beschränkt &lt;/strong&gt;und &lt;strong&gt;bedingt &lt;/strong&gt;rechtsfähig -&amp;gt; &lt;strong&gt;nur Rechte&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Frauen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;formales Bekenntnis &lt;/strong&gt;zur &lt;strong&gt;Gleichbehandlung &lt;/strong&gt;von &lt;strong&gt;Mann &lt;/strong&gt;und &lt;strong&gt;Frau &lt;/strong&gt;bei &lt;strong&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei &lt;strong&gt;Verschollenheit&lt;/strong&gt;: &lt;strong&gt;schlesisches System&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;neu: förmliches &lt;strong&gt;Todeserklärungsverfahren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;auf Antrag&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Rechtsfähigkeit in der NS Zeit?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;allgemeine &lt;/strong&gt;Rechtsfähigkeit &lt;strong&gt;abgelehnt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nürnberger Gesetze&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;RF &lt;/strong&gt;hängte von &lt;strong&gt;Rassenzugehörigkeit &lt;/strong&gt;und &lt;strong&gt;völkischer&lt;/strong&gt; &lt;strong&gt;Gemeinschaft &lt;/strong&gt;ab&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Frauen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;massive &lt;strong&gt;Verschlechterungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aberkennung passives Wahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbot &lt;/strong&gt;mancher &lt;strong&gt;Berufe&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsfähigkeit im modernen Recht?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Angeborene und erworbene Rechte&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;angeboren&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grundrechte &lt;/strong&gt;und &lt;strong&gt;Persönlichkeitsrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;erworben&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eigentumserwerb&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Weitere &lt;/strong&gt;durch &lt;strong&gt;Alter&lt;/strong&gt;, &lt;strong&gt;Ausbildung&lt;/strong&gt;, &lt;strong&gt;Staatsbürgerschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Beginn&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;mit &lt;strong&gt;Geburt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Lebensfähigkeit keine Voraussetzung &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Gleichheitsgedanke&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;große &lt;strong&gt;Familienrechtsreform 1970&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;bei &lt;strong&gt;Eherecht&lt;/strong&gt;, &lt;strong&gt;Scheidungsrecht&lt;/strong&gt;, ...&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Tod&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Todeserklärungsgesetz &lt;/strong&gt;1950 &lt;/li&gt;&lt;li class="ql-indent-1"&gt;für &lt;strong&gt;Todeserklärungen &lt;/strong&gt;und &lt;strong&gt;Todesbeweis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verschollenheit&lt;/strong&gt;: Verfahren auf &lt;strong&gt;Antrag&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Anefangsklage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Auch bei &lt;strong&gt;Diebstahl ging die Gewere über&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Daher &lt;strong&gt;besondere&lt;/strong&gt; &lt;strong&gt;Deliktsklage &lt;/strong&gt;des &lt;strong&gt;Eigentümers gegen &lt;/strong&gt;jeden dritten &lt;strong&gt;Besitzer&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Fahrnisklage&lt;/em&gt;&lt;/strong&gt;/&lt;em&gt;Anefangsklage&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Ziel: &lt;strong&gt;Herausgabe &lt;/strong&gt;der Sache und &lt;strong&gt;Bestrafung &lt;/strong&gt;des Diebs&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ablauf&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Beklagter Besitzer &lt;/strong&gt;muss &lt;strong&gt;rechtmäßigen&lt;/strong&gt; &lt;strong&gt;Erwerb ausweisen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Dazu &lt;strong&gt;gibt&lt;/strong&gt; er die &lt;strong&gt;Sache &lt;/strong&gt;seinem &lt;strong&gt;Vormann&lt;/strong&gt;, und &lt;strong&gt;scheidet aus&lt;/strong&gt; &lt;strong&gt;Prozess &lt;/strong&gt;aus (&lt;em&gt;Dritthandverfahren&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dies &lt;strong&gt;wiederholt &lt;/strong&gt;sich &lt;strong&gt;bis&lt;/strong&gt; der &lt;strong&gt;Dieb&lt;/strong&gt; &lt;strong&gt;gefunden &lt;/strong&gt;ist&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Derjenige bei dem die &lt;strong&gt;Sache &lt;/strong&gt;bei der Weitergabe &lt;strong&gt;stehen&lt;/strong&gt; &lt;strong&gt;bleibt &lt;/strong&gt;muss sie an den Kläger &lt;strong&gt;herausgeben&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Folge&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Herausgabe &lt;/strong&gt;und &lt;strong&gt;Diebstahlbuße&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aber: konnte sich von &lt;strong&gt;strafrechtlicher&lt;/strong&gt; &lt;strong&gt;Verantwortung&lt;/strong&gt; &lt;strong&gt;befreien&lt;/strong&gt; mit &lt;strong&gt;Nachweis &lt;/strong&gt;von Kauf&lt;/li&gt;&lt;li class="ql-indent-1"&gt;am &lt;strong&gt;öffentlichen Markt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;von &lt;strong&gt;seriösem Vertrauensmann&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;von &lt;strong&gt;Übersee&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Entwicklung der gewillkürten Erbfolge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;zuerst &lt;/strong&gt;nur &lt;strong&gt;geborene &lt;/strong&gt;Erben&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Testament&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;anfangs&lt;/strong&gt; durch &lt;strong&gt;Kirche &lt;/strong&gt;(kanonisches Testament)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eingeschränkte Testierfreiheit &lt;/strong&gt;(&lt;em&gt;Zustimmung &lt;/em&gt;von &lt;strong&gt;&lt;em&gt;Ehefrau&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;und &lt;strong&gt;&lt;em&gt;Kindern&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sammlung von &lt;strong&gt;Legaten &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Testamentsvollstrecker&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Oft &lt;strong&gt;Unwiderruflichkeitsklauseln&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erst &lt;/strong&gt;im &lt;strong&gt;SMA &lt;/strong&gt;rein &lt;strong&gt;einseitiger &lt;/strong&gt;Vertrag&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Rezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Testierfreiheit &lt;/strong&gt;mit &lt;strong&gt;Altersgrenze &lt;/strong&gt;(F &lt;strong&gt;18&lt;/strong&gt;, M &lt;strong&gt;20&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Arten&lt;em&gt;: Testament&lt;/em&gt;, &lt;em&gt;Kodizill &lt;/em&gt;und &lt;em&gt;Erbvertrag &lt;/em&gt;bekannt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Intestaterbfolge &lt;/strong&gt;(= gesetzl. ) nur &lt;strong&gt;wenn kein Testament&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Möglichkeit der &lt;strong&gt;Enterbung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong&gt;Erbfolgeakte außergerichtlich &lt;/strong&gt;(Eröffnung des Testaments, Antreten der Erbschaft, Ergreifung des Nachlassbesitzes)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;gewillkürte&lt;/strong&gt; und &lt;strong&gt;gesetzl&lt;/strong&gt;. Erbfolge &lt;strong&gt;nicht &lt;/strong&gt;mehr gegenseitig &lt;strong&gt;ausgeschlossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reihenfolge: &lt;strong&gt;Erbvertrag&lt;/strong&gt;,&lt;strong&gt; Testament&lt;/strong&gt;, dann &lt;strong&gt;subsidiär gesetzl &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Arten: &lt;strong&gt;Testament&lt;/strong&gt;, &lt;strong&gt;Kodizill&lt;/strong&gt;, &lt;strong&gt;Erbvertrag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbvertrag &lt;/strong&gt;muss &lt;strong&gt;1/4&lt;/strong&gt; für Testament/Intestat &lt;strong&gt;frei &lt;/strong&gt;lassen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;kein Pflichtteilsrecht&lt;/strong&gt; für &lt;strong&gt;Geschwister&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber&lt;strong&gt; für Aszendenten &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong&gt;Erbfolgeakte&lt;/strong&gt; nun &lt;strong&gt;gerichtlich&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Testierfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Arten: &lt;strong&gt;Testament&lt;/strong&gt;, &lt;strong&gt;Kodizill&lt;/strong&gt;, &lt;strong&gt;Erbvertrag&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pflichtteile &lt;/strong&gt;für &lt;strong&gt;Nachkommen &lt;/strong&gt;(&lt;em&gt;1/2&lt;/em&gt;) und &lt;strong&gt;Vorfahren &lt;/strong&gt;(&lt;em&gt;1/3&lt;/em&gt;) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;halbiert &lt;/strong&gt;wenn &lt;strong&gt;kein Naheverhältnis &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Unterschiede zwischen Testament, Kodizill, Legat und Erbvertrag?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Testament&lt;/em&gt;: &lt;strong&gt;Einseitige letztwillige &lt;/strong&gt;Verfügung mit &lt;strong&gt;Erbeinsetzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbe erhält &lt;strong&gt;ganzen Nachlass &lt;/strong&gt;oder &lt;strong&gt;quotenmäßig bestimmten &lt;/strong&gt;Teil&lt;/li&gt;&lt;li&gt;&lt;em&gt;Kodizill&lt;/em&gt;: &lt;strong&gt;Einseitige letztwillige &lt;/strong&gt;Verfügung &lt;strong&gt;ohne Erbeinsetzung&lt;/strong&gt;, aber mit &lt;strong&gt;&lt;em&gt;anderen&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;&lt;strong&gt;&lt;em&gt;Verfügungen&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Bestellung eines &lt;strong&gt;Vormundes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Legat&lt;/em&gt;: Einseitige &lt;strong&gt;letztwillige Verfügung ohne Erbeinsetzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Jemand erhält nur &lt;strong&gt;bestimmte&lt;/strong&gt; &lt;strong&gt;Dinge&lt;/strong&gt; &lt;/li&gt;&lt;li&gt;&lt;em&gt;Erbvertrag&lt;/em&gt;: &lt;strong&gt;zweiseitig verbindlich &lt;/strong&gt;zwischen &lt;strong&gt;Ehegatten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Entwicklung der gesetzl. Erbfolge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;zuerst &lt;strong&gt;Spezialsukzession &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Zerfall &lt;/strong&gt;in verschiedene &lt;strong&gt;Vermögensmassen &lt;/strong&gt;mit &lt;strong&gt;spezifischen Erbfolgeordnungen &lt;/strong&gt;(Aussteuer, Anwachsung, Anfall, ... )&lt;/li&gt;&lt;li&gt;dann entwickelt sich &lt;strong&gt;Parentelerbfolge &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;jüngere Generation bevorzugt:&lt;/em&gt; "Das Gut rinnt wie das Blut"&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Einschränkungen&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Fallrecht &lt;/strong&gt;für Liegenschaften im Mannesstamm&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbberechtigt &lt;/strong&gt;nur die &lt;strong&gt;Seite &lt;/strong&gt;von der das &lt;strong&gt;Erbe stammt &lt;/strong&gt;→  sonst &lt;strong&gt;Heimfall&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbenlaub&lt;/strong&gt;/Erbenlob&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gesamthandprinzip &lt;/strong&gt;des &lt;strong&gt;Hausvermögens&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;HMA: &lt;/em&gt;Unterscheidung &lt;strong&gt;Kaufgut&lt;/strong&gt;/&lt;strong&gt;Erbgut&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;SMA: &lt;/em&gt;&lt;strong&gt;Generalsukzession &lt;/strong&gt;aus &lt;strong&gt;RR &lt;/strong&gt;übernommen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;frühe Neuzeit/Rezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vielzahl &lt;/strong&gt;an &lt;strong&gt;Regelungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Frauen &lt;/strong&gt;erben nur &lt;strong&gt;subsidiär&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;verzigene&lt;/strong&gt;/&lt;strong&gt;unverzigene&lt;/strong&gt; &lt;strong&gt;Töchter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Kodifiziertes Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Joseph II:&lt;/strong&gt; Parentelsystem mit &lt;strong&gt;6 Parentelen&lt;/strong&gt; als &lt;strong&gt;einheitliche &lt;/strong&gt;Regelung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;durchgehendes Repräsentationsrecht &lt;/strong&gt;in allen Parentelen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;ABGB 1811&lt;/strong&gt;: übernimmt &lt;strong&gt;Parentelsystem&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Teilnovelle 1914&lt;/strong&gt;: Begrenzung bei &lt;strong&gt;4. Parentele ohne Repräsentationsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;gestzl&lt;/strong&gt;. Erbfolge &lt;strong&gt;subsidiär &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;alle &lt;strong&gt;Rechte &lt;/strong&gt;und &lt;strong&gt;Verbindl&lt;/strong&gt;. &lt;strong&gt;vererbbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Prinzip der &lt;strong&gt;Generalsukzession &lt;/strong&gt;-&amp;gt; bei &lt;strong&gt;Spezialsukzession zerfällt Nachlass&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Parentelsystem &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erbunfähig&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ausländer &lt;/strong&gt;deren &lt;strong&gt;Heimatland &lt;/strong&gt;Ö &lt;strong&gt;Staatsbürger schlechter stellt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbunwürdigkeit&lt;/strong&gt; oder &lt;strong&gt;Inkapazität&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Anwachsungsprinzip?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Hausvermögen &lt;/strong&gt;ist &lt;strong&gt;gesamthändisch &lt;/strong&gt;Strukturiert&lt;/li&gt;&lt;li&gt;Bei &lt;strong&gt;Tod&lt;/strong&gt; eines &lt;strong&gt;Genossen&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anwachsung&lt;/strong&gt; zu den &lt;strong&gt;übrigen&lt;/strong&gt; &lt;strong&gt;Miteigentümern&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Anfallsprinzip?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erbe&lt;/strong&gt; wird mit &lt;strong&gt;Tod &lt;/strong&gt;des &lt;strong&gt;Erblassers Eigentümer &lt;/strong&gt;der Erbschaft&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erwerbswille&lt;/strong&gt; bleibt &lt;strong&gt;unberücksichtigt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Antrittsprinzip?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erwerbswille &lt;/strong&gt;des &lt;strong&gt;Erben &lt;/strong&gt;wird &lt;strong&gt;berücksichtigt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Erst mit &lt;strong&gt;Willenserklärung &lt;/strong&gt;(&lt;em&gt;Erbserklärung&lt;/em&gt;) wird der Erbe &lt;strong&gt;berechtigt &lt;/strong&gt;am &lt;strong&gt;Nachlassvermögen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Gewere allgemein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beschreibt &lt;strong&gt;Zugehörigkeit &lt;/strong&gt;einer &lt;strong&gt;Sache &lt;/strong&gt;zum &lt;strong&gt;Wirtschaftskreis &lt;/strong&gt;einer &lt;strong&gt;Person &lt;/strong&gt;(oder eines Verbandes)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Träger &lt;/strong&gt;kann &lt;strong&gt;rechtswidrige Zugriffe &lt;/strong&gt;auf die Sache &lt;strong&gt;abwehren&lt;/strong&gt;, und nach &lt;strong&gt;Wegnahme herausverlangen (&lt;em&gt;dingliche Berechtigung&lt;/em&gt;)&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;basiert auf &lt;strong style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;tatsächlicher Sachherschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;Rechtsscheinwirkung&lt;/em&gt;&lt;/strong&gt;: &lt;strong&gt;Besitz &lt;/strong&gt;der Sache &lt;strong&gt;begründet&lt;/strong&gt; &lt;strong&gt;Vermutung des&lt;/strong&gt; &lt;strong&gt;Rechts &lt;/strong&gt;an der Sache&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur durch (&lt;strong&gt;gerichtlichen&lt;/strong&gt;) &lt;strong&gt;Beweis &lt;/strong&gt;einer &lt;strong&gt;stärkeren&lt;/strong&gt; &lt;strong&gt;Berechtigung gebrochen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -520,7 +1174,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B129"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -686,6 +1340,878 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add latest set of flash cads
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VL Geschichte des Privaten Rechts (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VL Geschichte des Privaten Rechts (JKU, Austria).xlsx
@@ -19,12 +19,378 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wann wurden eheliche den unehelichen Kindern gleichgestellt?&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Wie lange&lt;/strong&gt; hielt das an? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Josephinische Ehegesetzgebung 1783&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ausnahme: &lt;strong&gt;Ehebruchskinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Endete &lt;/strong&gt;mit &lt;strong&gt;Leopold II 1791 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Leopold musste viele der als radikal geltenden Reformen Joseph II zurücknehmen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie entwickelte sich das Erbrecht der &lt;strong&gt;un&lt;/strong&gt;ehelichen Kinder?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleiche Rechte&lt;/strong&gt;, wenn in Hausverband aufgenommen&lt;/li&gt;&lt;li&gt;Später &lt;strong&gt;christlichem Einfluss:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein Erbrechts&lt;/strong&gt; ggü. &lt;strong&gt;Vater&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehebruchskinder&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein &lt;/strong&gt;Erbrecht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;natürliche &lt;/strong&gt;Kinder (&lt;strong&gt;kein Ehehindernis &lt;/strong&gt;bei Eltern):&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbrecht &lt;strong&gt;gegen Mutter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Josephinisches Gesetzbuch&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Angleichung &lt;/strong&gt;an Rechtsstellung der &lt;strong&gt;ehelichen&lt;/strong&gt; &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;außer Ehebruchskinder&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zunächst &lt;strong&gt;keine Ansprüche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ab&lt;strong&gt; TN 1914&lt;/strong&gt;: Erbrecht &lt;strong&gt;nur gegen Mutter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Erbrechtsänderungsgesetz 1989&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;völlige Gleichstellung&lt;/strong&gt; mit ehelichen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Grund für Religionsspezifische Regeln im Eherecht im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Staat&lt;/strong&gt; hatte &lt;strong&gt;Interesse &lt;/strong&gt;daran &lt;strong&gt;Ehe gesetzlich &lt;/strong&gt;zu &lt;strong&gt;regeln &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Formell&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Inhaltlich &lt;/strong&gt;aber &lt;strong&gt;Regeln&lt;/strong&gt; &lt;strong&gt;der Konfessionen &lt;/strong&gt;übernommen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Materiell&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verhindert&lt;/strong&gt;, dass &lt;strong&gt;Gläubige &lt;/strong&gt;durch staatl. &lt;strong&gt;Eherecht gezwungen&lt;/strong&gt; sind &lt;strong&gt;gegen Regeln &lt;/strong&gt;ihrer &lt;strong&gt;Konfession&lt;/strong&gt; zu &lt;strong&gt;verstoßen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer ist normalerweise Erbe im MA?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gut an &lt;strong&gt;Sippe gebunden &lt;/strong&gt;- &lt;strong&gt;Gesamthand&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Anwachsung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;später im MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Parentelerbfolge&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Das Gut rinnt wie das Blut&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Deszendenten &lt;/strong&gt;vor &lt;strong&gt;Aszendeten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frauen subsidiär&lt;/strong&gt; -&amp;gt; nur wenn keine männlichen Erben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer konnte sich im ABGB 1811 nicht scheiden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Katholiken &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehe &lt;strong&gt;nur durch Tod &lt;/strong&gt;gelöst&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die leibliche Haftung (anders als die persönliche)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Schuldner haftet mit &lt;strong&gt;Körper&lt;/strong&gt; oder &lt;strong&gt;Freiheit&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind &lt;strong&gt;leibliche Haftung&lt;/strong&gt;, &lt;strong&gt;Sachhaftung&lt;/strong&gt;, &lt;strong&gt;Vermögenshaftung&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;leibliche Haftung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;G&lt;/strong&gt; kann S &lt;strong&gt;töten&lt;/strong&gt;, &lt;strong&gt;verstümmeln&lt;/strong&gt;, &lt;strong&gt;verknechten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;am &lt;strong&gt;Vermögen schadlos &lt;/strong&gt;halten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gewaltunterworfene &lt;/strong&gt;als &lt;strong&gt;Geiseln &lt;/strong&gt;nehmen bis Bezahlung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Sachhaftung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;G&lt;/strong&gt; hatte &lt;strong&gt;Sachherrschaft&lt;/strong&gt;, bei &lt;strong&gt;Nichtbezahlung Eigentum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Später &lt;strong&gt;nur &lt;/strong&gt;noch &lt;strong&gt;Verwertungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Vermögenshaftung (persönliche Haftung)&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aus &lt;strong&gt;leiblicher Haftung&lt;/strong&gt; wurde &lt;strong&gt;Schuldknechtschaft&lt;/strong&gt;, dann &lt;strong&gt;Schuldhaft &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;G&lt;/strong&gt; konnte aber dann &lt;strong&gt;keinen&lt;/strong&gt; &lt;strong&gt;Nutzen&lt;/strong&gt; &lt;strong&gt;aus S&lt;/strong&gt; ziehen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;war also &lt;strong&gt;nur&lt;/strong&gt; ein &lt;strong&gt;Druckmittel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher: &lt;em&gt;Vermögenshaftung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zugriff &lt;/strong&gt;auf das &lt;strong&gt;Vermögen&lt;/strong&gt; &lt;strong&gt;des S&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man die unbeschränkte Haftung eines Erben?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Vermögenshaftung &lt;/strong&gt;bzw &lt;strong&gt;persönliche &lt;/strong&gt;Haftung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Seit&lt;/strong&gt; &lt;strong&gt;wann &lt;/strong&gt;kennen wir das Prinzip, wonach Erben unbeschränkt haften können? Durch&lt;/p&gt;&lt;p&gt;welchen &lt;strong&gt;Einfluss&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Seit der &lt;strong&gt;Neuzeit &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;durch den &lt;strong&gt;Einfluss&lt;/strong&gt; der &lt;strong&gt;Rezeption&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herauslösen &lt;/strong&gt;des &lt;strong&gt;Schuldrechts aus&lt;/strong&gt; dem &lt;strong&gt;Strafrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Es gab in Einzelfällen die Veranlassung, dass Erben Schulden zu begleichen hatten – Warum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bei &lt;strong&gt;Vertragsschulden&lt;/strong&gt;, wenn &lt;strong&gt;Geschäftspartner &lt;/strong&gt;des Erblassers &lt;strong&gt;bereits&lt;/strong&gt; &lt;strong&gt;geleistet&lt;/strong&gt; hat&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist der Legatar ein Erbe? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nein - &lt;strong&gt;Vermächtnis&lt;/strong&gt;/&lt;strong&gt;Legat &lt;/strong&gt;hat &lt;strong&gt;keine Erbeinsetzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wie röm. &lt;strong&gt;Damnationslegat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur &lt;strong&gt;schuldrechtlicher Anspruch &lt;/strong&gt;ggü. dem &lt;strong&gt;Erben &lt;/strong&gt;auf &lt;strong&gt;Herausgabe &lt;/strong&gt;der vermachten Sachen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktionierten Testament und Testierfreiheit in der Neuzeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Testierfreiheit &lt;/strong&gt;mit &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Altersgrenze &lt;/strong&gt;(F &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;18&lt;/span&gt;, M &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;20&lt;/span&gt;)&lt;/li&gt;&lt;li&gt;Arten&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;: &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Testament&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Kodizill &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Erbvertrag &lt;/strong&gt;bekannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;subsidiär gesetzl. &lt;/strong&gt;Erbfolge.&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Pflichtteilsrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Möglichkeit der &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Enterbung&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbfolgeakte außergerichtlich &lt;/strong&gt;(Eröffnung des Testaments, Antreten der Erbschaft, Ergreifung des Nachlassbesitzes)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Anerbenrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;bäuerliche&lt;/em&gt; &lt;em&gt;Erbfolge &lt;/em&gt;- besonderes Erbrecht an &lt;strong&gt;landwirtschaftl&lt;/strong&gt;. &lt;strong&gt;Höfen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unteilbar &lt;/strong&gt;- nur&lt;strong&gt; einer von mehreren Erben&lt;/strong&gt; bekam den &lt;strong&gt;ganzen Hof&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;um &lt;strong&gt;Wirtschaftlichkeit &lt;/strong&gt;des Betriebs zu &lt;strong&gt;garantieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Auch im &lt;em&gt;ABGB 1811&lt;/em&gt; noch als &lt;em&gt;gesetzl&lt;/em&gt;. &lt;em&gt;Erbrecht &lt;/em&gt;enthalten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;konnte &lt;/strong&gt;aber per &lt;strong&gt;letztwilliger&lt;/strong&gt; &lt;strong&gt;Verfügung ausgeschlossen &lt;/strong&gt;werden&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die fränkische Affatomie und langobardische Thinx?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Affatomie&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur möglich wenn &lt;strong&gt;keine leibl. Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;König &lt;/strong&gt;musste Affatomie &lt;strong&gt;zustimmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;erbloses Gut normalerweise &lt;/strong&gt;an &lt;strong&gt;König&lt;/strong&gt; &lt;strong&gt;fiel&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Thinx&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verschaffte&lt;/strong&gt; &lt;strong&gt;Begünstigtem &lt;/strong&gt;die &lt;strong&gt;Rechtsstellung&lt;/strong&gt; eines &lt;strong&gt;Sohnes &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;quasi &lt;em&gt;Adoption&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erbe &lt;/strong&gt;damit &lt;strong&gt;ohne Blutsverwandtschaft &lt;/strong&gt;möglich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Teilung nach Köpfen und die Teilung nach Stämmen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;nach &lt;em&gt;Köpfen&lt;/em&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;alle&lt;/strong&gt; zur Erbschaft berufenen &lt;strong&gt;teilen Nachlass gleichmäßig &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;nach &lt;em&gt;Stämmen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nachkommen vertreten&lt;/strong&gt; &lt;strong&gt;Erben&lt;/strong&gt;, falls Erbe zum Zeitpunkt des Erbfalls nicht mehr lebt &lt;/li&gt;&lt;li&gt;-&amp;gt; &lt;strong&gt;Repräsentationsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Erbquote des überlebenden Ehegatten in der gesetzl. Erbfolge heute?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Quote &lt;strong&gt;abhängig&lt;/strong&gt; von &lt;strong&gt;restlicher&lt;/strong&gt; &lt;strong&gt;Verwandtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ggü. lebender&lt;strong&gt; 1. Parentel&lt;/strong&gt;: &lt;strong&gt;1/3&lt;/strong&gt; Ehegatte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ggü. lebender &lt;strong&gt;2. Parentel&lt;/strong&gt;: &lt;strong&gt;2/3&lt;/strong&gt; Ehegatee&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Unabhängig von Erbrecht: &lt;strong&gt;gesetzl Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;alle zum &lt;strong&gt;Haushalt &lt;/strong&gt;gehörenden &lt;strong&gt;beweglichen Sachen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anspruch &lt;/strong&gt;auf &lt;strong&gt;verbleib &lt;/strong&gt;in der &lt;strong&gt;ehelichen Wohnung&lt;/strong&gt; gegen Erben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Besteht im Mittelalter ein Ehegattenerbrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;im &lt;strong&gt;heimischen Gewohnheitsrecht&lt;/strong&gt; &lt;strong&gt;kein Erbrecht&lt;/strong&gt; der Ehegatten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eheschließung &lt;/strong&gt;begründet &lt;strong&gt;keine Verwandtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fallrecht &lt;/strong&gt;stand einem &lt;strong&gt;Ehegattenrecht entgegen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Auch kein Drang: &lt;strong&gt;Ehegüterrecht &lt;/strong&gt;ermöglichte für &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert der Erbschaftserwerb heute?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;gerichtliches Nachlassverfahren (&lt;strong&gt;Verlassenschaftsabhandlung&lt;/strong&gt;) legt Nachlass fest &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Todesfallaufnahme&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dann &lt;strong&gt;Erbserklärung &lt;/strong&gt;des berufenen Erben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der sein Recht beweisen muss - &lt;strong&gt;Erbrechtsausweis&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ist alles vorhanden, folgt die &lt;em&gt;gerichtliche Besitzeinweisung &lt;/em&gt;(&lt;strong&gt;Einantwortung&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bis dahin&lt;/strong&gt; &lt;strong&gt;ruht &lt;/strong&gt;der Nachlass&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der ausgewiesene &lt;strong&gt;Erbe kann &lt;/strong&gt;diesen aber schon &lt;strong&gt;verwalten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das beneficium inventarii?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Beschränkte Erbenhaftung&lt;/strong&gt; - haftet &lt;strong&gt;nur mit &lt;/strong&gt;dem &lt;strong&gt;Nachlass&lt;/strong&gt;, nicht persönlich.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Herrscht heute formelles oder materielles Eintrittsrecht?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;em&gt;Formelles&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erbe erbt aus &lt;strong&gt;eigenem Recht&lt;/strong&gt;, &lt;strong&gt;nicht &lt;/strong&gt;aus Recht des &lt;strong&gt;Gradnächsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;d.h. bei &lt;strong&gt;Erbunfähigkeit &lt;/strong&gt;des &lt;strong&gt;Gradnächsten &lt;/strong&gt;erben dessen &lt;strong&gt;Nachkommen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was war die Parentelenordnung im MA?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ursprünglich&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;engerer &lt;/strong&gt;Erbenkreis: &lt;strong&gt;Hausgemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;weiterer&lt;/strong&gt; Erbenkreis: &lt;strong&gt;Blutsverwandte &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Parentelenordnung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anerkennung &lt;/strong&gt;des &lt;strong&gt;Repräsentationsrecht &lt;/strong&gt;für &lt;strong&gt;Kinder &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;dehnte engeren&lt;/strong&gt; Erbenkreis &lt;strong&gt;aus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;führte zu &lt;strong&gt;Parentelenordnung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;jüngere Generation ist älterer erbrechtlich vorangestellt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;strong&gt;Das Gut rinnt wie das Blut&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Erbgut und Kaufgut?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbgut&lt;/em&gt;: hat man &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;selbst vererbt &lt;/strong&gt;bekommen, wird &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;familiär weitergegeben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Kaufgut&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;selbst erwirtschaftetes &lt;/strong&gt;Vermögen zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;freien&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verfügung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Spezialsukzession?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der &lt;strong&gt;Nachlass &lt;/strong&gt;zerfällt in &lt;strong&gt;verschiedene Vermögensmassen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gehen in &lt;strong&gt;spezifischer Erbfolge &lt;/strong&gt;auf die &lt;strong&gt;Erben &lt;/strong&gt;über&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abweichung &lt;/strong&gt;von der &lt;strong&gt;gesetzlichen Erbfolge&lt;/strong&gt; ist &lt;strong&gt;möglich &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren Näherrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;dingliche Erwerbsrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Bei &lt;strong&gt;Eigentumswechsel &lt;/strong&gt;kann ein &lt;strong&gt;näher Berechtigter &lt;/strong&gt;(z.B.: Sippengenosse)&lt;strong&gt; &lt;/strong&gt;als der neue Eigentümer &lt;strong&gt;innerhalb &lt;/strong&gt;einer gewissen &lt;strong&gt;Frist&lt;/strong&gt; das &lt;strong&gt;Gut &lt;/strong&gt;an &lt;strong&gt;sich nehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schützt &lt;strong&gt;Sippeneigentum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abschwächung &lt;/strong&gt;zu &lt;strong&gt;Vorkaufs&lt;/strong&gt;- und &lt;strong&gt;Einstandsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Besserberechtigte musste &lt;strong&gt;Kaufpreis &lt;/strong&gt;und &lt;strong&gt;Kosten erstatten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur &lt;strong&gt;vertraglich begründete &lt;/strong&gt;Näherrechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren Leiherechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bodenleihe &lt;/strong&gt;verschaffte &lt;strong&gt;gegen&lt;/strong&gt; &lt;strong&gt;Entgelt Nutzungsrechte &lt;/strong&gt;an fremden Boden&lt;/li&gt;&lt;li&gt;Unterscheidung:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;freihe &lt;/em&gt;Leihe: &lt;strong&gt;Leistung&lt;/strong&gt; &lt;strong&gt;aus &lt;/strong&gt;dem &lt;strong&gt;Leihgut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;unfreie &lt;/em&gt;Leihe: &lt;strong&gt;persönliche &lt;/strong&gt;und &lt;strong&gt;wirtschaftliche Leistung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Arten (nach &lt;strong&gt;Personengruppen&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;bäuerliche&lt;/em&gt; Leihe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;städtische &lt;/em&gt;Leihe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ritterliche &lt;/em&gt;Leihe&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Ewigsatzung, was die Totsatzung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Ewigsatzung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Früchte &lt;/strong&gt;werden &lt;strong&gt;nicht&lt;/strong&gt; auf die &lt;strong&gt;Schuld angerechnet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pfand &lt;strong&gt;löst &lt;/strong&gt;sich &lt;strong&gt;NICHT selbst&lt;/strong&gt; auf.&lt;/li&gt;&lt;li&gt;&lt;em&gt;Totsatzung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Früchte &lt;/strong&gt;wurden auf die &lt;strong&gt;Schuld angerechnet &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pfand löst &lt;/strong&gt;sich somit nach gewisser Zeit &lt;strong&gt;selbst auf&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Fahrnispfandrecht? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Faustpfand &lt;/strong&gt;-&amp;gt; Übertragung &lt;strong&gt;leibliche Gewere &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;wurde &lt;strong&gt;Eigentümer&lt;/strong&gt;, wenn &lt;strong&gt;nicht in Frist eingelöst&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;13 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;konnte auf &lt;strong&gt;gesamtes Vermögen &lt;/strong&gt;zugreifen, wenn Pfand &lt;strong&gt;unterging &lt;/strong&gt;oder an &lt;strong&gt;Wert verlor &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Einführung des &lt;strong&gt;Verkaufspfandes&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Entwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;konnte durch &lt;strong&gt;Willensübereinstimmung &lt;/strong&gt;entstehen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;rechtlich schwach &lt;/strong&gt;(&lt;strong&gt;keine Verfolgungsklage &lt;/strong&gt;des Gläubigers &lt;strong&gt;ggü Dritten&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;18 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rückkehr zum &lt;strong&gt;Faustpfand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Faustpfand&lt;/strong&gt; und &lt;strong&gt;Hypothek&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Hypothek?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Pfandrecht &lt;/strong&gt;der &lt;strong&gt;jüngeren Satzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;besitzloses &lt;/strong&gt;Pfand im Liegenschaftsrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;in der &lt;strong&gt;Rezeption &lt;/strong&gt;(&lt;strong&gt;Neuzeit&lt;/strong&gt;) entwickelt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;hat &lt;strong&gt;Hypothek &lt;/strong&gt;(&lt;em&gt;beschränkt dingliches Recht&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;Nichtbegleichung &lt;/strong&gt;der Schuld kann er es &lt;strong&gt;geltend machen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Begründet durch&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;formfreien Vertrag &lt;/strong&gt;(&lt;strong&gt;Vertrags&lt;/strong&gt;pfandrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kraft &lt;strong&gt;Gesetz &lt;/strong&gt;(&lt;strong&gt;gesetzliches &lt;/strong&gt;Pfandrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;richterliche &lt;/strong&gt;Verfügung (&lt;strong&gt;Pfändungs&lt;/strong&gt;pfandrecht)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Dienstbarkeiten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Übernommen aus &lt;strong&gt;RR&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Grunddienstbarkeiten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;beschränkt dingliche Rechte &lt;/strong&gt;an &lt;strong&gt;Grundstücken&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eigentümer&lt;/strong&gt; muss &lt;strong&gt;Ausübung &lt;/strong&gt;des Rechts &lt;strong&gt;dulden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ins &lt;strong&gt;ABGB 1811&lt;/strong&gt; übernommen&lt;/li&gt;&lt;li&gt;&lt;em&gt;persönliche&lt;/em&gt; &lt;em&gt;Dienstbarkeiten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grunddienstbarkeiten &lt;/strong&gt;die einer &lt;strong&gt;bestimmten Person &lt;/strong&gt;zugeordnet werden -&amp;gt; &lt;em&gt;Leibzucht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;durch&lt;strong&gt; Rezeption&lt;/strong&gt;: &lt;strong&gt;Personalservituten &lt;/strong&gt;(&lt;em&gt;ususfructus, usus, habitatio&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind beschränkt dingliche Rechte?&lt;/p&gt;&lt;p&gt;Nennen sie ein Beispiel&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Belastungen &lt;/strong&gt;des Eigentums &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beschränkt&lt;/strong&gt; die Rechte des &lt;strong&gt;Eigentümers&lt;/strong&gt;, &lt;/li&gt;&lt;li class="ql-indent-1"&gt;gibt &lt;strong&gt;Teilberechtigungen&lt;/strong&gt; an den &lt;strong&gt;Berechtigten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Arten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pfand&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dienstbarkeiten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reallasten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Aufbau des ABGB?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Institutionensystem &lt;/em&gt;(auch &lt;strong&gt;gaianisches &lt;/strong&gt;System)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zweiteilung in &lt;strong&gt;Personen&lt;/strong&gt;- und &lt;strong&gt;Vermögensrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Pandektensystem&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aufteilung in &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Allgemeinen &lt;/strong&gt;Teil&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schuld&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sachen&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Familien&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erb&lt;/strong&gt;recht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Landtafeln?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Seit 13/14 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Form / Teil des &lt;strong&gt;Grundbuchs&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;für &lt;strong&gt;Adelige&lt;/strong&gt; &lt;strong&gt;Liegenschaften &lt;/strong&gt;- &lt;em&gt;Eintragungspflicht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;dingliche Rechte &lt;/strong&gt;gelten nur mit &lt;strong&gt;Eintragung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Typenzwang?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sachenrecht definiert &lt;/strong&gt;alle möglichen &lt;strong&gt;dingliche Berechtigungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es können &lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;weiteren &lt;/strong&gt;"&lt;strong&gt;erfunden&lt;/strong&gt;" werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;= &lt;em&gt;numerus clausus&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Stellung unehelicher Kinder im älteren Recht?&lt;/p&gt;&lt;p&gt;Wann änderte sich dies?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleichstellung &lt;/strong&gt;mit &lt;strong&gt;ehelichen&lt;/strong&gt;, wenn in &lt;strong&gt;Hausverband aufgenommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;sonst &lt;/strong&gt;Zugehörigkeit zu &lt;strong&gt;Muttersippe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schlechterstellung &lt;/strong&gt;ab &lt;strong&gt;christlicher &lt;/strong&gt;Zeit&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Stellung Joseph II zu unehelichen Kindern&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundsätzliche Gleichstellung &lt;/strong&gt;eheliche und uneheliche&lt;/li&gt;&lt;li&gt;Ausnahme: &lt;strong&gt;Ehebruchskinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Stellung der ehelichen und unehelichen Kinder im MA und im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Eheliche &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eheliche Kinder unter &lt;strong&gt;Munt &lt;/strong&gt;des Vaters&lt;/li&gt;&lt;li class="ql-indent-2"&gt;u.a. &lt;strong&gt;Verwaltung &lt;/strong&gt;von &lt;strong&gt;Vermögen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste &lt;/strong&gt;Form der &lt;strong&gt;Unterhaltspflicht&lt;/strong&gt;: &lt;strong&gt;Zweckbindung &lt;/strong&gt;es &lt;strong&gt;Kindesvermögens&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aussteuer &lt;/strong&gt;(Ausstattung) bei Ausscheiden des Kindes &lt;strong&gt;aus Muntgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Uneheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gleichberechtigt &lt;/strong&gt;wenn in Hausverband &lt;strong&gt;aufgenommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Christlicher &lt;/strong&gt;Einfluss:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Verlust Erbrecht &lt;/strong&gt;gegen Vater&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Ausschluss &lt;/strong&gt;aus &lt;strong&gt;Berufen &lt;/strong&gt;und &lt;strong&gt;Zünften&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;keine kirchlichen &lt;/strong&gt;Ämter&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Eheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unterhalt &lt;/strong&gt;Vater, &lt;strong&gt;Pflege &lt;/strong&gt;Mutter&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater &lt;strong&gt;gesetzlicher Vertreter&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater &lt;strong&gt;verwaltet Kindesvermögen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kind erhält &lt;strong&gt;Familien&lt;/strong&gt;+ &lt;strong&gt;Standesrecht &lt;/strong&gt;des &lt;strong&gt;Vaters&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Uneheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bis 1. TN &lt;strong&gt;kein Verwandtschaftsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dann gegenüber Mutter &lt;/strong&gt;gleiche Rechte &lt;strong&gt;wie eheliche&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater: &lt;strong&gt;Unterhaltsanspruch&lt;/strong&gt;, &lt;strong&gt;Besuchsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ehe- und Familienmodell ABGB 1811 und welches war davor?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;patriarchales &lt;/strong&gt;Familienmodell - "&lt;strong&gt;Überlegenheit &lt;/strong&gt;des &lt;strong&gt;Mannes&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;davor&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vernunftrechtliche &lt;/strong&gt;Familie: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ansätze partnerschaftlichen &lt;/strong&gt;Modells&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Recht auf &lt;strong&gt;Persönlichkeitsentfaltung Frau &lt;/strong&gt;+ &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Selbstbestimmungsrecht der Frau bei Ehe - früher und heute?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Frau unter &lt;strong&gt;Muntgewalt &lt;/strong&gt;- wenig Selbstbestimmung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Mittelalter&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Besserstellung &lt;/strong&gt;der Frau durch &lt;strong&gt;christlichen &lt;/strong&gt;Einfluss&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehemann vertrat &lt;/strong&gt;Frau vor &lt;strong&gt;Gericht &lt;/strong&gt;und bei &lt;strong&gt;Rechtsgeschäften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Frau &lt;/strong&gt;konnte &lt;strong&gt;alltägliche Rechtsgeschäfte &lt;/strong&gt;&lt;em&gt;für Mann &lt;/em&gt;durchführen&lt;/li&gt;&lt;li&gt;Aufkommen &lt;strong&gt;gegenseitiger Treuepflicht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeit&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leitungsfunktion &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;ausgebaut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verpflichtung &lt;/strong&gt;der &lt;strong&gt;Sicherung &lt;/strong&gt;des &lt;strong&gt;Unterhalts &lt;/strong&gt;der Frau&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Treue- und Beistandspflicht usus (aber nicht rechtlich verankert)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Naturrechtliche Lehre&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Katalog&lt;strong&gt; gegenseitige Rechte &lt;/strong&gt;und &lt;strong&gt;Pflichten &lt;/strong&gt;der Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Seit &lt;em&gt;Familienrechtsreform 1975&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;eheliche &lt;strong&gt;Gleichberechtigung &lt;/strong&gt;von Mann und Frau&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Seit wann gibt es in Österreich die Zivilehe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Seit den &lt;strong&gt;Maigesetzen 1868&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Notzivilehe &lt;/strong&gt;-&amp;gt; ohne kanonische Vorschriften&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Seit &lt;em&gt;1945&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;obligatorische&lt;/em&gt; Zivilehe&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Eliminierung &lt;/strong&gt;der &lt;strong&gt;nationalsozialistischen &lt;/strong&gt;Bestimmungen des &lt;strong&gt;dt. Ehegestez 1938&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Übernahme &lt;/strong&gt;ins &lt;strong&gt;ABGB&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eheschließung bis ABGB 1811&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Mittelalter: &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mehrere&lt;/strong&gt; &lt;strong&gt;Formen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Kirche &lt;/em&gt;hatte &lt;em&gt;Ehehoheit &lt;/em&gt;&lt;/li&gt;&lt;li&gt;Siehe Frage "&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Welche Arten der Ehe gab es im Mittelalter?"&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kompetenzkonflikt &lt;/strong&gt;Kirche vs Staat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Staatliches &lt;/strong&gt;Eherecht &lt;strong&gt;als&lt;/strong&gt; &lt;strong&gt;zweites&lt;/strong&gt;, ebenso &lt;strong&gt;gültiges&lt;/strong&gt;, Eherecht &lt;strong&gt;neben Kirchlichem&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;18 JH (vernunftrechtlische Naturrecht) &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehe dient &lt;/strong&gt;dem&lt;strong&gt; Staats&lt;/strong&gt;interesse&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;polizeistaatliches Ehemodell&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Joseph II 1783&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trennung Ehesakrament&lt;/strong&gt; &lt;strong&gt;Ehevertrag&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;nicht obligatorische &lt;/strong&gt;Zivilehe&lt;/li&gt;&lt;li&gt;Siehe Karte&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;dreigeteilt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Siehe Karte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hat es eine Zeit gegeben, in der das kanonische Recht auch für Katholiken-Ehen gegolten hat?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zwischen Konkordat 1855 und Maigesetze 1868&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die weitere Entwicklung des Eherechts nach ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Konkordat 1855&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit Kirche &lt;/strong&gt;unterstellt&lt;/li&gt;&lt;li&gt;&lt;em&gt;Maigesetze 1868 &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Notzivilehe &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wiederherstellung &lt;/strong&gt;Eherecht &lt;strong&gt;ABGB &lt;/strong&gt;1811&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit &lt;/strong&gt;wieder &lt;strong&gt;staatlich &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Festsetzung &lt;strong&gt;Monogamie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;keine &lt;/strong&gt;Möglichkeit der &lt;strong&gt;Scheidung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dispensehe 1919 &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Frage dazu&lt;/li&gt;&lt;li&gt;&lt;em&gt;Konkordat 1934&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eherecht&lt;/strong&gt; für &lt;strong&gt;Katholiken&lt;/strong&gt; wieder an &lt;strong&gt;Kirche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dt. Ehegesetz 1938&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;einheitliches Eherecht &lt;/strong&gt;im ganzen Reich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;siehe Frage dazu&lt;/li&gt;&lt;li&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übernommen aus &lt;strong&gt;Ehegesetz 1938 &lt;/strong&gt;"&lt;strong&gt;entnazifizert&lt;/strong&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Obligatorische Zivilehe &lt;/strong&gt;für alle Konfessionen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eherecht ABGB 1811 - Unterschied zu heute&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;ABGB &lt;/em&gt;hatte (anders als heute) &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dreifach gegliedertes &lt;/strong&gt;Eherecht: Katholiken, Protestanten, Juden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehehindernis&lt;/strong&gt;: Wiederverheiratung nicht möglich, solange &lt;strong&gt;katholischer&lt;/strong&gt; &lt;strong&gt;Ehepartner noch lebt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Keine &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Zivilehe&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Güterstand im Älteren Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Vermögenstrennung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;hat Recht auf &lt;strong&gt;Verwaltung &lt;/strong&gt;+ &lt;strong&gt;Nutzung &lt;/strong&gt;von &lt;strong&gt;Frauenvermögen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Leibgedinge&lt;/em&gt;: &lt;strong&gt;unentgeltliches Nutzungsrecht &lt;/strong&gt;auf Lebenszeit an einem Objekt des Ehepartners.&lt;/li&gt;&lt;li&gt;&lt;em&gt;Heiratsgabensystem&lt;/em&gt;: &lt;strong&gt;Heimsteuer &lt;/strong&gt;+ &lt;strong&gt;Widerlage&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Heiratsgabensystem im Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;= Zur &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Heimsteuer&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Heiratsgabe der &lt;strong&gt;Frau &lt;/strong&gt;- Zuschuss zu finanziellen Lasten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gegengewicht &lt;/strong&gt;zu &lt;strong&gt;Mann &lt;/strong&gt;als einzige &lt;strong&gt;Einnahmequelle&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Widerlage &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;fällig bei (&lt;strong&gt;Vor&lt;/strong&gt;)&lt;strong&gt;Tod&lt;/strong&gt; des &lt;strong&gt;Mannes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;wenn Heimsteuer &lt;/strong&gt;geleistet wurde&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Im &lt;strong&gt;Todesfalle &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;-&amp;gt; beides zusammen zur &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Güterstand im Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;beschränkte Gütergemeinschaft &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur für &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;bestimmte&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Objekte&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(z.B.: &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Liegenschaften&lt;/span&gt;)&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;Gesamthand&lt;/strong&gt;" -&amp;gt; Rechtsgeschäfte erfordern Zu&lt;strong&gt;stimmung beider&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Errungenschaftsgemeinschaften&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;der &lt;strong&gt;beschränkten &lt;/strong&gt;Gütergemeinschaft&lt;/li&gt;&lt;li&gt;Auch &lt;strong&gt;zukünftiges Vermögen &lt;/strong&gt;miteinbezogen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Fahrnisgemeinschaft&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Errungenschaften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eingebrachte&lt;/strong&gt; und &lt;strong&gt;unentgeltlich erworbene &lt;/strong&gt;&lt;em&gt;Fahrnis&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Rentleinsheirat&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;allgemeine &lt;/strong&gt;&lt;strong&gt;Gütergemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;eingebrachtes&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erworbenes&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Vermögen beider&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die große Familienrechtsreform?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1970er&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Verwirklichung des &lt;strong&gt;Gleichberechtigungsgrundsatzes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;elterliche Gleichberechtigung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;verstärkter&lt;strong&gt; Schutz&lt;/strong&gt; der &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anerkennung&lt;/strong&gt; der &lt;strong&gt;Privatautonomie &lt;/strong&gt;im &lt;strong&gt;familiären &lt;/strong&gt;Bereich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Polizeistaatliche Familienmodell?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Christliche &lt;strong&gt;Familie &lt;/strong&gt;hatte &lt;strong&gt;im MA &lt;/strong&gt;im &lt;strong&gt;Obrigkeitsstaat &lt;/strong&gt;eine &lt;strong&gt;staatsdienende&lt;/strong&gt; Bedeutung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wurde durch &lt;strong&gt;aristotelische Hauslehre &lt;/strong&gt;erklärt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hausherr&lt;/strong&gt; sorgt für &lt;em&gt;obrigkeitstreues Verhalten &lt;/em&gt;der &lt;strong&gt;Hausgenossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Staat überwacht &lt;/strong&gt;die Pflichterfüllung des &lt;strong&gt;Hausherrn&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Familie &lt;/strong&gt;war also &lt;strong&gt;Element &lt;/strong&gt;des &lt;strong&gt;Polizeistaats&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Beziehung der Ehegatten untereinander im ABGB 1811?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;als "&lt;strong&gt;Haupt&lt;/strong&gt;" der Familie&lt;/li&gt;&lt;li class="ql-indent-1"&gt;hat &lt;strong&gt;Unterhaltspflicht &lt;/strong&gt;und &lt;strong&gt;Leitungsrecht&lt;/strong&gt; &lt;strong&gt;gegenüber Frau&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ansicht der "traditionelle Rollenverteilung"&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Aristotelische Hauslehre?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Haus &lt;/strong&gt;(Familie) ist &lt;strong&gt;Teil &lt;/strong&gt;einer &lt;strong&gt;übergeordneten Gemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestimmt den &lt;em&gt;Sozialstatus &lt;/em&gt;der Menschen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater vertritt &lt;/strong&gt;Familie nach außen &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater &lt;/strong&gt;hat &lt;strong&gt;Gewalt &lt;/strong&gt;über &lt;strong&gt;Hausgemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Majorenitäts-Jahresbestimmung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Volljährigkeit &lt;/strong&gt;in allen &lt;strong&gt;dt. Erbkönigreichen&lt;/strong&gt; und &lt;strong&gt;Ländern &lt;/strong&gt;auf &lt;strong&gt;24 Jahre&lt;/strong&gt; festgesetzt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Fähigkeiten kommen abgeschichteten Söhnen zu?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vermögensrechtlich Selbständig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Familiengründung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;etc&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet Abschichtung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Erreichen der &lt;strong&gt;Mündigkeit &lt;/strong&gt;von &lt;strong&gt;Haussöhnen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Nach &lt;strong&gt;Ausscheiden &lt;/strong&gt;aus dem &lt;strong&gt;väterlichen Haushalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Teilbereiche der Handlungsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Deliktsfähigkeit&lt;/em&gt;: Fähigkeit, sich durch &lt;strong&gt;rechtswidriges Verhalten&lt;/strong&gt; zu &lt;strong&gt;verpflichten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Geschäftsfähigkeit&lt;/em&gt;: Fähigkeit sich durch &lt;strong&gt;Rechtsgeschäfte&lt;/strong&gt; zu &lt;strong&gt;verpflichten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die allgemeine (unbeschränkte) Rechtsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Recht der&lt;/strong&gt; &lt;strong&gt;Persönlichkeit&lt;/strong&gt; im &lt;em&gt;Naturrecht&lt;/em&gt; und &lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Siehe auch Frage "Statuslehre"&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Statuslehre?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;röm Recht übernommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;libertatis&lt;/strong&gt;: &lt;em&gt;Freie&lt;/em&gt; vs &lt;em&gt;Sklaven&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;civitatis&lt;/strong&gt;: &lt;em&gt;Bürger &lt;/em&gt;vs &lt;em&gt;Fremde&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;familiae&lt;/strong&gt;: &lt;em&gt;Zugehörigkeit &lt;/em&gt;zu &lt;em&gt;Familie&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Entwicklung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Codex &lt;strong&gt;Theresianus &lt;/strong&gt;folgte &lt;strong&gt;Statuslehre&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ablösung &lt;/strong&gt;durch &lt;strong&gt;naturrechtliche &lt;/strong&gt;Vorstellungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Recht der Persönlichkeit&lt;/em&gt; (angeborenes Recht, &lt;strong&gt;frei zu handeln &lt;/strong&gt;und seine &lt;strong&gt;Würde &lt;/strong&gt;zu &lt;strong&gt;behaupten&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;= Allgemeine (unbeschränkte) Rechtsfähigkeit&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Übernahme&lt;/strong&gt; ins &lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Abhängigkeit der Bauern?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geteilt in &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;freie &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unfreie &lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Leibeigenschaft &lt;/strong&gt;in&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; Ö &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;nicht institutionalisiert&lt;/strong&gt;, &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;aber &lt;/span&gt;diverse &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Einschränkungen &lt;/strong&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Abhängigkeiten&lt;/span&gt; der &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unfreien &lt;/em&gt;&lt;em&gt;Bauern&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Sachenrechtlich &lt;/em&gt;(&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Abgaben &lt;/strong&gt;für Grund und Boden)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Politisch &lt;/em&gt;(&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundherr &lt;/span&gt;hatte &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichts&lt;/strong&gt;- und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Verwaltungsaufgaben&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Persönlich &lt;/em&gt;(&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Heiratsbewilligung&lt;/strong&gt;, befohlene &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Tätigkeit&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wohnsitzentscheidungen&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ab &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;16. JH&lt;/em&gt; (&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Bauernkriege&lt;/strong&gt;) -&amp;gt; Trend zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufhebung &lt;/strong&gt;der &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;persönlichen Abhängigkeit&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erst &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;18/19 JH beseitigt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Aufgaben hatte das Ehegüterrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Versorgung &lt;/strong&gt;des &lt;strong&gt;überlebenden &lt;/strong&gt;Ehegatten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufteilung &lt;/strong&gt;der &lt;strong&gt;finanziellen &lt;/strong&gt;Lasten (Finanzieller &lt;strong&gt;Beitrag der&lt;/strong&gt; &lt;strong&gt;Frau &lt;/strong&gt;wurde gefordert) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist mit Geschlechtervormundschaft gemeint?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Frau &lt;/strong&gt;ist &lt;strong&gt;immer unter &lt;/strong&gt;der &lt;strong&gt;Muntgewalt&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Väterliche Munt &lt;/em&gt;bis zur Verheiratung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dann &lt;em&gt;eheherrliche Munt&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Bei Ableben des Vaters vor Hochzeit:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;verwandsschaftliche Munt &lt;/em&gt;(Bruder oder anderer männl. Verwandter)&lt;/li&gt;&lt;li&gt;als Witwe entweder Munt der Verwandschaft oder des toten Ehemanns&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Salvatorische Klausel?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nach der Salvatorischen Klausel sollte das &lt;strong&gt;ius commune &lt;/strong&gt;nur &lt;strong&gt;subsidiär &lt;/strong&gt;gelten&lt;/p&gt;&lt;ul&gt;&lt;li&gt; &lt;strong&gt;Geltungsnachweises &lt;/strong&gt;für das &lt;strong&gt;Gewohnheitsrecht &lt;/strong&gt;war jedoch &lt;strong&gt;schwierig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher &lt;strong&gt;Trendumkehr&lt;/strong&gt;: Gegner musste &lt;em&gt;Beweis der Nichtrezeption&lt;/em&gt; erbringen, um das &lt;strong&gt;Gewohnheitsrecht durchzusetzen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Aussteuer?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mitgift&lt;/strong&gt; der &lt;strong&gt;Familie&lt;/strong&gt; der &lt;strong&gt;Frau&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;auch &lt;strong&gt;Heimsteuer&lt;/strong&gt; genannt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Was &lt;/strong&gt;und &lt;strong&gt;wann&lt;/strong&gt; waren die drei Phasen der Rezeption?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Frührezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;12.&lt;/strong&gt; und &lt;strong&gt;13&lt;/strong&gt;. JH &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Hauptrezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;15 &lt;/strong&gt;bis &lt;strong&gt;17&lt;/strong&gt;. JH &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Nachrezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;18&lt;/strong&gt; JH&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;in &lt;/strong&gt;Ö vor allem &lt;strong&gt;erbrechtliche &lt;/strong&gt;Bestimmungen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Wovon hängt die Handlungsfähigkeit heutzutage ab?&lt;/p&gt;</t>
   </si>
   <si>
@@ -49,360 +415,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Wirtschaftlicher &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Feudalismus&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;mittelalterliche Grundherrschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;leihender &lt;strong&gt;Bauer&lt;/strong&gt;: &lt;strong&gt;unmittelbare &lt;/strong&gt;Gewere&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grundherr&lt;/strong&gt;: &lt;strong&gt;mittelbare &lt;/strong&gt;Gewere &lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wer konnte sich im ABGB 1811 nicht scheiden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Katholiken &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehe &lt;strong&gt;nur durch Tod &lt;/strong&gt;gelöst&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die leibliche Haftung (anders als die persönliche)?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Schuldner haftet mit &lt;strong&gt;Körper&lt;/strong&gt; oder &lt;strong&gt;Freiheit&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind &lt;strong&gt;leibliche Haftung&lt;/strong&gt;, &lt;strong&gt;Sachhaftung&lt;/strong&gt;, &lt;strong&gt;Vermögenshaftung&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;leibliche Haftung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;G&lt;/strong&gt; kann S &lt;strong&gt;töten&lt;/strong&gt;, &lt;strong&gt;verstümmeln&lt;/strong&gt;, &lt;strong&gt;verknechten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;am &lt;strong&gt;Vermögen schadlos &lt;/strong&gt;halten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gewaltunterworfene &lt;/strong&gt;als &lt;strong&gt;Geiseln &lt;/strong&gt;nehmen bis Bezahlung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Sachhaftung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;G&lt;/strong&gt; hatte &lt;strong&gt;Sachherrschaft&lt;/strong&gt;, bei &lt;strong&gt;Nichtbezahlung Eigentum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Später &lt;strong&gt;nur &lt;/strong&gt;noch &lt;strong&gt;Verwertungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Vermögenshaftung (persönliche Haftung)&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aus &lt;strong&gt;leiblicher Haftung&lt;/strong&gt; wurde &lt;strong&gt;Schuldknechtschaft&lt;/strong&gt;, dann &lt;strong&gt;Schuldhaft &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;G&lt;/strong&gt; konnte aber dann &lt;strong&gt;keinen&lt;/strong&gt; &lt;strong&gt;Nutzen&lt;/strong&gt; &lt;strong&gt;aus S&lt;/strong&gt; ziehen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;war also &lt;strong&gt;nur&lt;/strong&gt; ein &lt;strong&gt;Druckmittel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher: &lt;em&gt;Vermögenshaftung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zugriff &lt;/strong&gt;auf das &lt;strong&gt;Vermögen&lt;/strong&gt; &lt;strong&gt;des S&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie nennt man die unbeschränkte Haftung eines Erben?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Vermögenshaftung &lt;/strong&gt;bzw &lt;strong&gt;persönliche &lt;/strong&gt;Haftung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Seit&lt;/strong&gt; &lt;strong&gt;wann &lt;/strong&gt;kennen wir das Prinzip, wonach Erben unbeschränkt haften können? Durch&lt;/p&gt;&lt;p&gt;welchen &lt;strong&gt;Einfluss&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Seit der &lt;strong&gt;Neuzeit &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;durch den &lt;strong&gt;Einfluss&lt;/strong&gt; der &lt;strong&gt;Rezeption&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herauslösen &lt;/strong&gt;des &lt;strong&gt;Schuldrechts aus&lt;/strong&gt; dem &lt;strong&gt;Strafrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Es gab in Einzelfällen die Veranlassung, dass Erben Schulden zu begleichen hatten – Warum?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Bei &lt;strong&gt;Vertragsschulden&lt;/strong&gt;, wenn &lt;strong&gt;Geschäftspartner &lt;/strong&gt;des Erblassers &lt;strong&gt;bereits&lt;/strong&gt; &lt;strong&gt;geleistet&lt;/strong&gt; hat&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ist der Legatar ein Erbe? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nein - &lt;strong&gt;Vermächtnis&lt;/strong&gt;/&lt;strong&gt;Legat &lt;/strong&gt;hat &lt;strong&gt;keine Erbeinsetzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wie röm. &lt;strong&gt;Damnationslegat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur &lt;strong&gt;schuldrechtlicher Anspruch &lt;/strong&gt;ggü. dem &lt;strong&gt;Erben &lt;/strong&gt;auf &lt;strong&gt;Herausgabe &lt;/strong&gt;der vermachten Sachen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktionierten Testament und Testierfreiheit in der Neuzeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Testierfreiheit &lt;/strong&gt;mit &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Altersgrenze &lt;/strong&gt;(F &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;18&lt;/span&gt;, M &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;20&lt;/span&gt;)&lt;/li&gt;&lt;li&gt;Arten&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;: &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Testament&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Kodizill &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Erbvertrag &lt;/strong&gt;bekannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;subsidiär gesetzl. &lt;/strong&gt;Erbfolge.&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Pflichtteilsrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Möglichkeit der &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Enterbung&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbfolgeakte außergerichtlich &lt;/strong&gt;(Eröffnung des Testaments, Antreten der Erbschaft, Ergreifung des Nachlassbesitzes)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Anerbenrecht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;bäuerliche&lt;/em&gt; &lt;em&gt;Erbfolge &lt;/em&gt;- besonderes Erbrecht an &lt;strong&gt;landwirtschaftl&lt;/strong&gt;. &lt;strong&gt;Höfen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unteilbar &lt;/strong&gt;- nur&lt;strong&gt; einer von mehreren Erben&lt;/strong&gt; bekam den &lt;strong&gt;ganzen Hof&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;um &lt;strong&gt;Wirtschaftlichkeit &lt;/strong&gt;des Betriebs zu &lt;strong&gt;garantieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Auch im &lt;em&gt;ABGB 1811&lt;/em&gt; noch als &lt;em&gt;gesetzl&lt;/em&gt;. &lt;em&gt;Erbrecht &lt;/em&gt;enthalten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;konnte &lt;/strong&gt;aber per &lt;strong&gt;letztwilliger&lt;/strong&gt; &lt;strong&gt;Verfügung ausgeschlossen &lt;/strong&gt;werden&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die fränkische Affatomie und langobardische Thinx?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Affatomie&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur möglich wenn &lt;strong&gt;keine leibl. Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;König &lt;/strong&gt;musste Affatomie &lt;strong&gt;zustimmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;erbloses Gut normalerweise &lt;/strong&gt;an &lt;strong&gt;König&lt;/strong&gt; &lt;strong&gt;fiel&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Thinx&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verschaffte&lt;/strong&gt; &lt;strong&gt;Begünstigtem &lt;/strong&gt;die &lt;strong&gt;Rechtsstellung&lt;/strong&gt; eines &lt;strong&gt;Sohnes &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;quasi &lt;em&gt;Adoption&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erbe &lt;/strong&gt;damit &lt;strong&gt;ohne Blutsverwandtschaft &lt;/strong&gt;möglich&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Teilung nach Köpfen und die Teilung nach Stämmen? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;nach &lt;em&gt;Köpfen&lt;/em&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;alle&lt;/strong&gt; zur Erbschaft berufenen &lt;strong&gt;teilen Nachlass gleichmäßig &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;nach &lt;em&gt;Stämmen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;basierend auf &lt;strong&gt;Repräsentationsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;der jeweils &lt;strong&gt;Gradnächste &lt;/strong&gt;erbt&lt;/li&gt;&lt;li&gt;Also: &lt;strong&gt;Sohn &lt;/strong&gt;des &lt;strong&gt;Erblassers&lt;/strong&gt; schließt &lt;strong&gt;Enkel aus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie entwickelte sich das Erbrecht der &lt;strong&gt;un&lt;/strong&gt;ehelichen Kinder?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleiche Rechte&lt;/strong&gt;, wenn in Hausverband aufgenommen&lt;/li&gt;&lt;li&gt;Später &lt;strong&gt;christlichem Einfluss:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein Erbrechts&lt;/strong&gt; ggü. &lt;strong&gt;Vater&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehebruchskinder&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein &lt;/strong&gt;Erbrecht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;natürliche &lt;/strong&gt;Kinder (&lt;strong&gt;kein Ehehindernis &lt;/strong&gt;bei Eltern):&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbrecht &lt;strong&gt;gegen Mutter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Josephinisches Gesetzbuch&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Angleichung &lt;/strong&gt;an Rechtsstellung der &lt;strong&gt;ehelichen&lt;/strong&gt; &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;außer Ehebruchskinder&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zunächst &lt;strong&gt;keine Ansprüche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ab&lt;strong&gt; TN 1918&lt;/strong&gt;: Erbrecht &lt;strong&gt;nur gegen Mutter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Erbrechtsänderungsgesetz 1989&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;völlige Gleichstellung&lt;/strong&gt; mit ehelichen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann wurden eheliche den unehelichen Kindern gleichgestellt?&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Wie lange&lt;/strong&gt; hielt das an? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Josephinische Ehegesetzgebung 1786&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ausnahme: &lt;strong&gt;Ehebruchskinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Endete &lt;/strong&gt;mit &lt;strong&gt;Leopold II 1791 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Leopold musste viele der als radikal geltenden Reformen Joseph II zurücknehmen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Erbquote des überlebenden Ehegatten in der gesetzl. Erbfolge heute?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Quote &lt;strong&gt;abhängig&lt;/strong&gt; von &lt;strong&gt;restlicher&lt;/strong&gt; &lt;strong&gt;Verwandtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ggü. lebender&lt;strong&gt; 1. Parentel&lt;/strong&gt;: &lt;strong&gt;1/3&lt;/strong&gt; Ehegatte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ggü. lebender &lt;strong&gt;2. Parentel&lt;/strong&gt;: &lt;strong&gt;2/3&lt;/strong&gt; Ehegatee&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Unabhängig von Erbrecht: &lt;strong&gt;gesetzl Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;alle zum &lt;strong&gt;Haushalt &lt;/strong&gt;gehörenden &lt;strong&gt;beweglichen Sachen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anspruch &lt;/strong&gt;auf &lt;strong&gt;verbleib &lt;/strong&gt;in der &lt;strong&gt;ehelichen Wohnung&lt;/strong&gt; gegen Erben&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Besteht im Mittelalter ein Ehegattenerbrecht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;im &lt;strong&gt;heimischen Gewohnheitsrecht&lt;/strong&gt; &lt;strong&gt;kein Erbrecht&lt;/strong&gt; der Ehegatten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eheschließung &lt;/strong&gt;begründet &lt;strong&gt;keine Verwandtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fallrecht &lt;/strong&gt;stand einem &lt;strong&gt;Ehegattenrecht entgegen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Auch kein Drang: &lt;strong&gt;Ehegüterrecht &lt;/strong&gt;ermöglichte für &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktioniert der Erbschaftserwerb heute?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;gerichtliches Nachlassverfahren (&lt;strong&gt;Verlassenschaftsabhandlung&lt;/strong&gt;) legt Nachlass fest &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Todesfallaufnahme&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dann &lt;strong&gt;Erbserklärung &lt;/strong&gt;des berufenen Erben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der sein Recht beweisen muss - &lt;strong&gt;Erbrechtsausweis&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ist alles vorhanden, folgt die &lt;em&gt;gerichtliche Besitzeinweisung &lt;/em&gt;(&lt;strong&gt;Einantwortung&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bis dahin&lt;/strong&gt; &lt;strong&gt;ruht &lt;/strong&gt;der Nachlass&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der ausgewiesene &lt;strong&gt;Erbe kann &lt;/strong&gt;diesen aber schon &lt;strong&gt;verwalten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das beneficium inventarii?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Beschränkte Erbenhaftung&lt;/strong&gt; - haftet &lt;strong&gt;nur mit &lt;/strong&gt;dem &lt;strong&gt;Nachlass&lt;/strong&gt;, nicht persönlich.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Was &lt;/strong&gt;und &lt;strong&gt;wann&lt;/strong&gt; waren die drei Phasen der Rezeption?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Frührezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;12.&lt;/strong&gt; und &lt;strong&gt;13&lt;/strong&gt;. JH &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Hauptrezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;15 &lt;/strong&gt;bis &lt;strong&gt;17&lt;/strong&gt;. JH &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Nachrezeption&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;18&lt;/strong&gt; JH&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;in &lt;/strong&gt;Ö vor allem &lt;strong&gt;erbrechtliche &lt;/strong&gt;Bestimmungen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Parentelenordnung im MA?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;ursprünglich&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;engerer &lt;/strong&gt;Erbenkreis: &lt;strong&gt;Hausgemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;weiterer&lt;/strong&gt; Erbenkreis: &lt;strong&gt;Blutsverwandte &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Parentelenordnung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anerkennung &lt;/strong&gt;des &lt;strong&gt;Repräsentationsrecht &lt;/strong&gt;für &lt;strong&gt;Kinder &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;dehnte engeren&lt;/strong&gt; Erbenkreis &lt;strong&gt;aus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;führte zu &lt;strong&gt;Parentelenordnung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;jüngere Generation ist älterer erbrechtlich vorangestellt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;strong&gt;Das Gut rinnt wie das Blut&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Erbgut und Kaufgut?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbgut&lt;/em&gt;: hat man &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;selbst vererbt &lt;/strong&gt;bekommen, wird &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;familiär weitergegeben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Kaufgut&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;selbst erwirtschaftetes &lt;/strong&gt;Vermögen zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;freien&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verfügung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Spezialsukzession?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Der &lt;strong&gt;Nachlass &lt;/strong&gt;zerfällt in &lt;strong&gt;verschiedene Vermögensmassen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gehen in &lt;strong&gt;spezifischer Erbfolge &lt;/strong&gt;auf die &lt;strong&gt;Erben &lt;/strong&gt;über&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abweichung &lt;/strong&gt;von der &lt;strong&gt;gesetzlichen Erbfolge&lt;/strong&gt; ist &lt;strong&gt;möglich &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren Näherrechte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;dingliche Erwerbsrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Bei &lt;strong&gt;Eigentumswechsel &lt;/strong&gt;kann ein &lt;strong&gt;näher Berechtigter &lt;/strong&gt;(z.B.: Sippengenosse)&lt;strong&gt; &lt;/strong&gt;als der neue Eigentümer &lt;strong&gt;innerhalb &lt;/strong&gt;einer gewissen &lt;strong&gt;Frist&lt;/strong&gt; das &lt;strong&gt;Gut &lt;/strong&gt;an &lt;strong&gt;sich nehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schützt &lt;strong&gt;Sippeneigentum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ende MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abschwächung &lt;/strong&gt;zu &lt;strong&gt;Vorkaufs&lt;/strong&gt;- und &lt;strong&gt;Einstandsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Besserberechtigte musste &lt;strong&gt;Kaufpreis &lt;/strong&gt;und &lt;strong&gt;Kosten erstatten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur &lt;strong&gt;vertraglich begründete &lt;/strong&gt;Näherrechte&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren Leiherechte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bodenleihe &lt;/strong&gt;verschaffte &lt;strong&gt;gegen&lt;/strong&gt; &lt;strong&gt;Entgelt Nutzungsrechte &lt;/strong&gt;an fremden Boden&lt;/li&gt;&lt;li&gt;Unterscheidung:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;freihe &lt;/em&gt;Leihe: &lt;strong&gt;Leistung&lt;/strong&gt; &lt;strong&gt;aus &lt;/strong&gt;dem &lt;strong&gt;Leihgut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;unfreie &lt;/em&gt;Leihe: &lt;strong&gt;persönliche &lt;/strong&gt;und &lt;strong&gt;wirtschaftliche Leistung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Arten (nach &lt;strong&gt;Personengruppen&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;bäuerliche&lt;/em&gt; Leihe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;städtische &lt;/em&gt;Leihe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ritterliche &lt;/em&gt;Leihe&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Ewigsatzung, was die Totsatzung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Ewigsatzung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Früchte &lt;/strong&gt;werden &lt;strong&gt;nicht&lt;/strong&gt; auf die &lt;strong&gt;Schuld angerechnet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pfand &lt;strong&gt;löst &lt;/strong&gt;sich &lt;strong&gt;NICHT selbst&lt;/strong&gt; auf.&lt;/li&gt;&lt;li&gt;&lt;em&gt;Totsatzung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Früchte &lt;/strong&gt;wurden auf die &lt;strong&gt;Schuld angerechnet &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pfand löst &lt;/strong&gt;sich somit nach gewisser Zeit &lt;strong&gt;selbst auf&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Fahrnispfandrecht? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Faustpfand &lt;/strong&gt;-&amp;gt; Übertragung &lt;strong&gt;leibliche Gewere &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;wurde &lt;strong&gt;Eigentümer&lt;/strong&gt;, wenn &lt;strong&gt;nicht in Frist eingelöst&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;13 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;konnte auf &lt;strong&gt;gesamtes Vermögen &lt;/strong&gt;zugreifen, wenn Pfand &lt;strong&gt;unterging &lt;/strong&gt;oder an &lt;strong&gt;Wert verlor &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Einführung des &lt;strong&gt;Verkaufspfandes&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Entwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;konnte durch &lt;strong&gt;Willensübereinstimmung &lt;/strong&gt;entstehen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;rechtlich schwach &lt;/strong&gt;(&lt;strong&gt;keine Verfolgungsklage &lt;/strong&gt;des Gläubigers &lt;strong&gt;ggü Dritten&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;18 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rückkehr zum &lt;strong&gt;Faustpfand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Faustpfand&lt;/strong&gt; und &lt;strong&gt;Hypothek&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Hypothek?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Pfandrecht &lt;/strong&gt;der &lt;strong&gt;jüngeren Satzung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;besitzloses &lt;/strong&gt;Pfand im Liegenschaftsrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;in der &lt;strong&gt;Rezeption &lt;/strong&gt;(&lt;strong&gt;Neuzeit&lt;/strong&gt;) entwickelt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;hat &lt;strong&gt;Hypothek &lt;/strong&gt;(&lt;em&gt;beschränkt dingliches Recht&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;Nichtbegleichung &lt;/strong&gt;der Schuld kann er es &lt;strong&gt;geltend machen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Begründet durch&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;formfreien Vertrag &lt;/strong&gt;(&lt;strong&gt;Vertrags&lt;/strong&gt;pfandrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kraft &lt;strong&gt;Gesetz &lt;/strong&gt;(&lt;strong&gt;gesetzliches &lt;/strong&gt;Pfandrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;richterliche &lt;/strong&gt;Verfügung (&lt;strong&gt;Pfändungs&lt;/strong&gt;pfandrecht)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Dienstbarkeiten?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Übernommen aus &lt;strong&gt;RR&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Grunddienstbarkeiten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;beschränkt dingliche Rechte &lt;/strong&gt;an &lt;strong&gt;Grundstücken&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eigentümer&lt;/strong&gt; muss &lt;strong&gt;Ausübung &lt;/strong&gt;des Rechts &lt;strong&gt;dulden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ins &lt;strong&gt;ABGB 1811&lt;/strong&gt; übernommen&lt;/li&gt;&lt;li&gt;&lt;em&gt;persönliche&lt;/em&gt; &lt;em&gt;Dienstbarkeiten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Grunddienstbarkeiten &lt;/strong&gt;die einer &lt;strong&gt;bestimmten Person &lt;/strong&gt;zugeordnet werden -&amp;gt; &lt;em&gt;Leibzucht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;durch&lt;strong&gt; Rezeption&lt;/strong&gt;: &lt;strong&gt;Personalservituten &lt;/strong&gt;(&lt;em&gt;ususfructus, usus, habitatio&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind beschränkt dingliche Rechte?&lt;/p&gt;&lt;p&gt;Nennen sie ein Beispiel&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Belastungen &lt;/strong&gt;des Eigentums &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beschränkt&lt;/strong&gt; die Rechte des &lt;strong&gt;Eigentümers&lt;/strong&gt;, &lt;/li&gt;&lt;li class="ql-indent-1"&gt;gibt &lt;strong&gt;Teilberechtigungen&lt;/strong&gt; an den &lt;strong&gt;Berechtigten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Arten&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pfand&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dienstbarkeiten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reallasten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Aufbau des ABGB?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Institutionensystem &lt;/em&gt;(auch &lt;strong&gt;gaianisches &lt;/strong&gt;System)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zweiteilung in &lt;strong&gt;Personen&lt;/strong&gt;- und &lt;strong&gt;Vermögensrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Pandektensystem&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aufteilung in &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Allgemeinen &lt;/strong&gt;Teil&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schuld&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sachen&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Familien&lt;/strong&gt;recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erb&lt;/strong&gt;recht&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Landtafeln?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Seit 13/14 JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Form / Teil des &lt;strong&gt;Grundbuchs&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;für &lt;strong&gt;Adelige&lt;/strong&gt; &lt;strong&gt;Liegenschaften &lt;/strong&gt;- &lt;em&gt;Eintragungspflicht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;dingliche Rechte &lt;/strong&gt;gelten nur mit &lt;strong&gt;Eintragung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Typenzwang?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sachenrecht definiert &lt;/strong&gt;alle möglichen &lt;strong&gt;dingliche Berechtigungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es können &lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;weiteren &lt;/strong&gt;"&lt;strong&gt;erfunden&lt;/strong&gt;" werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;= &lt;em&gt;numerus clausus&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Stellung unehelicher Kinder im älteren Recht?&lt;/p&gt;&lt;p&gt;Wann änderte sich dies?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gleichstellung &lt;/strong&gt;mit &lt;strong&gt;ehelichen&lt;/strong&gt;, wenn in &lt;strong&gt;Hausverband aufgenommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;sonst &lt;/strong&gt;Zugehörigkeit zu &lt;strong&gt;Muttersippe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schlechterstellung &lt;/strong&gt;ab &lt;strong&gt;christlicher &lt;/strong&gt;Zeit&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Stellung Joseph II zu unehelichen Kindern&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundsätzliche Gleichstellung &lt;/strong&gt;eheliche und uneheliche&lt;/li&gt;&lt;li&gt;Ausnahme: &lt;strong&gt;Ehebruchskinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Stellung der ehelichen und unehelichen Kinder im MA und im ABGB 1811?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Eheliche &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eheliche Kinder unter &lt;strong&gt;Munt &lt;/strong&gt;des Vaters&lt;/li&gt;&lt;li class="ql-indent-2"&gt;u.a. &lt;strong&gt;Verwaltung &lt;/strong&gt;von &lt;strong&gt;Vermögen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste &lt;/strong&gt;Form der &lt;strong&gt;Unterhaltspflicht&lt;/strong&gt;: &lt;strong&gt;Zweckbindung &lt;/strong&gt;es &lt;strong&gt;Kindesvermögens&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aussteuer &lt;/strong&gt;(Ausstattung) bei Ausscheiden des Kindes &lt;strong&gt;aus Muntgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Uneheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gleichberechtigt &lt;/strong&gt;wenn in Hausverband &lt;strong&gt;aufgenommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Christlicher &lt;/strong&gt;Einfluss:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Verlust Erbrecht &lt;/strong&gt;gegen Vater&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Ausschluss &lt;/strong&gt;aus &lt;strong&gt;Berufen &lt;/strong&gt;und &lt;strong&gt;Zünften&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;keine kirchlichen &lt;/strong&gt;Ämter&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Eheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unterhalt &lt;/strong&gt;Vater, &lt;strong&gt;Pflege &lt;/strong&gt;Mutter&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater &lt;strong&gt;gesetzlicher Vertreter&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater &lt;strong&gt;verwaltet Kindesvermögen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kind erhält &lt;strong&gt;Familien&lt;/strong&gt;+ &lt;strong&gt;Standesrecht &lt;/strong&gt;des &lt;strong&gt;Vaters&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Uneheliche Kinder&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bis 1. TN &lt;strong&gt;kein Verwandtschaftsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dann gegenüber Mutter &lt;/strong&gt;gleiche Rechte &lt;strong&gt;wie eheliche&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vater: &lt;strong&gt;Unterhaltsanspruch&lt;/strong&gt;, &lt;strong&gt;Besuchsrecht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ehe- und Familienmodell ABGB 1811 und welches war davor?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;patriarchales &lt;/strong&gt;Familienmodell - "&lt;strong&gt;Überlegenheit &lt;/strong&gt;des &lt;strong&gt;Mannes&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;davor&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vernunftrechtliche &lt;/strong&gt;Familie: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ansätze partnerschaftlichen &lt;/strong&gt;Modells&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Recht auf &lt;strong&gt;Persönlichkeitsentfaltung Frau &lt;/strong&gt;+ &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Selbstbestimmungsrecht der Frau bei Ehe - früher und heute?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Frau unter &lt;strong&gt;Muntgewalt &lt;/strong&gt;- wenig Selbstbestimmung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Mittelalter&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Besserstellung &lt;/strong&gt;der Frau durch &lt;strong&gt;christlichen &lt;/strong&gt;Einfluss&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehemann vertrat &lt;/strong&gt;Frau vor &lt;strong&gt;Gericht &lt;/strong&gt;und bei &lt;strong&gt;Rechtsgeschäften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Frau &lt;/strong&gt;konnte &lt;strong&gt;alltägliche Rechtsgeschäfte &lt;/strong&gt;&lt;em&gt;für Mann &lt;/em&gt;durchführen&lt;/li&gt;&lt;li&gt;Aufkommen &lt;strong&gt;gegenseitiger Treuepflicht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeit&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leitungsfunktion &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;ausgebaut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verpflichtung &lt;/strong&gt;der &lt;strong&gt;Sicherung &lt;/strong&gt;des &lt;strong&gt;Unterhalts &lt;/strong&gt;der Frau&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Treue- und Beistandspflicht usus (aber nicht rechtlich verankert)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Naturrechtliche Lehre&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Katalog&lt;strong&gt; gegenseitige Rechte &lt;/strong&gt;und &lt;strong&gt;Pflichten &lt;/strong&gt;der Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Seit &lt;em&gt;Familienrechtsreform 1975&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;eheliche &lt;strong&gt;Gleichberechtigung &lt;/strong&gt;von Mann und Frau&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Seit wann gibt es in Österreich die Zivilehe?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Seit den &lt;strong&gt;Maigesetzen 1868&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Notzivilehe &lt;/strong&gt;-&amp;gt; ohne kanonische Vorschriften&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Seit &lt;em&gt;1945&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;obligatorische&lt;/em&gt; Zivilehe&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Eliminierung &lt;/strong&gt;der &lt;strong&gt;nationalsozialistischen &lt;/strong&gt;Bestimmungen des &lt;strong&gt;dt. Ehegestez 1938&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Übernahme &lt;/strong&gt;ins &lt;strong&gt;ABGB&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Eheschließung bis ABGB 1811&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Mittelalter: &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mehrere&lt;/strong&gt; &lt;strong&gt;Formen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Kirche &lt;/em&gt;hatte &lt;em&gt;Ehehoheit &lt;/em&gt;&lt;/li&gt;&lt;li&gt;Siehe Frage "&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Welche Arten der Ehe gab es im Mittelalter?"&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Neuzeitliche Rechtsentwicklung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kompetenzkonflikt &lt;/strong&gt;Kirche vs Staat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Staatliches &lt;/strong&gt;Eherecht &lt;strong&gt;als&lt;/strong&gt; &lt;strong&gt;zweites&lt;/strong&gt;, ebenso &lt;strong&gt;gültiges&lt;/strong&gt;, Eherecht &lt;strong&gt;neben Kirchlichem&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;18 JH (vernunftrechtlische Naturrecht) &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehe dient &lt;/strong&gt;dem&lt;strong&gt; Staats&lt;/strong&gt;interesse&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;polizeistaatliches Ehemodell&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Joseph II 1783&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trennung Ehesakrament&lt;/strong&gt; &lt;strong&gt;Ehevertrag&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;nicht obligatorische &lt;/strong&gt;Zivilehe&lt;/li&gt;&lt;li&gt;Siehe Karte&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;dreigeteilt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Siehe Karte&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Hat es eine Zeit gegeben, in der das kanonische Recht auch für Katholiken-Ehen gegolten hat?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zwischen Konkordat 1855 und Maigesetze 1868&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die weitere Entwicklung des Eherechts nach ABGB 1811?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Konkordat 1855&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit Kirche &lt;/strong&gt;unterstellt&lt;/li&gt;&lt;li&gt;&lt;em&gt;Maigesetze 1868 &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Notzivilehe &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wiederherstellung &lt;/strong&gt;Eherecht &lt;strong&gt;ABGB &lt;/strong&gt;1811&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehegerichtsbarkeit &lt;/strong&gt;wieder &lt;strong&gt;staatlich &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Festsetzung &lt;strong&gt;Monogamie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;keine &lt;/strong&gt;Möglichkeit der &lt;strong&gt;Scheidung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dispensehe 1919 &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Frage dazu&lt;/li&gt;&lt;li&gt;&lt;em&gt;Konkordat 1934&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eherecht&lt;/strong&gt; für &lt;strong&gt;Katholiken&lt;/strong&gt; wieder an &lt;strong&gt;Kirche&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dt. Ehegesetz 1938&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;einheitliches Eherecht &lt;/strong&gt;im ganzen Reich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;siehe Frage dazu&lt;/li&gt;&lt;li&gt;&lt;em&gt;Modernes Recht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übernommen aus &lt;strong&gt;Ehegesetz 1938 &lt;/strong&gt;"&lt;strong&gt;entnazifizert&lt;/strong&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Obligatorische Zivilehe &lt;/strong&gt;für alle Konfessionen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Eherecht ABGB 1811 - Unterschied zu heute&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;ABGB &lt;/em&gt;hatte (anders als heute) &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dreifach gegliedertes &lt;/strong&gt;Eherecht: Katholiken, Protestanten, Juden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ehehindernis&lt;/strong&gt;: Wiederverheiratung nicht möglich, solange &lt;strong&gt;katholischer&lt;/strong&gt; &lt;strong&gt;Ehepartner noch lebt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Keine &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;Zivilehe&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Güterstand im Älteren Recht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Vermögenstrennung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;hat Recht auf &lt;strong&gt;Verwaltung &lt;/strong&gt;+ &lt;strong&gt;Nutzung &lt;/strong&gt;von &lt;strong&gt;Frauenvermögen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Leibgedinge&lt;/em&gt;: &lt;strong&gt;unentgeltliches Nutzungsrecht &lt;/strong&gt;auf Lebenszeit an einem Objekt des Ehepartners.&lt;/li&gt;&lt;li&gt;&lt;em&gt;Heiratsgabensystem&lt;/em&gt;: &lt;strong&gt;Heimsteuer &lt;/strong&gt;+ &lt;strong&gt;Widerlage&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Heiratsgabensystem im Mittelalter?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;= Zur &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Heimsteuer&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Heiratsgabe der &lt;strong&gt;Frau &lt;/strong&gt;- Zuschuss zu finanziellen Lasten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gegengewicht &lt;/strong&gt;zu &lt;strong&gt;Mann &lt;/strong&gt;als einzige &lt;strong&gt;Einnahmequelle&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Widerlage &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;fällig bei (&lt;strong&gt;Vor&lt;/strong&gt;)&lt;strong&gt;Tod&lt;/strong&gt; des &lt;strong&gt;Mannes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;wenn Heimsteuer &lt;/strong&gt;geleistet wurde&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Im &lt;strong&gt;Todesfalle &lt;/strong&gt;des &lt;strong&gt;Mannes &lt;/strong&gt;-&amp;gt; beides zusammen zur &lt;strong&gt;Witwenversorgung&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Güterstand im Mittelalter?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;beschränkte Gütergemeinschaft &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur für &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;bestimmte&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Objekte&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(z.B.: &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Liegenschaften&lt;/span&gt;)&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;Gesamthand&lt;/strong&gt;" -&amp;gt; Rechtsgeschäfte erfordern Zu&lt;strong&gt;stimmung beider&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Errungenschaftsgemeinschaften&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;der &lt;strong&gt;beschränkten &lt;/strong&gt;Gütergemeinschaft&lt;/li&gt;&lt;li&gt;Auch &lt;strong&gt;zukünftiges Vermögen &lt;/strong&gt;miteinbezogen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Fahrnisgemeinschaft&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Errungenschaften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eingebrachte&lt;/strong&gt; und &lt;strong&gt;unentgeltlich erworbene &lt;/strong&gt;&lt;em&gt;Fahrnis&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Rentleinsheirat&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;allgemeine &lt;/strong&gt;&lt;strong&gt;Gütergemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;eingebrachtes&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erworbenes&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Vermögen beider&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die große Familienrechtsreform?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1970er&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Verwirklichung des &lt;strong&gt;Gleichberechtigungsgrundsatzes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;elterliche Gleichberechtigung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;verstärkter&lt;strong&gt; Schutz&lt;/strong&gt; der &lt;strong&gt;Kinder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anerkennung&lt;/strong&gt; der &lt;strong&gt;Privatautonomie &lt;/strong&gt;im &lt;strong&gt;familiären &lt;/strong&gt;Bereich&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Polizeistaatliche Familienmodell?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Christliche &lt;strong&gt;Familie &lt;/strong&gt;hatte &lt;strong&gt;im MA &lt;/strong&gt;im &lt;strong&gt;Obrigkeitsstaat &lt;/strong&gt;eine &lt;strong&gt;staatsdienende&lt;/strong&gt; Bedeutung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wurde durch &lt;strong&gt;aristotelische Hauslehre &lt;/strong&gt;erklärt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hausherr&lt;/strong&gt; sorgt für &lt;em&gt;obrigkeitstreues Verhalten &lt;/em&gt;der &lt;strong&gt;Hausgenossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Staat überwacht &lt;/strong&gt;die Pflichterfüllung des &lt;strong&gt;Hausherrn&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Familie &lt;/strong&gt;war also &lt;strong&gt;Element &lt;/strong&gt;des &lt;strong&gt;Polizeistaats&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Beziehung der Ehegatten untereinander im ABGB 1811?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mann &lt;/strong&gt;als "&lt;strong&gt;Haupt&lt;/strong&gt;" der Familie&lt;/li&gt;&lt;li class="ql-indent-1"&gt;hat &lt;strong&gt;Unterhaltspflicht &lt;/strong&gt;und &lt;strong&gt;Leitungsrecht&lt;/strong&gt; &lt;strong&gt;gegenüber Frau&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ansicht der "traditionelle Rollenverteilung"&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Aristotelische Hauslehre?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Haus &lt;/strong&gt;(Familie) ist &lt;strong&gt;Teil &lt;/strong&gt;einer &lt;strong&gt;übergeordneten Gemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestimmt den &lt;em&gt;Sozialstatus &lt;/em&gt;der Menschen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater vertritt &lt;/strong&gt;Familie nach außen &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vater &lt;/strong&gt;hat &lt;strong&gt;Gewalt &lt;/strong&gt;über &lt;strong&gt;Hausgemeinschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Majorenitäts-Jahresbestimmung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Volljährigkeit &lt;/strong&gt;in allen &lt;strong&gt;dt. Erbkönigreichen&lt;/strong&gt; und &lt;strong&gt;Ländern &lt;/strong&gt;auf &lt;strong&gt;24 Jahre&lt;/strong&gt; festgesetzt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Fähigkeiten kommen abgeschichteten Söhnen zu?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vermögensrechtlich Selbständig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Familiengründung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;etc&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was bedeutet Abschichtung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Erreichen der &lt;strong&gt;Mündigkeit &lt;/strong&gt;von &lt;strong&gt;Haussöhnen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Nach &lt;strong&gt;Ausscheiden &lt;/strong&gt;aus dem &lt;strong&gt;väterlichen Haushalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Teilbereiche der Handlungsfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Deliktsfähigkeit&lt;/em&gt;: Fähigkeit, sich durch &lt;strong&gt;rechtswidriges Verhalten&lt;/strong&gt; zu &lt;strong&gt;verpflichten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Geschäftsfähigkeit&lt;/em&gt;: Fähigkeit sich durch &lt;strong&gt;Rechtsgeschäfte&lt;/strong&gt; zu &lt;strong&gt;verpflichten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die allgemeine (unbeschränkte) Rechtsfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Recht der&lt;/strong&gt; &lt;strong&gt;Persönlichkeit&lt;/strong&gt; im &lt;em&gt;Naturrecht&lt;/em&gt; und &lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Siehe auch Frage "Statuslehre"&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Statuslehre?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;röm Recht übernommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;libertatis&lt;/strong&gt;: &lt;em&gt;Freie&lt;/em&gt; vs &lt;em&gt;Sklaven&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;civitatis&lt;/strong&gt;: &lt;em&gt;Bürger &lt;/em&gt;vs &lt;em&gt;Fremde&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Status &lt;strong&gt;familiae&lt;/strong&gt;: &lt;em&gt;Zugehörigkeit &lt;/em&gt;zu &lt;em&gt;Familie&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Entwicklung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Codex &lt;strong&gt;Theresianus &lt;/strong&gt;folgte &lt;strong&gt;Statuslehre&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ablösung &lt;/strong&gt;durch &lt;strong&gt;naturrechtliche &lt;/strong&gt;Vorstellungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Recht der Persönlichkeit&lt;/em&gt; (angeborenes Recht, &lt;strong&gt;frei zu handeln &lt;/strong&gt;und seine &lt;strong&gt;Würde &lt;/strong&gt;zu &lt;strong&gt;behaupten&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;= Allgemeine (unbeschränkte) Rechtsfähigkeit&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Übernahme&lt;/strong&gt; ins &lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Abhängigkeit der Bauern?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Geteilt in &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;freie &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unfreie &lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Leibeigenschaft &lt;/strong&gt;in&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; Ö &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;nicht institutionalisiert&lt;/strong&gt;, &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;aber &lt;/span&gt;diverse &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Einschränkungen &lt;/strong&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Rechtsfähigkeit&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Abhängigkeiten&lt;/span&gt; der &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unfreien &lt;/em&gt;&lt;em&gt;Bauern&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Sachenrechtlich &lt;/em&gt;(&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Abgaben &lt;/strong&gt;für Grund und Boden)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Politisch &lt;/em&gt;(&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundherr &lt;/span&gt;hatte &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichts&lt;/strong&gt;- und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Verwaltungsaufgaben&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Persönlich &lt;/em&gt;(&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Heiratsbewilligung&lt;/strong&gt;, befohlene &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Tätigkeit&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wohnsitzentscheidungen&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ab &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;16. JH&lt;/em&gt; (&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Bauernkriege&lt;/strong&gt;) -&amp;gt; Trend zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufhebung &lt;/strong&gt;der &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;persönlichen Abhängigkeit&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erst &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;18/19 JH beseitigt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Aufgaben hatte das Ehegüterrecht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Versorgung &lt;/strong&gt;des &lt;strong&gt;überlebenden &lt;/strong&gt;Ehegatten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufteilung &lt;/strong&gt;der &lt;strong&gt;finanziellen &lt;/strong&gt;Lasten (Finanzieller &lt;strong&gt;Beitrag der&lt;/strong&gt; &lt;strong&gt;Frau &lt;/strong&gt;wurde gefordert) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist mit Geschlechtervormundschaft gemeint?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Frau &lt;/strong&gt;ist &lt;strong&gt;immer unter &lt;/strong&gt;der &lt;strong&gt;Muntgewalt&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Väterliche Munt &lt;/em&gt;bis zur Verheiratung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dann &lt;em&gt;eheherrliche Munt&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Bei Ableben des Vaters vor Hochzeit:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;verwandsschaftliche Munt &lt;/em&gt;(Bruder oder anderer männl. Verwandter)&lt;/li&gt;&lt;li&gt;als Witwe entweder Munt der Verwandschaft oder des toten Ehemanns&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Salvatorische Klausel?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nach der Salvatorischen Klausel sollte das &lt;strong&gt;ius commune &lt;/strong&gt;nur &lt;strong&gt;subsidiär &lt;/strong&gt;gelten&lt;/p&gt;&lt;ul&gt;&lt;li&gt; &lt;strong&gt;Geltungsnachweises &lt;/strong&gt;für das &lt;strong&gt;Gewohnheitsrecht &lt;/strong&gt;war jedoch &lt;strong&gt;schwierig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Daher &lt;strong&gt;Trendumkehr&lt;/strong&gt;: Gegner musste &lt;em&gt;Beweis der Nichtrezeption&lt;/em&gt; erbringen, um das &lt;strong&gt;Gewohnheitsrecht durchzusetzen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Aussteuer?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Mitgift&lt;/strong&gt; der &lt;strong&gt;Familie&lt;/strong&gt; der &lt;strong&gt;Frau&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;auch &lt;strong&gt;Heimsteuer&lt;/strong&gt; genannt&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was war der Güterstand in der Neuzeit/Rezeption?&lt;/p&gt;</t>
   </si>
   <si>
@@ -421,18 +433,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zugriff&lt;/strong&gt; aufs &lt;strong&gt;Kindesvermögen &lt;/strong&gt;rechtl. &lt;strong&gt;eingeschränkt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;"Kindesgut ist eisern Gut"&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur &lt;strong&gt;verwalten&lt;/strong&gt; und &lt;strong&gt;nutzen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Substanz &lt;/strong&gt;durfte &lt;strong&gt;nicht angegriffen &lt;/strong&gt;werden&lt;/li&gt;&lt;li&gt;&lt;em&gt;Erbenlaub/Erbenlob&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbgut &lt;/strong&gt;und &lt;strong&gt;Liegenschaften&lt;/strong&gt; nur mit &lt;strong&gt;Zustimmung &lt;/strong&gt;der Kinder &lt;strong&gt;veräußert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was war der Grund für Religionsspezifische Regeln im Eherecht im ABGB 1811?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Staat&lt;/strong&gt; hatte &lt;strong&gt;Interesse &lt;/strong&gt;daran &lt;strong&gt;Ehe gesetzlich &lt;/strong&gt;zu &lt;strong&gt;regeln &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Formell&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Inhaltlich &lt;/strong&gt;aber &lt;strong&gt;Regeln&lt;/strong&gt; &lt;strong&gt;der Konfessionen &lt;/strong&gt;übernommen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;em&gt;Materiell&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verhindert&lt;/strong&gt;, dass &lt;strong&gt;Gläubige &lt;/strong&gt;durch staatl. &lt;strong&gt;Eherecht gezwungen&lt;/strong&gt; sind &lt;strong&gt;gegen Regeln &lt;/strong&gt;ihrer &lt;strong&gt;Konfession&lt;/strong&gt; zu &lt;strong&gt;verstoßen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer ist normalerweise Erbe im MA?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Älteres Recht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gut an &lt;strong&gt;Sippe gebunden &lt;/strong&gt;- &lt;strong&gt;Gesamthand&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Anwachsung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;später im MA&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Parentelerbfolge&lt;/strong&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Das Gut rinnt wie das Blut&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Deszendenten &lt;/strong&gt;vor &lt;strong&gt;Aszendeten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frauen subsidiär&lt;/strong&gt; -&amp;gt; nur wenn keine männlichen Erben&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Welche Liegenschaftsgewere werden unterschieden? &lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -508,7 +508,7 @@
     <t>&lt;p&gt;Entwicklung des Ehegatten&lt;strong&gt;erbrechts&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;em&gt;heimisches Gewohnheitsrecht &lt;/em&gt;(&lt;strong&gt;älteres &lt;/strong&gt;Recht)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;kein Erbrecht&lt;/strong&gt; des Ehegatten, weil &lt;strong&gt;Eheschließung keine&lt;/strong&gt; &lt;strong&gt;Verwandtschaft &lt;/strong&gt;begründete&lt;/li&gt;&lt;li&gt;Wenn &lt;strong&gt;keine Verwandten&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Fiskus &lt;/strong&gt;erhält Erbgut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kein Bedürfnis &lt;/strong&gt;nach Ausgestaltung des &lt;strong&gt;Ehegattenerbrechts&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;MA&lt;/strong&gt; und &lt;strong&gt;frühe&lt;/strong&gt; &lt;strong&gt;Neuzeit&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Ehegüterrecht &lt;/em&gt;&lt;/strong&gt;für finanzielle Absicherung des Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ansätze &lt;/strong&gt;zur Ausgestaltung des &lt;strong&gt;Ehegattenerbr&lt;/strong&gt;.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ehegüterrechtl&lt;/strong&gt;. Ansprüche wurden mit &lt;strong&gt;Vorstellung von&lt;/strong&gt; &lt;strong&gt;Erbrecht&lt;/strong&gt; &lt;strong&gt;verbunden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;besonders im &lt;strong&gt;Bauernstand&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Üblich: &lt;strong&gt;Ehegatte &lt;/strong&gt;erhält &lt;strong&gt;Hälfte&lt;/strong&gt; der &lt;strong&gt;Errungenschaft &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wichtige &lt;strong&gt;Motivation&lt;/strong&gt;: &lt;strong&gt;unversorgte Witwen &lt;/strong&gt;mangels ehegüterrechtlicher Vereinbarungen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Rezeption &lt;/strong&gt;des gemeinsamen &lt;strong&gt;Ehegattenerbrechts &lt;/strong&gt;im &lt;strong&gt;18 JH&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ehegatte erhielt &lt;strong&gt;Erbrecht nach&lt;/strong&gt; &lt;strong&gt;allen Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;falls ehegüterr&lt;/strong&gt;. &lt;strong&gt;Vereinbarung&lt;/strong&gt;: Ehegatte hat &lt;strong&gt;Wahl &lt;/strong&gt;ob &lt;strong&gt;Ehegüter oder Erbe &lt;/strong&gt;antreten.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sonderstellung unbemittelter &lt;/strong&gt;Gatte: wenn &lt;strong&gt;gänzlich&lt;/strong&gt; &lt;strong&gt;unversorgt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;1/4 des Nachlasses&lt;/strong&gt; (oder &lt;em&gt;Kindeskopfteil &lt;/em&gt;bei &lt;em&gt;vier+ Kindern&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Josephinisches &lt;/strong&gt;&lt;em&gt;Erbfolgepatent &lt;/em&gt;&lt;strong&gt;1786&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehegatte &lt;/strong&gt;wird Erbfolger, &lt;strong&gt;wenn kein&lt;/strong&gt; &lt;strong&gt;Verwandter &lt;/strong&gt;in&lt;strong&gt; 6 Parentelen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Zusätzlich &lt;strong&gt;Fruchtgenussrecht &lt;/strong&gt;an &lt;strong&gt;1/4 des Vermögens &lt;/strong&gt;(&lt;em&gt;endet mit erneuter Ehe&lt;/em&gt;).&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;ABGB 1811&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;basierend&lt;/strong&gt; auf &lt;strong&gt;Josephinischem&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fruchtgenuss &lt;/strong&gt;zu unbeschränktem&lt;strong&gt; Eigentum&lt;/strong&gt; &lt;strong&gt;erweitert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;Kind 1/4&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;anderen Erben&lt;/strong&gt; &lt;strong&gt;1/2 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne Verwandte &lt;/strong&gt;in &lt;strong&gt;1+2. Linie&lt;/strong&gt; und &lt;strong&gt;ohne Großeltern&lt;/strong&gt;: &lt;strong&gt;ganze &lt;/strong&gt;Verlassenschaft&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;kein Pflichtteil&lt;/strong&gt;, aber &lt;strong&gt;Vorausvermächtnis &lt;/strong&gt;(&lt;em&gt;bewegliche Sachen &lt;/em&gt;des Haushalts)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;heutiges Ehegattenerbrecht&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;entstand aus &lt;strong&gt;Familienrechtsreform&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anhebung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Erbteils&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilanspruch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erben müssen Ehegatten &lt;strong&gt;verbleib in Wohnung &lt;/strong&gt;ermöglichen (&lt;strong&gt;Schuldrechtl&lt;/strong&gt;. &lt;strong&gt;Anspruch &lt;/strong&gt;des Ehegatten gegen Erben)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehegatte erhält &lt;strong&gt;haushaltszugehörige Sachen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;gewohnte Umgebung&lt;/strong&gt; behalten&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;&lt;em&gt;heimisches Gewohnheitsrecht &lt;/em&gt;(&lt;strong&gt;älteres &lt;/strong&gt;Recht)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;kein Erbrecht&lt;/strong&gt; des Ehegatten, weil &lt;strong&gt;Eheschließung keine&lt;/strong&gt; &lt;strong&gt;Verwandtschaft &lt;/strong&gt;begründete&lt;/li&gt;&lt;li&gt;Wenn &lt;strong&gt;keine Verwandten&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Fiskus &lt;/strong&gt;erhält Erbgut&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kein Bedürfnis &lt;/strong&gt;nach Ausgestaltung des &lt;strong&gt;Ehegattenerbrechts&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;da &lt;strong&gt;MA&lt;/strong&gt; und &lt;strong&gt;frühe&lt;/strong&gt; &lt;strong&gt;Neuzeit&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Ehegüterrecht &lt;/em&gt;&lt;/strong&gt;für finanzielle Absicherung des Ehegatten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Spätmittelalter&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ansätze &lt;/strong&gt;zur Ausgestaltung des &lt;strong&gt;Ehegattenerbr&lt;/strong&gt;.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ehegüterrechtl&lt;/strong&gt;. Ansprüche wurden mit &lt;strong&gt;Vorstellung von&lt;/strong&gt; &lt;strong&gt;Erbrecht&lt;/strong&gt; &lt;strong&gt;verbunden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;besonders im &lt;strong&gt;Bauernstand&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Üblich: &lt;strong&gt;Ehegatte &lt;/strong&gt;erhält &lt;strong&gt;Hälfte&lt;/strong&gt; der &lt;strong&gt;Errungenschaft &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wichtige &lt;strong&gt;Motivation&lt;/strong&gt;: &lt;strong&gt;unversorgte Witwen &lt;/strong&gt;mangels ehegüterrechtlicher Vereinbarungen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Rezeption des Ehegattenerbrechts im 18. JH&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ehegatte erhielt &lt;strong&gt;Erbrecht nach&lt;/strong&gt; &lt;strong&gt;allen Verwandten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;falls ehegüterr&lt;/strong&gt;. &lt;strong&gt;Vereinbarung&lt;/strong&gt;: Ehegatte hat &lt;strong&gt;Wahl &lt;/strong&gt;ob &lt;strong&gt;Ehegüter oder Erbe &lt;/strong&gt;antreten.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sonderstellung unbemittelter &lt;/strong&gt;Gatte: wenn &lt;strong&gt;gänzlich&lt;/strong&gt; &lt;strong&gt;unversorgt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;1/4 des Nachlasses&lt;/strong&gt; (oder &lt;em&gt;Kindeskopfteil &lt;/em&gt;bei &lt;em&gt;vier+ Kindern&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Josephinisches Erbfolgepatent 1786&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ehegatte &lt;/strong&gt;wird Erbfolger, &lt;strong&gt;wenn kein&lt;/strong&gt; &lt;strong&gt;Verwandter &lt;/strong&gt;in&lt;strong&gt; 6 Parentelen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Zusätzlich &lt;strong&gt;Fruchtgenussrecht &lt;/strong&gt;an &lt;strong&gt;1/4 des Vermögens &lt;/strong&gt;(&lt;em&gt;endet mit erneuter Ehe&lt;/em&gt;).&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;basierend&lt;/strong&gt; auf &lt;strong&gt;Josephinischem&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fruchtgenuss &lt;/strong&gt;zu unbeschränktem&lt;strong&gt; Eigentum&lt;/strong&gt; &lt;strong&gt;erweitert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;Kind 1/4&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neben &lt;strong&gt;anderen Erben&lt;/strong&gt; &lt;strong&gt;1/2 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne Verwandte &lt;/strong&gt;in &lt;strong&gt;1+2. Linie&lt;/strong&gt; und &lt;strong&gt;ohne Großeltern&lt;/strong&gt;: &lt;strong&gt;ganze &lt;/strong&gt;Verlassenschaft&lt;/li&gt;&lt;li&gt;noch &lt;strong&gt;kein Pflichtteil&lt;/strong&gt;, aber &lt;strong&gt;Vorausvermächtnis &lt;/strong&gt;(&lt;em&gt;bewegliche Sachen &lt;/em&gt;des Haushalts)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;heutiges Ehegattenerbrecht&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;entstand aus &lt;strong&gt;Familienrechtsreform&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anhebung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Erbteils&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilanspruch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erweiterung &lt;/strong&gt;des &lt;strong&gt;gesetzl&lt;/strong&gt;. &lt;strong&gt;Vorausvermächtnis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erben müssen Ehegatten &lt;strong&gt;verbleib in Wohnung &lt;/strong&gt;ermöglichen (&lt;strong&gt;Schuldrechtl&lt;/strong&gt;. &lt;strong&gt;Anspruch &lt;/strong&gt;des Ehegatten gegen Erben)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ehegatte erhält &lt;strong&gt;haushaltszugehörige Sachen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;gewohnte Umgebung&lt;/strong&gt; behalten&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was war der &lt;strong&gt;Freiteil&lt;/strong&gt; (&lt;strong&gt;Sohnesquote&lt;/strong&gt;) bei der Testierfähigkeit?&lt;/p&gt;</t>
@@ -622,7 +622,7 @@
     <t>&lt;p&gt;Was sind die Prinzipien des Grundbuchrechts?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;&lt;em&gt;Intabulationsprinzip&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;ab&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;18. JH&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dingliche Rechte nur durch&lt;/strong&gt; &lt;strong&gt;Eintragung &lt;/strong&gt;im Grundbuch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bücherl. Vormann&lt;/strong&gt; -&amp;gt; Recht des Vormannes muss eingetragen werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eintragung benötigt &lt;strong&gt;gültigen Titel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Vertrauensgrundsatz&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gutgläubiger Erwerber &lt;/strong&gt;darf auf Grundbuch &lt;strong&gt;vertrauen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nicht&lt;/strong&gt; &lt;strong&gt;eingetragene RG &lt;/strong&gt;haben &lt;strong&gt;keine Wirkung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;: Nur für nachträgliche außerbücherliche Rechtsänderungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Später&lt;/em&gt;: auch für anfangs fehlerhafte Eintragungen&lt;/li&gt;&lt;li&gt;&lt;em&gt;Prioritätsprinzip&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;zeitlich &lt;/strong&gt;frühere Antrag geht &lt;strong&gt;vor dem späteren -&amp;gt; &lt;/strong&gt;maßgebend&lt;strong&gt;: &lt;/strong&gt;Zeitpunkt des &lt;strong&gt;Gesuchseingangs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Im &lt;em&gt;GrundbuchG 1871&lt;/em&gt;: Zeitpunkt der &lt;strong&gt;Eintragung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Spezialitätsprinzip&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bürgerliche Rechte &lt;/strong&gt;nur an &lt;strong&gt;bestimmten Grundbuchskörpern&lt;/strong&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;em&gt;Intabulationsprinzip&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ab&lt;span style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;18. JH&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dingliche Rechte nur durch&lt;/strong&gt; &lt;strong&gt;Eintragung &lt;/strong&gt;im Grundbuch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bücherl. Vormann&lt;/strong&gt; -&amp;gt; Recht des Vormannes muss eingetragen werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eintragung benötigt &lt;strong&gt;gültigen Titel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Vertrauensgrundsatz&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gutgläubiger Erwerber &lt;/strong&gt;darf auf Grundbuch &lt;strong&gt;vertrauen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nicht&lt;/strong&gt; &lt;strong&gt;eingetragene RG &lt;/strong&gt;haben &lt;strong&gt;keine Wirkung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;ABGB 1811&lt;/em&gt;: Nur für nachträgliche außerbücherliche Rechtsänderungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Später&lt;/em&gt;: auch für anfangs fehlerhafte Eintragungen&lt;/li&gt;&lt;li&gt;&lt;em&gt;Prioritätsprinzip&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;zeitlich &lt;/strong&gt;frühere Antrag geht &lt;strong&gt;vor dem späteren -&amp;gt; &lt;/strong&gt;maßgebend&lt;strong&gt;: &lt;/strong&gt;Zeitpunkt des &lt;strong&gt;Gesuchseingangs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Im &lt;em&gt;GrundbuchG 1871&lt;/em&gt;: Zeitpunkt der &lt;strong&gt;Eintragung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Spezialitätsprinzip&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bürgerliche Rechte &lt;/strong&gt;können nicht durch einen Akt am ganzen Liegenschaftsbesitz einer Person eingetragen werden, sondern nur an einzelnen, &lt;strong&gt;bestimmten Grundbuchskörpern&lt;/strong&gt;&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was waren die Dispensehe bzw. Severehe?&lt;/p&gt;</t>

</xml_diff>